<commit_message>
Updated installed worlds excel
</commit_message>
<xml_diff>
--- a/CustomWorldsInstalled.xlsx
+++ b/CustomWorldsInstalled.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\Git\Archipelago\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90ADEF59-257B-46F8-B9DB-2F709FF58968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97172E97-4806-4ACC-8037-48AE0CF415A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9735" yWindow="21600" windowWidth="28800" windowHeight="15435" xr2:uid="{3DBB16FA-FE5F-4BB0-89C2-A45EA748065E}"/>
+    <workbookView xWindow="4770" yWindow="1845" windowWidth="28800" windowHeight="15435" xr2:uid="{3DBB16FA-FE5F-4BB0-89C2-A45EA748065E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>World</t>
   </si>
@@ -92,24 +92,12 @@
     <t>Inscryption</t>
   </si>
   <si>
-    <t>v103</t>
-  </si>
-  <si>
-    <t>0.3.3</t>
-  </si>
-  <si>
     <t>0.6.3</t>
   </si>
   <si>
-    <t>1.5.1</t>
-  </si>
-  <si>
     <t>0.7.2</t>
   </si>
   <si>
-    <t>0.4.3</t>
-  </si>
-  <si>
     <t>0.1.0</t>
   </si>
   <si>
@@ -120,13 +108,94 @@
   </si>
   <si>
     <t>Chrono Trigger Jets of Time</t>
+  </si>
+  <si>
+    <t>Kingdom Hearts Re:Chain of Memories</t>
+  </si>
+  <si>
+    <t>v1.2.1</t>
+  </si>
+  <si>
+    <t>Kingdom Hearts 1</t>
+  </si>
+  <si>
+    <t>v1.2.5</t>
+  </si>
+  <si>
+    <t>0.3.4</t>
+  </si>
+  <si>
+    <t>1.5.3</t>
+  </si>
+  <si>
+    <t>0.4.4</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>https://github.com/DrBibop/Archipelago_Inscryption/releases</t>
+  </si>
+  <si>
+    <t>https://github.com/qwint/APMinit/releases</t>
+  </si>
+  <si>
+    <t>https://github.com/CookieCat45/Archipelago-ahit/releases</t>
+  </si>
+  <si>
+    <t>https://github.com/pseudoregalia-modding/pseudoregalia-archipelago/tags</t>
+  </si>
+  <si>
+    <t>https://github.com/CodeTriangle/CCMultiworldRandomizer/releases</t>
+  </si>
+  <si>
+    <t>https://github.com/Bartz24/Archipelago/releases</t>
+  </si>
+  <si>
+    <t>https://wiki.ctjot.com/doku.php?id=multiworld</t>
+  </si>
+  <si>
+    <t>https://github.com/cleartonic/arch_ffvcd/releases</t>
+  </si>
+  <si>
+    <t>https://github.com/gaithernOrg/ArchipelagoKHRECOM/releases</t>
+  </si>
+  <si>
+    <t>https://github.com/gaithernOrg/KH1FM-AP/releases</t>
+  </si>
+  <si>
+    <t>https://github.com/Dinopony/ArchipelagoOoS/releases</t>
+  </si>
+  <si>
+    <t>v111</t>
+  </si>
+  <si>
+    <t>https://discord.com/channels/731205301247803413/1156395911874875473</t>
+  </si>
+  <si>
+    <t>https://discord.com/channels/731205301247803413/1092478908022136876</t>
+  </si>
+  <si>
+    <t>https://github.com/qwint/ap-shahrazad/releases</t>
+  </si>
+  <si>
+    <t>https://discord.com/channels/731205301247803413/1159482310652076082</t>
+  </si>
+  <si>
+    <t>https://github.com/doshyw/CelesteArchipelago/releases</t>
+  </si>
+  <si>
+    <t>https://discord.com/channels/731205301247803413/1022545979146252288</t>
+  </si>
+  <si>
+    <t>https://discord.com/channels/731205301247803413/1169389087371841708</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,6 +207,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -184,10 +261,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -200,8 +278,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -534,22 +614,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{901AF876-1585-4DEB-9BCA-32AAC89A46F9}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -562,19 +643,28 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>21</v>
+        <v>29</v>
+      </c>
+      <c r="C2" s="5">
+        <v>45430</v>
       </c>
       <c r="D2" s="5">
-        <v>45422</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>45435</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -584,46 +674,67 @@
       <c r="D3" s="5">
         <v>45422</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="5">
         <v>45410</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D5" s="5">
         <v>45422</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>23</v>
+        <v>30</v>
+      </c>
+      <c r="C6" s="5">
+        <v>45428</v>
       </c>
       <c r="D6" s="5">
-        <v>45422</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>45435</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>19</v>
+        <v>28</v>
+      </c>
+      <c r="C7" s="5">
+        <v>45421</v>
       </c>
       <c r="D7" s="5">
-        <v>45422</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>45435</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -633,24 +744,30 @@
       <c r="D8" s="5">
         <v>45422</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="5">
-        <v>45414</v>
+        <v>45428</v>
       </c>
       <c r="D9" s="5">
-        <v>45422</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>45435</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C10" s="5">
         <v>45265</v>
@@ -658,89 +775,169 @@
       <c r="D10" s="5">
         <v>45422</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="5">
+        <v>45434</v>
+      </c>
+      <c r="D11" s="5">
+        <v>45435</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="5">
+        <v>45369</v>
+      </c>
+      <c r="D12" s="5">
+        <v>45435</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="5">
-        <v>45422</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="5">
-        <v>45410</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="5">
-        <v>45317</v>
+      <c r="B13" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="D13" s="5">
         <v>45422</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D14" s="5">
-        <v>45422</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>45410</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
+      </c>
+      <c r="C15" s="5">
+        <v>45317</v>
       </c>
       <c r="D15" s="5">
         <v>45422</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="5">
-        <v>45298</v>
+        <v>19</v>
       </c>
       <c r="D16" s="5">
         <v>45422</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="C17" s="5">
-        <v>45421</v>
+        <v>45414</v>
       </c>
       <c r="D17" s="5">
         <v>45422</v>
       </c>
+      <c r="E17" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="5">
+        <v>45429</v>
+      </c>
+      <c r="D18" s="5">
+        <v>45435</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="5">
+        <v>45428</v>
+      </c>
+      <c r="D19" s="5">
+        <v>45435</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D17">
-    <sortCondition ref="A2:A17"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D19">
+    <sortCondition ref="A2:A19"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="E13" r:id="rId1" xr:uid="{A5B7ED1F-2322-489C-9115-C445E82B54FB}"/>
+    <hyperlink ref="E12" r:id="rId2" xr:uid="{90F7D550-3232-4E6C-9AB7-856BDF3EA309}"/>
+    <hyperlink ref="E11" r:id="rId3" xr:uid="{E94C9C6D-6FA4-4184-9965-129FE7CC3A62}"/>
+    <hyperlink ref="E10" r:id="rId4" xr:uid="{5D7F93FB-6C49-403A-9AD8-F4281B6B2D94}"/>
+    <hyperlink ref="E8" r:id="rId5" xr:uid="{8C8885B9-A3DC-40DD-B18B-F3B348BB2202}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{EC4A68ED-DCD0-44C0-9669-EAC47138143B}"/>
+    <hyperlink ref="E6" r:id="rId7" xr:uid="{2531395D-2F00-44AD-B326-97CA7E60977D}"/>
+    <hyperlink ref="E5" r:id="rId8" xr:uid="{A1F02D1E-D96D-4326-BAA2-C7F18AF552BF}"/>
+    <hyperlink ref="E2" r:id="rId9" xr:uid="{570BB61D-4BF2-492C-9F85-AE7F0E875798}"/>
+    <hyperlink ref="E16" r:id="rId10" xr:uid="{39C13D86-F950-4EA9-AD8E-0CD6464A6C33}"/>
+    <hyperlink ref="E18" r:id="rId11" xr:uid="{AB23B92F-9660-4602-A770-B4DC053103FF}"/>
+    <hyperlink ref="E15" r:id="rId12" xr:uid="{AE8D7F00-E698-4DC8-8467-18A519416BF0}"/>
+    <hyperlink ref="E17" r:id="rId13" xr:uid="{2C45B0C7-121E-4FEE-90E6-19A508CC0856}"/>
+    <hyperlink ref="E19" r:id="rId14" xr:uid="{73DD7FA1-8A09-481E-9BF0-EDD88E86EAC3}"/>
+    <hyperlink ref="E4" r:id="rId15" xr:uid="{B7739609-1510-4E1E-B8C4-81240570A0B0}"/>
+    <hyperlink ref="E9" r:id="rId16" xr:uid="{9D4D35EE-2216-4D82-ABE0-0760E544D7F3}"/>
+    <hyperlink ref="E3" r:id="rId17" xr:uid="{BF5E4EB1-198E-4E95-86E7-1EF1374FF963}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the multiserver to send a goal_complete event to dynx so that she can unpin hints for completed games
</commit_message>
<xml_diff>
--- a/CustomWorldsInstalled.xlsx
+++ b/CustomWorldsInstalled.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\Git\Archipelago\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97172E97-4806-4ACC-8037-48AE0CF415A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46EEFC5C-2F8D-4524-8FE7-1DC1FB3C90A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4770" yWindow="1845" windowWidth="28800" windowHeight="15435" xr2:uid="{3DBB16FA-FE5F-4BB0-89C2-A45EA748065E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{3DBB16FA-FE5F-4BB0-89C2-A45EA748065E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>World</t>
   </si>
@@ -113,24 +113,12 @@
     <t>Kingdom Hearts Re:Chain of Memories</t>
   </si>
   <si>
-    <t>v1.2.1</t>
-  </si>
-  <si>
     <t>Kingdom Hearts 1</t>
   </si>
   <si>
-    <t>v1.2.5</t>
-  </si>
-  <si>
     <t>0.3.4</t>
   </si>
   <si>
-    <t>1.5.3</t>
-  </si>
-  <si>
-    <t>0.4.4</t>
-  </si>
-  <si>
     <t>Source</t>
   </si>
   <si>
@@ -189,6 +177,42 @@
   </si>
   <si>
     <t>https://discord.com/channels/731205301247803413/1169389087371841708</t>
+  </si>
+  <si>
+    <t>1.5.4</t>
+  </si>
+  <si>
+    <t>Last Install Date</t>
+  </si>
+  <si>
+    <t>0.5.0-pre1</t>
+  </si>
+  <si>
+    <t>v1.4.0</t>
+  </si>
+  <si>
+    <t>v1.2.7</t>
+  </si>
+  <si>
+    <t>0.3.0</t>
+  </si>
+  <si>
+    <t>Outer Wilds</t>
+  </si>
+  <si>
+    <t>0.2.1</t>
+  </si>
+  <si>
+    <t>https://github.com/Ixrec/OuterWildsArchipelagoRandomizer/releases</t>
+  </si>
+  <si>
+    <t>https://github.com/ArchipelaGOAL/Archipelago/releases</t>
+  </si>
+  <si>
+    <t>0.0.3</t>
+  </si>
+  <si>
+    <t>Jak and Daxter</t>
   </si>
 </sst>
 </file>
@@ -265,7 +289,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -279,12 +303,154 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="17">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -614,23 +780,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{901AF876-1585-4DEB-9BCA-32AAC89A46F9}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="75" customWidth="1"/>
+    <col min="14" max="14" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -644,27 +812,34 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O1" s="7">
+        <v>45435</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="C2" s="5">
-        <v>45430</v>
+        <v>45446</v>
       </c>
       <c r="D2" s="5">
-        <v>45435</v>
+        <v>45447</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="N2" s="5"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -675,21 +850,27 @@
         <v>45422</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
+      <c r="B4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="5">
+        <v>45308</v>
+      </c>
       <c r="D4" s="5">
         <v>45410</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -697,32 +878,32 @@
         <v>45422</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="C6" s="5">
-        <v>45428</v>
+        <v>45447</v>
       </c>
       <c r="D6" s="5">
-        <v>45435</v>
+        <v>45447</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C7" s="5">
         <v>45421</v>
@@ -731,10 +912,10 @@
         <v>45435</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -745,24 +926,24 @@
         <v>45422</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="5">
-        <v>45428</v>
+        <v>45438</v>
       </c>
       <c r="D9" s="5">
-        <v>45435</v>
+        <v>45447</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -776,168 +957,215 @@
         <v>45422</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="C11" s="5">
-        <v>45434</v>
+        <v>45444</v>
       </c>
       <c r="D11" s="5">
-        <v>45435</v>
+        <v>45447</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="5">
+        <v>45440</v>
+      </c>
+      <c r="D12" s="5">
+        <v>45447</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="5">
-        <v>45369</v>
-      </c>
-      <c r="D12" s="5">
-        <v>45435</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B13" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="5">
+        <v>45443</v>
+      </c>
+      <c r="D13" s="5">
+        <v>45447</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D14" s="5">
         <v>45422</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="E14" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="5">
+      <c r="B15" s="4">
+        <v>6.3</v>
+      </c>
+      <c r="C15" s="5">
+        <v>45403</v>
+      </c>
+      <c r="D15" s="5">
         <v>45410</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="5">
-        <v>45317</v>
-      </c>
-      <c r="D15" s="5">
-        <v>45422</v>
-      </c>
       <c r="E15" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>19</v>
+        <v>54</v>
+      </c>
+      <c r="C16" s="5">
+        <v>45445</v>
       </c>
       <c r="D16" s="5">
-        <v>45422</v>
+        <v>45447</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C17" s="5">
-        <v>45414</v>
+        <v>45317</v>
       </c>
       <c r="D17" s="5">
         <v>45422</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="5">
-        <v>45429</v>
+        <v>19</v>
       </c>
       <c r="D18" s="5">
-        <v>45435</v>
+        <v>45422</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="5">
+        <v>45414</v>
+      </c>
+      <c r="D19" s="5">
+        <v>45422</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="5">
+        <v>45442</v>
+      </c>
+      <c r="D20" s="5">
+        <v>45447</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C21" s="5">
         <v>45428</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D21" s="5">
         <v>45435</v>
       </c>
-      <c r="E19" s="6" t="s">
-        <v>47</v>
+      <c r="E21" s="6" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D19">
-    <sortCondition ref="A2:A19"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O21">
+    <sortCondition ref="A2:A21"/>
   </sortState>
+  <conditionalFormatting sqref="A2:XFD100">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$D2&gt;$O$1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E13" r:id="rId1" xr:uid="{A5B7ED1F-2322-489C-9115-C445E82B54FB}"/>
-    <hyperlink ref="E12" r:id="rId2" xr:uid="{90F7D550-3232-4E6C-9AB7-856BDF3EA309}"/>
-    <hyperlink ref="E11" r:id="rId3" xr:uid="{E94C9C6D-6FA4-4184-9965-129FE7CC3A62}"/>
+    <hyperlink ref="E14" r:id="rId1" xr:uid="{A5B7ED1F-2322-489C-9115-C445E82B54FB}"/>
+    <hyperlink ref="E13" r:id="rId2" xr:uid="{90F7D550-3232-4E6C-9AB7-856BDF3EA309}"/>
+    <hyperlink ref="E12" r:id="rId3" xr:uid="{E94C9C6D-6FA4-4184-9965-129FE7CC3A62}"/>
     <hyperlink ref="E10" r:id="rId4" xr:uid="{5D7F93FB-6C49-403A-9AD8-F4281B6B2D94}"/>
     <hyperlink ref="E8" r:id="rId5" xr:uid="{8C8885B9-A3DC-40DD-B18B-F3B348BB2202}"/>
     <hyperlink ref="E7" r:id="rId6" xr:uid="{EC4A68ED-DCD0-44C0-9669-EAC47138143B}"/>
     <hyperlink ref="E6" r:id="rId7" xr:uid="{2531395D-2F00-44AD-B326-97CA7E60977D}"/>
     <hyperlink ref="E5" r:id="rId8" xr:uid="{A1F02D1E-D96D-4326-BAA2-C7F18AF552BF}"/>
     <hyperlink ref="E2" r:id="rId9" xr:uid="{570BB61D-4BF2-492C-9F85-AE7F0E875798}"/>
-    <hyperlink ref="E16" r:id="rId10" xr:uid="{39C13D86-F950-4EA9-AD8E-0CD6464A6C33}"/>
-    <hyperlink ref="E18" r:id="rId11" xr:uid="{AB23B92F-9660-4602-A770-B4DC053103FF}"/>
-    <hyperlink ref="E15" r:id="rId12" xr:uid="{AE8D7F00-E698-4DC8-8467-18A519416BF0}"/>
-    <hyperlink ref="E17" r:id="rId13" xr:uid="{2C45B0C7-121E-4FEE-90E6-19A508CC0856}"/>
-    <hyperlink ref="E19" r:id="rId14" xr:uid="{73DD7FA1-8A09-481E-9BF0-EDD88E86EAC3}"/>
+    <hyperlink ref="E18" r:id="rId10" xr:uid="{39C13D86-F950-4EA9-AD8E-0CD6464A6C33}"/>
+    <hyperlink ref="E20" r:id="rId11" xr:uid="{AB23B92F-9660-4602-A770-B4DC053103FF}"/>
+    <hyperlink ref="E17" r:id="rId12" xr:uid="{AE8D7F00-E698-4DC8-8467-18A519416BF0}"/>
+    <hyperlink ref="E19" r:id="rId13" xr:uid="{2C45B0C7-121E-4FEE-90E6-19A508CC0856}"/>
+    <hyperlink ref="E21" r:id="rId14" xr:uid="{73DD7FA1-8A09-481E-9BF0-EDD88E86EAC3}"/>
     <hyperlink ref="E4" r:id="rId15" xr:uid="{B7739609-1510-4E1E-B8C4-81240570A0B0}"/>
     <hyperlink ref="E9" r:id="rId16" xr:uid="{9D4D35EE-2216-4D82-ABE0-0760E544D7F3}"/>
     <hyperlink ref="E3" r:id="rId17" xr:uid="{BF5E4EB1-198E-4E95-86E7-1EF1374FF963}"/>
+    <hyperlink ref="E16" r:id="rId18" xr:uid="{15529467-5046-410B-9B6C-654495986B9C}"/>
+    <hyperlink ref="E11" r:id="rId19" xr:uid="{65E5E7CE-44B2-4FB0-BD3D-351DBED5A38A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId18"/>
+  <pageSetup orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated installed world tracker
</commit_message>
<xml_diff>
--- a/CustomWorldsInstalled.xlsx
+++ b/CustomWorldsInstalled.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\Git\Archipelago\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46EEFC5C-2F8D-4524-8FE7-1DC1FB3C90A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A7E4F7-8CAF-44C3-B9E4-C797DA2610D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{3DBB16FA-FE5F-4BB0-89C2-A45EA748065E}"/>
   </bookViews>
@@ -98,9 +98,6 @@
     <t>0.7.2</t>
   </si>
   <si>
-    <t>0.1.0</t>
-  </si>
-  <si>
     <t>0.2.0b2</t>
   </si>
   <si>
@@ -213,6 +210,9 @@
   </si>
   <si>
     <t>Jak and Daxter</t>
+  </si>
+  <si>
+    <t>0.1.?</t>
   </si>
 </sst>
 </file>
@@ -309,140 +309,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -784,7 +651,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E31" sqref="E31"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -812,10 +679,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O1" s="7">
         <v>45435</v>
@@ -826,7 +693,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="5">
         <v>45446</v>
@@ -835,7 +702,7 @@
         <v>45447</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N2" s="5"/>
     </row>
@@ -850,7 +717,7 @@
         <v>45422</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -858,7 +725,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4" s="5">
         <v>45308</v>
@@ -867,26 +734,26 @@
         <v>45410</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="5">
         <v>45422</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="5">
         <v>45447</v>
@@ -895,7 +762,7 @@
         <v>45447</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -903,7 +770,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="5">
         <v>45421</v>
@@ -912,7 +779,7 @@
         <v>45435</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -926,7 +793,7 @@
         <v>45422</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -940,7 +807,7 @@
         <v>45447</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -948,7 +815,7 @@
         <v>17</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="5">
         <v>45265</v>
@@ -957,15 +824,15 @@
         <v>45422</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C11" s="5">
         <v>45444</v>
@@ -974,15 +841,15 @@
         <v>45447</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="5">
         <v>45440</v>
@@ -991,15 +858,15 @@
         <v>45447</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C13" s="5">
         <v>45443</v>
@@ -1008,7 +875,7 @@
         <v>45447</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -1022,7 +889,7 @@
         <v>45422</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -1039,15 +906,15 @@
         <v>45410</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="C16" s="5">
         <v>45445</v>
@@ -1056,7 +923,7 @@
         <v>45447</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1070,7 +937,7 @@
         <v>45422</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1084,7 +951,7 @@
         <v>45422</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1092,16 +959,16 @@
         <v>15</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>20</v>
+        <v>58</v>
       </c>
       <c r="C19" s="5">
-        <v>45414</v>
+        <v>45448</v>
       </c>
       <c r="D19" s="5">
-        <v>45422</v>
+        <v>45449</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1109,7 +976,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C20" s="5">
         <v>45442</v>
@@ -1118,7 +985,7 @@
         <v>45447</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1132,7 +999,7 @@
         <v>45435</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1140,7 +1007,7 @@
     <sortCondition ref="A2:A21"/>
   </sortState>
   <conditionalFormatting sqref="A2:XFD100">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>$D2&gt;$O$1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated multi-server to send a goal complete event to the webhook when a player completes their goal. Added ability to set whether the arch server is sending debuggable webhook data or not from config file. Added ability to set an admin password for all of the arch server rather than per room via config file.
</commit_message>
<xml_diff>
--- a/CustomWorldsInstalled.xlsx
+++ b/CustomWorldsInstalled.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\Git\Archipelago\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A7E4F7-8CAF-44C3-B9E4-C797DA2610D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACEC9149-33B3-4843-ABA1-EA40FED9FCB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{3DBB16FA-FE5F-4BB0-89C2-A45EA748065E}"/>
+    <workbookView xWindow="9660" yWindow="21480" windowWidth="29040" windowHeight="15840" xr2:uid="{3DBB16FA-FE5F-4BB0-89C2-A45EA748065E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -182,9 +182,6 @@
     <t>Last Install Date</t>
   </si>
   <si>
-    <t>0.5.0-pre1</t>
-  </si>
-  <si>
     <t>v1.4.0</t>
   </si>
   <si>
@@ -197,22 +194,25 @@
     <t>Outer Wilds</t>
   </si>
   <si>
-    <t>0.2.1</t>
-  </si>
-  <si>
     <t>https://github.com/Ixrec/OuterWildsArchipelagoRandomizer/releases</t>
   </si>
   <si>
     <t>https://github.com/ArchipelaGOAL/Archipelago/releases</t>
   </si>
   <si>
-    <t>0.0.3</t>
-  </si>
-  <si>
     <t>Jak and Daxter</t>
   </si>
   <si>
-    <t>0.1.?</t>
+    <t>0.5.0-pre2</t>
+  </si>
+  <si>
+    <t>0.1.1</t>
+  </si>
+  <si>
+    <t>0.0.4</t>
+  </si>
+  <si>
+    <t>0.2.3</t>
   </si>
 </sst>
 </file>
@@ -651,7 +651,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,7 +685,7 @@
         <v>47</v>
       </c>
       <c r="O1" s="7">
-        <v>45435</v>
+        <v>45449</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -725,7 +725,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" s="5">
         <v>45308</v>
@@ -753,13 +753,13 @@
         <v>21</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="C6" s="5">
-        <v>45447</v>
+        <v>45457</v>
       </c>
       <c r="D6" s="5">
-        <v>45447</v>
+        <v>45464</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>31</v>
@@ -789,6 +789,9 @@
       <c r="B8" s="4">
         <v>0.62</v>
       </c>
+      <c r="C8" s="5">
+        <v>45417</v>
+      </c>
       <c r="D8" s="5">
         <v>45422</v>
       </c>
@@ -801,10 +804,10 @@
         <v>6</v>
       </c>
       <c r="C9" s="5">
-        <v>45438</v>
+        <v>45453</v>
       </c>
       <c r="D9" s="5">
-        <v>45447</v>
+        <v>45464</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>44</v>
@@ -829,19 +832,19 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="C11" s="5">
-        <v>45444</v>
+        <v>45453</v>
       </c>
       <c r="D11" s="5">
-        <v>45447</v>
+        <v>45464</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -849,7 +852,7 @@
         <v>24</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" s="5">
         <v>45440</v>
@@ -866,7 +869,7 @@
         <v>23</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13" s="5">
         <v>45443</v>
@@ -885,6 +888,9 @@
       <c r="B14" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="C14" s="5">
+        <v>45405</v>
+      </c>
       <c r="D14" s="5">
         <v>45422</v>
       </c>
@@ -911,19 +917,19 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="5">
+        <v>45453</v>
+      </c>
+      <c r="D16" s="5">
+        <v>45464</v>
+      </c>
+      <c r="E16" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="5">
-        <v>45445</v>
-      </c>
-      <c r="D16" s="5">
-        <v>45447</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -959,13 +965,13 @@
         <v>15</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C19" s="5">
-        <v>45448</v>
+        <v>45457</v>
       </c>
       <c r="D19" s="5">
-        <v>45449</v>
+        <v>45464</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Added new option to seed generation to allow the seed to be tracked by discord. Add more relevant logging to the macros html to help differentiate between no file available and unsupported file type.
</commit_message>
<xml_diff>
--- a/CustomWorldsInstalled.xlsx
+++ b/CustomWorldsInstalled.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\Git\Archipelago\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D7DEC1A-A62C-4090-A7CF-EF5649474A11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4175E9D3-DC6D-4DB9-A362-CB9EFB0090BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{3DBB16FA-FE5F-4BB0-89C2-A45EA748065E}"/>
+    <workbookView xWindow="5010" yWindow="0" windowWidth="28800" windowHeight="15435" xr2:uid="{3DBB16FA-FE5F-4BB0-89C2-A45EA748065E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
   <si>
     <t>World</t>
   </si>
@@ -180,12 +180,6 @@
   </si>
   <si>
     <t>0.6.4</t>
-  </si>
-  <si>
-    <t>0.5.0</t>
-  </si>
-  <si>
-    <t>1.4.1</t>
   </si>
   <si>
     <t>Fire Emblem 8</t>
@@ -204,15 +198,9 @@
     <t>0.82.5</t>
   </si>
   <si>
-    <t>0.2.5</t>
-  </si>
-  <si>
     <t>0.0.9</t>
   </si>
   <si>
-    <t>2.3.2</t>
-  </si>
-  <si>
     <t>0.3.7</t>
   </si>
   <si>
@@ -232,6 +220,72 @@
   </si>
   <si>
     <t>https://github.com/lilymnky-F/Archipelago-Osu/releases</t>
+  </si>
+  <si>
+    <t>1.4.2</t>
+  </si>
+  <si>
+    <t>0.6.0</t>
+  </si>
+  <si>
+    <t>2.3.4</t>
+  </si>
+  <si>
+    <t>7.2b</t>
+  </si>
+  <si>
+    <t>0.2.6</t>
+  </si>
+  <si>
+    <t>Super Metroid Subversion</t>
+  </si>
+  <si>
+    <t>https://discord.com/channels/731205301247803413/1146853510378422272</t>
+  </si>
+  <si>
+    <t>EarthBound</t>
+  </si>
+  <si>
+    <t>Animal Well</t>
+  </si>
+  <si>
+    <t>0.3.1</t>
+  </si>
+  <si>
+    <t>https://github.com/ScipioWright/Archipelago-SW/releases</t>
+  </si>
+  <si>
+    <t>Pokemon Crystal</t>
+  </si>
+  <si>
+    <t>https://github.com/AliceMousie/Archipelago/releases</t>
+  </si>
+  <si>
+    <t>2.1.2</t>
+  </si>
+  <si>
+    <t>Pokemon FireRed and LeafGreen</t>
+  </si>
+  <si>
+    <t>0.5.2</t>
+  </si>
+  <si>
+    <t>https://github.com/vyneras/Archipelago/releases</t>
+  </si>
+  <si>
+    <t>Shapez</t>
+  </si>
+  <si>
+    <t>0.1.2</t>
+  </si>
+  <si>
+    <t>https://github.com/BlastSlimey/shapezipelago/releases</t>
+  </si>
+  <si>
+    <t>https://github.com/PinkSwitch/Archipelago/releases/</t>
+  </si>
+  <si>
+    <t>1.4.1</t>
   </si>
 </sst>
 </file>
@@ -672,11 +726,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{901AF876-1585-4DEB-9BCA-32AAC89A46F9}">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,393 +764,492 @@
         <v>40</v>
       </c>
       <c r="O1" s="6">
-        <v>45478</v>
+        <v>45507</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>8</v>
+        <v>69</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C2" s="4">
-        <v>45274</v>
+        <v>45519</v>
       </c>
       <c r="D2" s="4">
-        <v>45422</v>
+        <v>45519</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="C3" s="4">
-        <v>45308</v>
+        <v>45274</v>
       </c>
       <c r="D3" s="4">
-        <v>45410</v>
+        <v>45422</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>19</v>
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="4">
+        <v>45308</v>
       </c>
       <c r="D4" s="4">
-        <v>45422</v>
+        <v>45410</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5" s="4">
-        <v>45477</v>
+        <v>19</v>
       </c>
       <c r="D5" s="4">
-        <v>45478</v>
+        <v>45519</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C6" s="4">
-        <v>45493</v>
+        <v>45517</v>
       </c>
       <c r="D6" s="4">
-        <v>45507</v>
+        <v>45519</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>5</v>
+        <v>68</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="C7" s="4">
-        <v>45493</v>
+        <v>45506</v>
       </c>
       <c r="D7" s="4">
-        <v>45507</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>53</v>
+        <v>45519</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="C8" s="4">
-        <v>45467</v>
+        <v>45493</v>
       </c>
       <c r="D8" s="4">
-        <v>45478</v>
+        <v>45507</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="4">
+        <v>45493</v>
+      </c>
+      <c r="D9" s="4">
+        <v>45507</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>51</v>
-      </c>
-      <c r="C9" s="4">
-        <v>45425</v>
-      </c>
-      <c r="D9" s="4">
-        <v>45478</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="C10" s="4">
-        <v>45476</v>
+        <v>45467</v>
       </c>
       <c r="D10" s="4">
-        <v>45507</v>
+        <v>45478</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C11" s="4">
-        <v>45507</v>
+        <v>45425</v>
       </c>
       <c r="D11" s="4">
-        <v>45507</v>
+        <v>45478</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="C12" s="4">
-        <v>45504</v>
+        <v>45479</v>
       </c>
       <c r="D12" s="4">
         <v>45507</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>61</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C13" s="4">
-        <v>45500</v>
+        <v>45507</v>
       </c>
       <c r="D13" s="4">
         <v>45507</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C14" s="4">
-        <v>45467</v>
+        <v>45504</v>
       </c>
       <c r="D14" s="4">
-        <v>45478</v>
+        <v>45507</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="C15" s="4">
-        <v>45467</v>
+        <v>45517</v>
       </c>
       <c r="D15" s="4">
-        <v>45478</v>
+        <v>45519</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="3">
-        <v>7.2</v>
+        <v>20</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="C16" s="4">
-        <v>45500</v>
+        <v>45516</v>
       </c>
       <c r="D16" s="4">
-        <v>45507</v>
+        <v>45519</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="C17" s="4">
-        <v>45476</v>
+        <v>45466</v>
       </c>
       <c r="D17" s="4">
-        <v>45507</v>
+        <v>45478</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="C18" s="4">
-        <v>45500</v>
+        <v>45516</v>
       </c>
       <c r="D18" s="4">
-        <v>45507</v>
+        <v>45519</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>13</v>
+        <v>58</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="C19" s="4">
-        <v>45317</v>
+        <v>45478</v>
       </c>
       <c r="D19" s="4">
-        <v>45422</v>
+        <v>45507</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>17</v>
+        <v>65</v>
+      </c>
+      <c r="C20" s="4">
+        <v>45516</v>
       </c>
       <c r="D20" s="4">
-        <v>45422</v>
+        <v>45519</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="C21" s="4">
-        <v>45457</v>
+        <v>45317</v>
       </c>
       <c r="D21" s="4">
-        <v>45464</v>
+        <v>45422</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
       <c r="C22" s="4">
-        <v>45442</v>
+        <v>45488</v>
       </c>
       <c r="D22" s="4">
-        <v>45447</v>
+        <v>45519</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="4">
+        <v>45518</v>
+      </c>
+      <c r="D23" s="4">
+        <v>45519</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="4">
+        <v>45422</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="4">
+        <v>45457</v>
+      </c>
+      <c r="D25" s="4">
+        <v>45464</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" s="4">
+        <v>45518</v>
+      </c>
+      <c r="D26" s="4">
+        <v>45519</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="4">
+        <v>45442</v>
+      </c>
+      <c r="D27" s="4">
+        <v>45447</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4">
+        <v>45519</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C29" s="4">
         <v>45476</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D29" s="4">
         <v>45478</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E29" s="5" t="s">
         <v>36</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O23">
-    <sortCondition ref="A2:A23"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O29">
+    <sortCondition ref="A2:A29"/>
   </sortState>
-  <conditionalFormatting sqref="A2:XFD101">
+  <conditionalFormatting sqref="A2:XFD107">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>$D2&gt;$O$1</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E15" r:id="rId1" xr:uid="{A5B7ED1F-2322-489C-9115-C445E82B54FB}"/>
-    <hyperlink ref="E14" r:id="rId2" xr:uid="{90F7D550-3232-4E6C-9AB7-856BDF3EA309}"/>
-    <hyperlink ref="E13" r:id="rId3" xr:uid="{E94C9C6D-6FA4-4184-9965-129FE7CC3A62}"/>
-    <hyperlink ref="E10" r:id="rId4" xr:uid="{5D7F93FB-6C49-403A-9AD8-F4281B6B2D94}"/>
-    <hyperlink ref="E7" r:id="rId5" display="https://github.com/cleartonic/arch_ffvcd/releases" xr:uid="{8C8885B9-A3DC-40DD-B18B-F3B348BB2202}"/>
-    <hyperlink ref="E6" r:id="rId6" xr:uid="{EC4A68ED-DCD0-44C0-9669-EAC47138143B}"/>
-    <hyperlink ref="E5" r:id="rId7" xr:uid="{2531395D-2F00-44AD-B326-97CA7E60977D}"/>
-    <hyperlink ref="E4" r:id="rId8" xr:uid="{A1F02D1E-D96D-4326-BAA2-C7F18AF552BF}"/>
-    <hyperlink ref="E20" r:id="rId9" xr:uid="{39C13D86-F950-4EA9-AD8E-0CD6464A6C33}"/>
-    <hyperlink ref="E22" r:id="rId10" xr:uid="{AB23B92F-9660-4602-A770-B4DC053103FF}"/>
-    <hyperlink ref="E19" r:id="rId11" xr:uid="{AE8D7F00-E698-4DC8-8467-18A519416BF0}"/>
-    <hyperlink ref="E21" r:id="rId12" xr:uid="{2C45B0C7-121E-4FEE-90E6-19A508CC0856}"/>
-    <hyperlink ref="E23" r:id="rId13" xr:uid="{73DD7FA1-8A09-481E-9BF0-EDD88E86EAC3}"/>
-    <hyperlink ref="E3" r:id="rId14" xr:uid="{B7739609-1510-4E1E-B8C4-81240570A0B0}"/>
-    <hyperlink ref="E8" r:id="rId15" xr:uid="{9D4D35EE-2216-4D82-ABE0-0760E544D7F3}"/>
+    <hyperlink ref="E17" r:id="rId1" xr:uid="{A5B7ED1F-2322-489C-9115-C445E82B54FB}"/>
+    <hyperlink ref="E16" r:id="rId2" xr:uid="{90F7D550-3232-4E6C-9AB7-856BDF3EA309}"/>
+    <hyperlink ref="E15" r:id="rId3" xr:uid="{E94C9C6D-6FA4-4184-9965-129FE7CC3A62}"/>
+    <hyperlink ref="E12" r:id="rId4" xr:uid="{5D7F93FB-6C49-403A-9AD8-F4281B6B2D94}"/>
+    <hyperlink ref="E9" r:id="rId5" display="https://github.com/cleartonic/arch_ffvcd/releases" xr:uid="{8C8885B9-A3DC-40DD-B18B-F3B348BB2202}"/>
+    <hyperlink ref="E8" r:id="rId6" xr:uid="{EC4A68ED-DCD0-44C0-9669-EAC47138143B}"/>
+    <hyperlink ref="E6" r:id="rId7" xr:uid="{2531395D-2F00-44AD-B326-97CA7E60977D}"/>
+    <hyperlink ref="E5" r:id="rId8" xr:uid="{A1F02D1E-D96D-4326-BAA2-C7F18AF552BF}"/>
+    <hyperlink ref="E24" r:id="rId9" xr:uid="{39C13D86-F950-4EA9-AD8E-0CD6464A6C33}"/>
+    <hyperlink ref="E27" r:id="rId10" xr:uid="{AB23B92F-9660-4602-A770-B4DC053103FF}"/>
+    <hyperlink ref="E21" r:id="rId11" xr:uid="{AE8D7F00-E698-4DC8-8467-18A519416BF0}"/>
+    <hyperlink ref="E25" r:id="rId12" xr:uid="{2C45B0C7-121E-4FEE-90E6-19A508CC0856}"/>
+    <hyperlink ref="E29" r:id="rId13" xr:uid="{73DD7FA1-8A09-481E-9BF0-EDD88E86EAC3}"/>
+    <hyperlink ref="E4" r:id="rId14" xr:uid="{B7739609-1510-4E1E-B8C4-81240570A0B0}"/>
+    <hyperlink ref="E10" r:id="rId15" xr:uid="{9D4D35EE-2216-4D82-ABE0-0760E544D7F3}"/>
     <hyperlink ref="E2" r:id="rId16" xr:uid="{BF5E4EB1-198E-4E95-86E7-1EF1374FF963}"/>
-    <hyperlink ref="E18" r:id="rId17" xr:uid="{15529467-5046-410B-9B6C-654495986B9C}"/>
-    <hyperlink ref="E11" r:id="rId18" xr:uid="{65E5E7CE-44B2-4FB0-BD3D-351DBED5A38A}"/>
-    <hyperlink ref="E9" r:id="rId19" xr:uid="{75A12DC5-3325-4C7B-9F69-1A0B70EF2357}"/>
+    <hyperlink ref="E20" r:id="rId17" xr:uid="{15529467-5046-410B-9B6C-654495986B9C}"/>
+    <hyperlink ref="E13" r:id="rId18" xr:uid="{65E5E7CE-44B2-4FB0-BD3D-351DBED5A38A}"/>
+    <hyperlink ref="E11" r:id="rId19" xr:uid="{75A12DC5-3325-4C7B-9F69-1A0B70EF2357}"/>
+    <hyperlink ref="E3" r:id="rId20" xr:uid="{6A5A7183-040B-4C7C-A5E8-B8E3C0F52BCD}"/>
+    <hyperlink ref="E7" r:id="rId21" xr:uid="{C789739C-B0F4-4CB3-956F-269CAF2DFC8D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId20"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added new feature to set hint priority in the text clients. Updated and added new worlds
</commit_message>
<xml_diff>
--- a/CustomWorldsInstalled.xlsx
+++ b/CustomWorldsInstalled.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\Git\Archipelago\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4175E9D3-DC6D-4DB9-A362-CB9EFB0090BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF9986ED-1B1D-4DFD-B172-086ABBD8A9FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5010" yWindow="0" windowWidth="28800" windowHeight="15435" xr2:uid="{3DBB16FA-FE5F-4BB0-89C2-A45EA748065E}"/>
+    <workbookView xWindow="9300" yWindow="21480" windowWidth="29040" windowHeight="15840" xr2:uid="{3DBB16FA-FE5F-4BB0-89C2-A45EA748065E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="96">
   <si>
     <t>World</t>
   </si>
@@ -198,12 +198,6 @@
     <t>0.82.5</t>
   </si>
   <si>
-    <t>0.0.9</t>
-  </si>
-  <si>
-    <t>0.3.7</t>
-  </si>
-  <si>
     <t>Kingdom Hearts: Birth by Sleep</t>
   </si>
   <si>
@@ -228,15 +222,9 @@
     <t>0.6.0</t>
   </si>
   <si>
-    <t>2.3.4</t>
-  </si>
-  <si>
     <t>7.2b</t>
   </si>
   <si>
-    <t>0.2.6</t>
-  </si>
-  <si>
     <t>Super Metroid Subversion</t>
   </si>
   <si>
@@ -267,25 +255,76 @@
     <t>Pokemon FireRed and LeafGreen</t>
   </si>
   <si>
-    <t>0.5.2</t>
-  </si>
-  <si>
     <t>https://github.com/vyneras/Archipelago/releases</t>
   </si>
   <si>
     <t>Shapez</t>
   </si>
   <si>
-    <t>0.1.2</t>
-  </si>
-  <si>
     <t>https://github.com/BlastSlimey/shapezipelago/releases</t>
   </si>
   <si>
     <t>https://github.com/PinkSwitch/Archipelago/releases/</t>
   </si>
   <si>
-    <t>1.4.1</t>
+    <t>0.6.1</t>
+  </si>
+  <si>
+    <t>0.3.8</t>
+  </si>
+  <si>
+    <t>2.4.0</t>
+  </si>
+  <si>
+    <t>0.0.10</t>
+  </si>
+  <si>
+    <t>0.2.7</t>
+  </si>
+  <si>
+    <t>2.0.1</t>
+  </si>
+  <si>
+    <t>0.4.0</t>
+  </si>
+  <si>
+    <t>Rollercoaster Tycoon 2</t>
+  </si>
+  <si>
+    <t>https://github.com/Crazycolbster/rollercoaster-tycoon-randomizer/releases</t>
+  </si>
+  <si>
+    <t>Satisfactory</t>
+  </si>
+  <si>
+    <t>0.1.3.3</t>
+  </si>
+  <si>
+    <t>https://github.com/Jarno458/SatisfactoryArchipelagoMod/releases</t>
+  </si>
+  <si>
+    <t>Yacht Dice</t>
+  </si>
+  <si>
+    <t>2.1.1</t>
+  </si>
+  <si>
+    <t>https://github.com/spinerak/ArchipelagoYachtDice/releases</t>
+  </si>
+  <si>
+    <t>Mindustry</t>
+  </si>
+  <si>
+    <t>https://github.com/JohnMahglass/Archipelago-Mindustry/releases</t>
+  </si>
+  <si>
+    <t>https://github.com/lilDavid/Archipelago-Metroid-Zero-Mission/releases</t>
+  </si>
+  <si>
+    <t>Metroid Zero Mission</t>
+  </si>
+  <si>
+    <t>0.2.0-pre3</t>
   </si>
 </sst>
 </file>
@@ -726,11 +765,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{901AF876-1585-4DEB-9BCA-32AAC89A46F9}">
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,24 +803,24 @@
         <v>40</v>
       </c>
       <c r="O1" s="6">
-        <v>45507</v>
+        <v>45519</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="C2" s="4">
-        <v>45519</v>
+        <v>45529</v>
       </c>
       <c r="D2" s="4">
-        <v>45519</v>
+        <v>45533</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -831,13 +870,13 @@
         <v>18</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="C6" s="4">
-        <v>45517</v>
+        <v>45533</v>
       </c>
       <c r="D6" s="4">
-        <v>45519</v>
+        <v>45533</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>26</v>
@@ -845,19 +884,19 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C7" s="4">
-        <v>45506</v>
+        <v>45529</v>
       </c>
       <c r="D7" s="4">
-        <v>45519</v>
+        <v>45533</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -865,13 +904,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="C8" s="4">
-        <v>45493</v>
+        <v>45528</v>
       </c>
       <c r="D8" s="4">
-        <v>45507</v>
+        <v>45533</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>27</v>
@@ -947,13 +986,13 @@
         <v>45</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>53</v>
+        <v>79</v>
       </c>
       <c r="C13" s="4">
-        <v>45507</v>
+        <v>45528</v>
       </c>
       <c r="D13" s="4">
-        <v>45507</v>
+        <v>45533</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>44</v>
@@ -961,10 +1000,10 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C14" s="4">
         <v>45504</v>
@@ -973,7 +1012,7 @@
         <v>45507</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -981,13 +1020,13 @@
         <v>21</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="C15" s="4">
         <v>45517</v>
       </c>
       <c r="D15" s="4">
-        <v>45519</v>
+        <v>45533</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>30</v>
@@ -998,7 +1037,7 @@
         <v>20</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C16" s="4">
         <v>45516</v>
@@ -1012,61 +1051,61 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>11</v>
+        <v>94</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="C17" s="4">
-        <v>45466</v>
+        <v>45533</v>
       </c>
       <c r="D17" s="4">
-        <v>45478</v>
+        <v>45533</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>9</v>
+        <v>91</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="C18" s="4">
-        <v>45516</v>
+        <v>45528</v>
       </c>
       <c r="D18" s="4">
-        <v>45519</v>
+        <v>45533</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>31</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>58</v>
+        <v>11</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C19" s="4">
+        <v>45466</v>
+      </c>
+      <c r="D19" s="4">
         <v>45478</v>
       </c>
-      <c r="D19" s="4">
-        <v>45507</v>
-      </c>
       <c r="E19" s="5" t="s">
-        <v>60</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C20" s="4">
         <v>45516</v>
@@ -1075,159 +1114,241 @@
         <v>45519</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>13</v>
+        <v>56</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="C21" s="4">
-        <v>45317</v>
+        <v>45478</v>
       </c>
       <c r="D21" s="4">
-        <v>45422</v>
+        <v>45507</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="C22" s="4">
-        <v>45488</v>
+        <v>45532</v>
       </c>
       <c r="D22" s="4">
-        <v>45519</v>
+        <v>45533</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>76</v>
+        <v>13</v>
       </c>
       <c r="C23" s="4">
-        <v>45518</v>
+        <v>45317</v>
       </c>
       <c r="D23" s="4">
-        <v>45519</v>
+        <v>45422</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>77</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>12</v>
+        <v>68</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>17</v>
+        <v>70</v>
+      </c>
+      <c r="C24" s="4">
+        <v>45488</v>
       </c>
       <c r="D24" s="4">
-        <v>45422</v>
+        <v>45519</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>14</v>
+        <v>71</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="C25" s="4">
-        <v>45457</v>
+        <v>45533</v>
       </c>
       <c r="D25" s="4">
-        <v>45464</v>
+        <v>45533</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>35</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>78</v>
+        <v>12</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C26" s="4">
-        <v>45518</v>
+        <v>17</v>
       </c>
       <c r="D26" s="4">
-        <v>45519</v>
+        <v>45422</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>80</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="C27" s="4">
-        <v>45442</v>
+        <v>45479</v>
       </c>
       <c r="D27" s="4">
-        <v>45447</v>
+        <v>45533</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>33</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C28" s="4"/>
+        <v>85</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" s="4">
+        <v>45376</v>
+      </c>
       <c r="D28" s="4">
-        <v>45519</v>
+        <v>45533</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="4">
+        <v>45457</v>
+      </c>
+      <c r="D29" s="4">
+        <v>45464</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="4">
+        <v>45530</v>
+      </c>
+      <c r="D30" s="4">
+        <v>45533</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="4">
+        <v>45442</v>
+      </c>
+      <c r="D31" s="4">
+        <v>45447</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4">
+        <v>45519</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C33" s="4">
         <v>45476</v>
       </c>
-      <c r="D29" s="4">
+      <c r="D33" s="4">
         <v>45478</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="E33" s="5" t="s">
         <v>36</v>
       </c>
     </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" s="4">
+        <v>45526</v>
+      </c>
+      <c r="D34" s="4">
+        <v>45533</v>
+      </c>
+      <c r="E34" t="s">
+        <v>90</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O29">
-    <sortCondition ref="A2:A29"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O33">
+    <sortCondition ref="A2:A33"/>
   </sortState>
-  <conditionalFormatting sqref="A2:XFD107">
+  <conditionalFormatting sqref="A2:XFD111">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>$D2&gt;$O$1</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E17" r:id="rId1" xr:uid="{A5B7ED1F-2322-489C-9115-C445E82B54FB}"/>
+    <hyperlink ref="E19" r:id="rId1" xr:uid="{A5B7ED1F-2322-489C-9115-C445E82B54FB}"/>
     <hyperlink ref="E16" r:id="rId2" xr:uid="{90F7D550-3232-4E6C-9AB7-856BDF3EA309}"/>
     <hyperlink ref="E15" r:id="rId3" xr:uid="{E94C9C6D-6FA4-4184-9965-129FE7CC3A62}"/>
     <hyperlink ref="E12" r:id="rId4" xr:uid="{5D7F93FB-6C49-403A-9AD8-F4281B6B2D94}"/>
@@ -1235,15 +1356,15 @@
     <hyperlink ref="E8" r:id="rId6" xr:uid="{EC4A68ED-DCD0-44C0-9669-EAC47138143B}"/>
     <hyperlink ref="E6" r:id="rId7" xr:uid="{2531395D-2F00-44AD-B326-97CA7E60977D}"/>
     <hyperlink ref="E5" r:id="rId8" xr:uid="{A1F02D1E-D96D-4326-BAA2-C7F18AF552BF}"/>
-    <hyperlink ref="E24" r:id="rId9" xr:uid="{39C13D86-F950-4EA9-AD8E-0CD6464A6C33}"/>
-    <hyperlink ref="E27" r:id="rId10" xr:uid="{AB23B92F-9660-4602-A770-B4DC053103FF}"/>
-    <hyperlink ref="E21" r:id="rId11" xr:uid="{AE8D7F00-E698-4DC8-8467-18A519416BF0}"/>
-    <hyperlink ref="E25" r:id="rId12" xr:uid="{2C45B0C7-121E-4FEE-90E6-19A508CC0856}"/>
-    <hyperlink ref="E29" r:id="rId13" xr:uid="{73DD7FA1-8A09-481E-9BF0-EDD88E86EAC3}"/>
+    <hyperlink ref="E26" r:id="rId9" xr:uid="{39C13D86-F950-4EA9-AD8E-0CD6464A6C33}"/>
+    <hyperlink ref="E31" r:id="rId10" xr:uid="{AB23B92F-9660-4602-A770-B4DC053103FF}"/>
+    <hyperlink ref="E23" r:id="rId11" xr:uid="{AE8D7F00-E698-4DC8-8467-18A519416BF0}"/>
+    <hyperlink ref="E29" r:id="rId12" xr:uid="{2C45B0C7-121E-4FEE-90E6-19A508CC0856}"/>
+    <hyperlink ref="E33" r:id="rId13" xr:uid="{73DD7FA1-8A09-481E-9BF0-EDD88E86EAC3}"/>
     <hyperlink ref="E4" r:id="rId14" xr:uid="{B7739609-1510-4E1E-B8C4-81240570A0B0}"/>
     <hyperlink ref="E10" r:id="rId15" xr:uid="{9D4D35EE-2216-4D82-ABE0-0760E544D7F3}"/>
     <hyperlink ref="E2" r:id="rId16" xr:uid="{BF5E4EB1-198E-4E95-86E7-1EF1374FF963}"/>
-    <hyperlink ref="E20" r:id="rId17" xr:uid="{15529467-5046-410B-9B6C-654495986B9C}"/>
+    <hyperlink ref="E22" r:id="rId17" xr:uid="{15529467-5046-410B-9B6C-654495986B9C}"/>
     <hyperlink ref="E13" r:id="rId18" xr:uid="{65E5E7CE-44B2-4FB0-BD3D-351DBED5A38A}"/>
     <hyperlink ref="E11" r:id="rId19" xr:uid="{75A12DC5-3325-4C7B-9F69-1A0B70EF2357}"/>
     <hyperlink ref="E3" r:id="rId20" xr:uid="{6A5A7183-040B-4C7C-A5E8-B8E3C0F52BCD}"/>

</xml_diff>

<commit_message>
Updated worlds to latest versions
</commit_message>
<xml_diff>
--- a/CustomWorldsInstalled.xlsx
+++ b/CustomWorldsInstalled.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\Git\Archipelago\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D301C79-9965-457C-8BF1-79CC02B63CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94696357-5619-4A0C-A8B5-01E1E8676929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16980" yWindow="0" windowWidth="21420" windowHeight="21000" xr2:uid="{3DBB16FA-FE5F-4BB0-89C2-A45EA748065E}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{3DBB16FA-FE5F-4BB0-89C2-A45EA748065E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="180">
   <si>
     <t>World</t>
   </si>
@@ -192,9 +192,6 @@
     <t>Osu!</t>
   </si>
   <si>
-    <t>1.0.2</t>
-  </si>
-  <si>
     <t>https://github.com/lilymnky-F/Archipelago-Osu/releases</t>
   </si>
   <si>
@@ -294,31 +291,19 @@
     <t>Discord Discussion Post</t>
   </si>
   <si>
-    <t>2.4.1</t>
-  </si>
-  <si>
     <t>Link Between Worlds</t>
   </si>
   <si>
     <t>https://github.com/randomsalience/albw-archipelago/releases</t>
   </si>
   <si>
-    <t>0.2.0</t>
-  </si>
-  <si>
     <t>0.4.2</t>
   </si>
   <si>
     <t>0.1.2</t>
   </si>
   <si>
-    <t>2.1.3</t>
-  </si>
-  <si>
     <t>Sonic Adventure DX</t>
-  </si>
-  <si>
-    <t>0.8.6</t>
   </si>
   <si>
     <t>https://github.com/ClassicSpeed/sadx-classic-randomizer/releases</t>
@@ -484,18 +469,9 @@
 https://github.com/Anguirel86/Archipelago/tree/ctjot</t>
   </si>
   <si>
-    <t>0.6.0</t>
-  </si>
-  <si>
-    <t>0.3.2</t>
-  </si>
-  <si>
     <t>0.1.13</t>
   </si>
   <si>
-    <t>0.5.5</t>
-  </si>
-  <si>
     <t>Spyro 3</t>
   </si>
   <si>
@@ -545,6 +521,63 @@
   </si>
   <si>
     <t>https://discord.com/channels/731205301247803413/1210743818564149288</t>
+  </si>
+  <si>
+    <t>2.3.1</t>
+  </si>
+  <si>
+    <t>0.4.0</t>
+  </si>
+  <si>
+    <t>2.4.3</t>
+  </si>
+  <si>
+    <t>0.2.1</t>
+  </si>
+  <si>
+    <t>0.3.6.1</t>
+  </si>
+  <si>
+    <t>0.7.3</t>
+  </si>
+  <si>
+    <t>0.0.2</t>
+  </si>
+  <si>
+    <t>https://github.com/choatix/Archipelago/releases</t>
+  </si>
+  <si>
+    <t>0.5.8</t>
+  </si>
+  <si>
+    <t>0.8.8</t>
+  </si>
+  <si>
+    <t>2.1.4</t>
+  </si>
+  <si>
+    <t>Bingo</t>
+  </si>
+  <si>
+    <t>0.1.7</t>
+  </si>
+  <si>
+    <t>https://github.com/Cynichill/APBingo/releases</t>
+  </si>
+  <si>
+    <t>https://discord.com/channels/731205301247803413/1252051532971638784</t>
+  </si>
+  <si>
+    <t>0.0.1</t>
+  </si>
+  <si>
+    <t>https://github.com/spineraks-org/ArchipelagoWateryWords/releases</t>
+  </si>
+  <si>
+    <t>https://discord.com/channels/731205301247803413/1292965246847418388</t>
+  </si>
+  <si>
+    <t>Watery Words</t>
   </si>
 </sst>
 </file>
@@ -988,11 +1021,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{901AF876-1585-4DEB-9BCA-32AAC89A46F9}">
-  <dimension ref="A1:O48"/>
+  <dimension ref="A1:O50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A43" sqref="A43:XFD43"/>
+      <selection pane="bottomLeft" activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1011,7 +1044,7 @@
     <col min="12" max="12" width="9.140625" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="6" customWidth="1"/>
     <col min="14" max="14" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1028,16 +1061,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>83</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>84</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>35</v>
       </c>
       <c r="O1" s="6">
-        <v>45562</v>
+        <v>45575</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -1059,10 +1092,10 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C3" s="4">
         <v>45548</v>
@@ -1071,612 +1104,615 @@
         <v>45562</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C4" s="4">
+        <v>45602</v>
+      </c>
+      <c r="D4" s="4">
+        <v>45603</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C5" s="4">
         <v>45308</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D5" s="4">
         <v>45410</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="F5" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D6" s="4">
         <v>45519</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" s="4">
-        <v>45533</v>
-      </c>
-      <c r="D6" s="4">
-        <v>45533</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>22</v>
+      <c r="E6" s="7" t="s">
+        <v>142</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B7" s="3">
-        <v>2.1</v>
+        <v>15</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="C7" s="4">
-        <v>45555</v>
+        <v>45533</v>
       </c>
       <c r="D7" s="4">
-        <v>45562</v>
+        <v>45533</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>68</v>
+        <v>22</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="B8" s="3">
-        <v>0.3</v>
+        <v>56</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>161</v>
       </c>
       <c r="C8" s="4">
-        <v>45539</v>
+        <v>45600</v>
       </c>
       <c r="D8" s="4">
-        <v>45575</v>
+        <v>45603</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>156</v>
+        <v>67</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>148</v>
+        <v>99</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.3</v>
       </c>
       <c r="C9" s="4">
-        <v>45563</v>
+        <v>45539</v>
       </c>
       <c r="D9" s="4">
         <v>45575</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>82</v>
+        <v>148</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>105</v>
+        <v>80</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="4">
+        <v>45589</v>
+      </c>
+      <c r="D10" s="4">
+        <v>45603</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C11" s="4">
         <v>45493</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D11" s="4">
         <v>45507</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E11" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="C11" s="4">
-        <v>45526</v>
-      </c>
-      <c r="D11" s="4">
-        <v>45562</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="F11" s="5" t="s">
-        <v>33</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C12" s="4">
-        <v>45557</v>
+        <v>45526</v>
       </c>
       <c r="D12" s="4">
         <v>45562</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>121</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>43</v>
+        <v>98</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>44</v>
+        <v>86</v>
       </c>
       <c r="C13" s="4">
-        <v>45425</v>
+        <v>45557</v>
       </c>
       <c r="D13" s="4">
-        <v>45478</v>
+        <v>45562</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>145</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="C14" s="4">
-        <v>45542</v>
+        <v>45425</v>
       </c>
       <c r="D14" s="4">
-        <v>45547</v>
+        <v>45478</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>88</v>
+        <v>58</v>
       </c>
       <c r="C15" s="4">
-        <v>45568</v>
+        <v>45542</v>
       </c>
       <c r="D15" s="4">
-        <v>45575</v>
+        <v>45547</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>124</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>85</v>
+        <v>162</v>
       </c>
       <c r="C16" s="4">
-        <v>45540</v>
+        <v>45597</v>
       </c>
       <c r="D16" s="4">
-        <v>45547</v>
+        <v>45603</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>53</v>
+        <v>163</v>
       </c>
       <c r="C17" s="4">
-        <v>45516</v>
+        <v>45589</v>
       </c>
       <c r="D17" s="4">
-        <v>45519</v>
+        <v>45603</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>90</v>
+        <v>52</v>
       </c>
       <c r="C18" s="4">
-        <v>45555</v>
+        <v>45516</v>
       </c>
       <c r="D18" s="4">
-        <v>45562</v>
+        <v>45519</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>86</v>
+        <v>48</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>41</v>
+        <v>87</v>
       </c>
       <c r="C19" s="4">
-        <v>45527</v>
+        <v>45555</v>
       </c>
       <c r="D19" s="4">
-        <v>45547</v>
+        <v>45562</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>108</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="C20" s="4">
-        <v>45414</v>
+        <v>45527</v>
       </c>
       <c r="D20" s="4">
-        <v>45562</v>
+        <v>45547</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>98</v>
+        <v>58</v>
       </c>
       <c r="C21" s="4">
-        <v>45528</v>
+        <v>45414</v>
       </c>
       <c r="D21" s="4">
         <v>45562</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C22" s="4">
-        <v>45555</v>
+        <v>45528</v>
       </c>
       <c r="D22" s="4">
         <v>45562</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>142</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C23" s="4">
-        <v>45527</v>
+        <v>45555</v>
       </c>
       <c r="D23" s="4">
         <v>45562</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C24" s="4">
-        <v>45540</v>
+        <v>45527</v>
       </c>
       <c r="D24" s="4">
-        <v>45547</v>
+        <v>45562</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>88</v>
+        <v>164</v>
       </c>
       <c r="C25" s="4">
-        <v>45555</v>
+        <v>45602</v>
       </c>
       <c r="D25" s="4">
-        <v>45562</v>
+        <v>45603</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>78</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C26" s="4">
-        <v>45466</v>
+        <v>45597</v>
       </c>
       <c r="D26" s="4">
-        <v>45478</v>
+        <v>45603</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>20</v>
+        <v>77</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
-        <v>112</v>
+        <v>8</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>157</v>
+        <v>42</v>
       </c>
       <c r="C27" s="4">
-        <v>45544</v>
+        <v>45466</v>
       </c>
       <c r="D27" s="4">
-        <v>45575</v>
+        <v>45478</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>158</v>
+        <v>20</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>113</v>
+        <v>136</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>54</v>
+        <v>149</v>
       </c>
       <c r="C28" s="4">
-        <v>45516</v>
+        <v>45544</v>
       </c>
       <c r="D28" s="4">
-        <v>45519</v>
+        <v>45575</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>26</v>
+        <v>150</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C29" s="4">
-        <v>45478</v>
+        <v>45516</v>
       </c>
       <c r="D29" s="4">
-        <v>45507</v>
+        <v>45519</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>133</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>149</v>
+        <v>97</v>
       </c>
       <c r="C30" s="4">
-        <v>45568</v>
+        <v>45589</v>
       </c>
       <c r="D30" s="4">
-        <v>45575</v>
+        <v>45603</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
-        <v>10</v>
+        <v>37</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>165</v>
       </c>
       <c r="C31" s="4">
-        <v>45317</v>
+        <v>45597</v>
       </c>
       <c r="D31" s="4">
-        <v>45422</v>
+        <v>45603</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>29</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>63</v>
+        <v>10</v>
       </c>
       <c r="C32" s="4">
-        <v>45488</v>
+        <v>45317</v>
       </c>
       <c r="D32" s="4">
-        <v>45519</v>
+        <v>45422</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>114</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="C33" s="4">
-        <v>45568</v>
+        <v>45488</v>
       </c>
       <c r="D33" s="4">
-        <v>45575</v>
+        <v>45519</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>14</v>
+        <v>166</v>
+      </c>
+      <c r="C34" s="4">
+        <v>45582</v>
       </c>
       <c r="D34" s="4">
-        <v>45422</v>
+        <v>45603</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>123</v>
@@ -1684,351 +1720,398 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="C35" s="4">
-        <v>45568</v>
+        <v>14</v>
       </c>
       <c r="D35" s="4">
-        <v>45575</v>
+        <v>45422</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>71</v>
+        <v>21</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>73</v>
+        <v>143</v>
       </c>
       <c r="C36" s="4">
-        <v>45376</v>
+        <v>45568</v>
       </c>
       <c r="D36" s="4">
-        <v>45533</v>
+        <v>45575</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>135</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="5"/>
+        <v>71</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" s="4">
+        <v>45376</v>
+      </c>
+      <c r="D37" s="4">
+        <v>45533</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>73</v>
+      </c>
       <c r="F37" s="5" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
-        <v>11</v>
+        <v>114</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>41</v>
+        <v>167</v>
       </c>
       <c r="C38" s="4">
-        <v>45457</v>
+        <v>45572</v>
       </c>
       <c r="D38" s="4">
-        <v>45464</v>
+        <v>45603</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>30</v>
+        <v>168</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>155</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
-        <v>66</v>
+        <v>11</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>151</v>
+        <v>41</v>
       </c>
       <c r="C39" s="4">
-        <v>45571</v>
+        <v>45457</v>
       </c>
       <c r="D39" s="4">
-        <v>45575</v>
+        <v>45464</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>67</v>
+        <v>30</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
-        <v>92</v>
+        <v>65</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>93</v>
+        <v>169</v>
       </c>
       <c r="C40" s="4">
-        <v>45548</v>
+        <v>45603</v>
       </c>
       <c r="D40" s="4">
-        <v>45562</v>
+        <v>45603</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>94</v>
+        <v>66</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
-        <v>161</v>
+        <v>88</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="C41" s="4">
-        <v>45518</v>
+        <v>45599</v>
       </c>
       <c r="D41" s="4">
-        <v>45575</v>
+        <v>45603</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>163</v>
+        <v>89</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>164</v>
+        <v>120</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>41</v>
+        <v>154</v>
       </c>
       <c r="C42" s="4">
-        <v>45573</v>
+        <v>45518</v>
       </c>
       <c r="D42" s="4">
         <v>45575</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>27</v>
+        <v>87</v>
       </c>
       <c r="C43" s="4">
-        <v>45442</v>
+        <v>45597</v>
       </c>
       <c r="D43" s="4">
-        <v>45447</v>
+        <v>45603</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>28</v>
+        <v>145</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>28</v>
+        <v>146</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C44" s="4"/>
+        <v>4</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C44" s="4">
+        <v>45442</v>
+      </c>
       <c r="D44" s="4">
-        <v>45519</v>
+        <v>45447</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B45" s="3">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C45" s="4">
-        <v>45540</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="C45" s="4"/>
       <c r="D45" s="4">
-        <v>45575</v>
+        <v>45519</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>159</v>
+        <v>12</v>
+      </c>
+      <c r="B46" s="3">
+        <v>1.1000000000000001</v>
       </c>
       <c r="C46" s="4">
-        <v>45513</v>
+        <v>45540</v>
       </c>
       <c r="D46" s="4">
-        <v>45562</v>
+        <v>45575</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>160</v>
+        <v>31</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>132</v>
+        <v>31</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
-        <v>75</v>
+        <v>179</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>91</v>
+        <v>176</v>
       </c>
       <c r="C47" s="4">
-        <v>45555</v>
+        <v>45598</v>
       </c>
       <c r="D47" s="4">
-        <v>45562</v>
+        <v>45603</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>109</v>
+        <v>178</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
-        <v>165</v>
+        <v>126</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="C48" s="4">
+        <v>45513</v>
+      </c>
+      <c r="D48" s="4">
+        <v>45562</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C49" s="4">
+        <v>45582</v>
+      </c>
+      <c r="D49" s="4">
+        <v>45603</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C50" s="4">
         <v>45530</v>
       </c>
-      <c r="D48" s="4">
+      <c r="D50" s="4">
         <v>45575</v>
       </c>
-      <c r="E48" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>168</v>
+      <c r="E50" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F48">
-    <sortCondition ref="A2:A48"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F50">
+    <sortCondition ref="A2:A50"/>
   </sortState>
-  <conditionalFormatting sqref="A2:XFD124">
+  <conditionalFormatting sqref="A2:XFD126">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>$D2&gt;$O$1</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E26" r:id="rId1" xr:uid="{A5B7ED1F-2322-489C-9115-C445E82B54FB}"/>
-    <hyperlink ref="E17" r:id="rId2" xr:uid="{90F7D550-3232-4E6C-9AB7-856BDF3EA309}"/>
-    <hyperlink ref="E16" r:id="rId3" xr:uid="{E94C9C6D-6FA4-4184-9965-129FE7CC3A62}"/>
-    <hyperlink ref="E14" r:id="rId4" xr:uid="{5D7F93FB-6C49-403A-9AD8-F4281B6B2D94}"/>
-    <hyperlink ref="E10" r:id="rId5" display="https://github.com/cleartonic/arch_ffvcd/releases" xr:uid="{8C8885B9-A3DC-40DD-B18B-F3B348BB2202}"/>
-    <hyperlink ref="E12" r:id="rId6" xr:uid="{EC4A68ED-DCD0-44C0-9669-EAC47138143B}"/>
-    <hyperlink ref="E6" r:id="rId7" xr:uid="{2531395D-2F00-44AD-B326-97CA7E60977D}"/>
-    <hyperlink ref="E5" r:id="rId8" display="https://wiki.ctjot.com/doku.php?id=multiworld" xr:uid="{A1F02D1E-D96D-4326-BAA2-C7F18AF552BF}"/>
-    <hyperlink ref="E34" r:id="rId9" xr:uid="{39C13D86-F950-4EA9-AD8E-0CD6464A6C33}"/>
-    <hyperlink ref="E43" r:id="rId10" xr:uid="{AB23B92F-9660-4602-A770-B4DC053103FF}"/>
-    <hyperlink ref="E31" r:id="rId11" xr:uid="{AE8D7F00-E698-4DC8-8467-18A519416BF0}"/>
-    <hyperlink ref="E38" r:id="rId12" xr:uid="{2C45B0C7-121E-4FEE-90E6-19A508CC0856}"/>
-    <hyperlink ref="E45" r:id="rId13" xr:uid="{73DD7FA1-8A09-481E-9BF0-EDD88E86EAC3}"/>
-    <hyperlink ref="E4" r:id="rId14" xr:uid="{B7739609-1510-4E1E-B8C4-81240570A0B0}"/>
-    <hyperlink ref="E11" r:id="rId15" xr:uid="{9D4D35EE-2216-4D82-ABE0-0760E544D7F3}"/>
+    <hyperlink ref="E27" r:id="rId1" xr:uid="{A5B7ED1F-2322-489C-9115-C445E82B54FB}"/>
+    <hyperlink ref="E18" r:id="rId2" xr:uid="{90F7D550-3232-4E6C-9AB7-856BDF3EA309}"/>
+    <hyperlink ref="E17" r:id="rId3" xr:uid="{E94C9C6D-6FA4-4184-9965-129FE7CC3A62}"/>
+    <hyperlink ref="E15" r:id="rId4" xr:uid="{5D7F93FB-6C49-403A-9AD8-F4281B6B2D94}"/>
+    <hyperlink ref="E11" r:id="rId5" display="https://github.com/cleartonic/arch_ffvcd/releases" xr:uid="{8C8885B9-A3DC-40DD-B18B-F3B348BB2202}"/>
+    <hyperlink ref="E13" r:id="rId6" xr:uid="{EC4A68ED-DCD0-44C0-9669-EAC47138143B}"/>
+    <hyperlink ref="E7" r:id="rId7" xr:uid="{2531395D-2F00-44AD-B326-97CA7E60977D}"/>
+    <hyperlink ref="E6" r:id="rId8" display="https://wiki.ctjot.com/doku.php?id=multiworld" xr:uid="{A1F02D1E-D96D-4326-BAA2-C7F18AF552BF}"/>
+    <hyperlink ref="E35" r:id="rId9" xr:uid="{39C13D86-F950-4EA9-AD8E-0CD6464A6C33}"/>
+    <hyperlink ref="E44" r:id="rId10" xr:uid="{AB23B92F-9660-4602-A770-B4DC053103FF}"/>
+    <hyperlink ref="E32" r:id="rId11" xr:uid="{AE8D7F00-E698-4DC8-8467-18A519416BF0}"/>
+    <hyperlink ref="E39" r:id="rId12" xr:uid="{2C45B0C7-121E-4FEE-90E6-19A508CC0856}"/>
+    <hyperlink ref="E46" r:id="rId13" xr:uid="{73DD7FA1-8A09-481E-9BF0-EDD88E86EAC3}"/>
+    <hyperlink ref="E5" r:id="rId14" xr:uid="{B7739609-1510-4E1E-B8C4-81240570A0B0}"/>
+    <hyperlink ref="E12" r:id="rId15" xr:uid="{9D4D35EE-2216-4D82-ABE0-0760E544D7F3}"/>
     <hyperlink ref="E3" r:id="rId16" xr:uid="{BF5E4EB1-198E-4E95-86E7-1EF1374FF963}"/>
-    <hyperlink ref="E30" r:id="rId17" xr:uid="{15529467-5046-410B-9B6C-654495986B9C}"/>
-    <hyperlink ref="E15" r:id="rId18" xr:uid="{65E5E7CE-44B2-4FB0-BD3D-351DBED5A38A}"/>
-    <hyperlink ref="E13" r:id="rId19" xr:uid="{75A12DC5-3325-4C7B-9F69-1A0B70EF2357}"/>
+    <hyperlink ref="E31" r:id="rId17" xr:uid="{15529467-5046-410B-9B6C-654495986B9C}"/>
+    <hyperlink ref="E16" r:id="rId18" xr:uid="{65E5E7CE-44B2-4FB0-BD3D-351DBED5A38A}"/>
+    <hyperlink ref="E14" r:id="rId19" xr:uid="{75A12DC5-3325-4C7B-9F69-1A0B70EF2357}"/>
     <hyperlink ref="E2" r:id="rId20" xr:uid="{6A5A7183-040B-4C7C-A5E8-B8E3C0F52BCD}"/>
-    <hyperlink ref="E7" r:id="rId21" xr:uid="{C789739C-B0F4-4CB3-956F-269CAF2DFC8D}"/>
-    <hyperlink ref="E40" r:id="rId22" xr:uid="{A8E1490C-983B-4622-8DC5-5563FB81C76C}"/>
-    <hyperlink ref="E48" r:id="rId23" xr:uid="{DB56F6A2-172B-4E4C-8A53-CBAD5AE6BAAB}"/>
+    <hyperlink ref="E8" r:id="rId21" xr:uid="{C789739C-B0F4-4CB3-956F-269CAF2DFC8D}"/>
+    <hyperlink ref="E41" r:id="rId22" xr:uid="{A8E1490C-983B-4622-8DC5-5563FB81C76C}"/>
+    <hyperlink ref="E50" r:id="rId23" xr:uid="{DB56F6A2-172B-4E4C-8A53-CBAD5AE6BAAB}"/>
     <hyperlink ref="F2" r:id="rId24" xr:uid="{20EB67DC-FC82-4F1A-9B75-CBF513D8DE4E}"/>
-    <hyperlink ref="F43" r:id="rId25" xr:uid="{73781179-C544-4054-952B-FA4211662F26}"/>
-    <hyperlink ref="F45" r:id="rId26" xr:uid="{E86B653A-32F2-4FF7-91A8-FCB34C0FF2C2}"/>
-    <hyperlink ref="F8" r:id="rId27" xr:uid="{02494919-717B-478B-B79A-AE4E30A28014}"/>
-    <hyperlink ref="F19" r:id="rId28" xr:uid="{632AD9BE-E9BA-4153-995B-F235523DEE74}"/>
-    <hyperlink ref="F16" r:id="rId29" xr:uid="{B2B308EE-F30D-42F0-A7BD-4544BA18A6D9}"/>
-    <hyperlink ref="F28" r:id="rId30" xr:uid="{7DBCE998-F80D-4D11-B542-1A4709AE8490}"/>
-    <hyperlink ref="F27" r:id="rId31" xr:uid="{5D0C808C-7E89-43C9-A13D-EED2709CC1D7}"/>
-    <hyperlink ref="F32" r:id="rId32" xr:uid="{64C3416A-7C81-40DD-BC58-E6E2E34EA840}"/>
-    <hyperlink ref="F35" r:id="rId33" xr:uid="{BAAE57A6-92DF-4790-90A3-C20208627A9C}"/>
-    <hyperlink ref="F20" r:id="rId34" xr:uid="{C83AE148-8202-4A65-8B93-0A010403C63B}"/>
-    <hyperlink ref="F21" r:id="rId35" xr:uid="{AF726EF3-BA18-451C-8E63-28F5F4EA1FC9}"/>
-    <hyperlink ref="F30" r:id="rId36" xr:uid="{AE1B5F2A-8864-4E2F-976A-CE56ADD6F999}"/>
-    <hyperlink ref="F37" r:id="rId37" xr:uid="{C8E38BF7-6188-48AC-A664-93E9163A8930}"/>
-    <hyperlink ref="F12" r:id="rId38" xr:uid="{994E4A5D-DC36-473B-9922-C223D8B30D3B}"/>
-    <hyperlink ref="F7" r:id="rId39" xr:uid="{D3D17A4B-395F-4F48-A33C-49AC6AA8E1E4}"/>
-    <hyperlink ref="F34" r:id="rId40" xr:uid="{E5B6EC13-EF0E-494F-8472-535EF67D8363}"/>
-    <hyperlink ref="F15" r:id="rId41" xr:uid="{2420FD62-4E63-4C9C-BE75-6AFA574DD4FA}"/>
-    <hyperlink ref="F40" r:id="rId42" xr:uid="{606EF7C0-92E0-4433-9350-F0BD9155211D}"/>
-    <hyperlink ref="F17" r:id="rId43" xr:uid="{E24CEC8F-56F5-44DD-8ED0-C170E20F245E}"/>
-    <hyperlink ref="F10" r:id="rId44" xr:uid="{CC7B146B-DFA0-437C-BD1C-353C0E3A04D8}"/>
-    <hyperlink ref="F33" r:id="rId45" xr:uid="{E1771B7F-29FC-44FD-89DE-44BF99EEAF8F}"/>
+    <hyperlink ref="F44" r:id="rId25" xr:uid="{73781179-C544-4054-952B-FA4211662F26}"/>
+    <hyperlink ref="F46" r:id="rId26" xr:uid="{E86B653A-32F2-4FF7-91A8-FCB34C0FF2C2}"/>
+    <hyperlink ref="F9" r:id="rId27" xr:uid="{02494919-717B-478B-B79A-AE4E30A28014}"/>
+    <hyperlink ref="F20" r:id="rId28" xr:uid="{632AD9BE-E9BA-4153-995B-F235523DEE74}"/>
+    <hyperlink ref="F17" r:id="rId29" xr:uid="{B2B308EE-F30D-42F0-A7BD-4544BA18A6D9}"/>
+    <hyperlink ref="F29" r:id="rId30" xr:uid="{7DBCE998-F80D-4D11-B542-1A4709AE8490}"/>
+    <hyperlink ref="F28" r:id="rId31" xr:uid="{5D0C808C-7E89-43C9-A13D-EED2709CC1D7}"/>
+    <hyperlink ref="F33" r:id="rId32" xr:uid="{64C3416A-7C81-40DD-BC58-E6E2E34EA840}"/>
+    <hyperlink ref="F36" r:id="rId33" xr:uid="{BAAE57A6-92DF-4790-90A3-C20208627A9C}"/>
+    <hyperlink ref="F21" r:id="rId34" xr:uid="{C83AE148-8202-4A65-8B93-0A010403C63B}"/>
+    <hyperlink ref="F22" r:id="rId35" xr:uid="{AF726EF3-BA18-451C-8E63-28F5F4EA1FC9}"/>
+    <hyperlink ref="F31" r:id="rId36" xr:uid="{AE1B5F2A-8864-4E2F-976A-CE56ADD6F999}"/>
+    <hyperlink ref="F38" r:id="rId37" xr:uid="{C8E38BF7-6188-48AC-A664-93E9163A8930}"/>
+    <hyperlink ref="F13" r:id="rId38" xr:uid="{994E4A5D-DC36-473B-9922-C223D8B30D3B}"/>
+    <hyperlink ref="F8" r:id="rId39" xr:uid="{D3D17A4B-395F-4F48-A33C-49AC6AA8E1E4}"/>
+    <hyperlink ref="F35" r:id="rId40" xr:uid="{E5B6EC13-EF0E-494F-8472-535EF67D8363}"/>
+    <hyperlink ref="F16" r:id="rId41" xr:uid="{2420FD62-4E63-4C9C-BE75-6AFA574DD4FA}"/>
+    <hyperlink ref="F41" r:id="rId42" xr:uid="{606EF7C0-92E0-4433-9350-F0BD9155211D}"/>
+    <hyperlink ref="F18" r:id="rId43" xr:uid="{E24CEC8F-56F5-44DD-8ED0-C170E20F245E}"/>
+    <hyperlink ref="F11" r:id="rId44" xr:uid="{CC7B146B-DFA0-437C-BD1C-353C0E3A04D8}"/>
+    <hyperlink ref="F34" r:id="rId45" xr:uid="{E1771B7F-29FC-44FD-89DE-44BF99EEAF8F}"/>
     <hyperlink ref="F3" r:id="rId46" xr:uid="{8894D3F4-C9DD-4F73-B8D1-80EDE63AE046}"/>
-    <hyperlink ref="F11" r:id="rId47" xr:uid="{E6A676E9-77F9-4254-821A-7039857E625D}"/>
-    <hyperlink ref="F25" r:id="rId48" xr:uid="{03AEB7E0-B241-406C-88D9-A0F51076BEFC}"/>
-    <hyperlink ref="F29" r:id="rId49" xr:uid="{56FA5804-441B-4115-81F2-E6F57B48EEB0}"/>
-    <hyperlink ref="F6" r:id="rId50" xr:uid="{CD854081-ECE1-4806-B8AA-BFE6EA05BB4B}"/>
-    <hyperlink ref="F36" r:id="rId51" xr:uid="{330B2B26-05E9-4ABC-ABA3-42999D67AAE8}"/>
-    <hyperlink ref="F4" r:id="rId52" xr:uid="{34A7DD68-4900-4D76-B1DC-EBBDA4A2B1A6}"/>
-    <hyperlink ref="F24" r:id="rId53" xr:uid="{2C0DFA88-75D9-4BB4-A9EE-449C4C108A11}"/>
-    <hyperlink ref="F18" r:id="rId54" xr:uid="{F4FF688C-35E4-4D35-8C51-CD53EB6C2A8E}"/>
-    <hyperlink ref="F39" r:id="rId55" xr:uid="{2CB090FD-FB84-4A03-A89B-50F8A1C9F5BD}"/>
-    <hyperlink ref="F9" r:id="rId56" xr:uid="{B03C78ED-3523-452D-AD83-025C4F648157}"/>
-    <hyperlink ref="F26" r:id="rId57" xr:uid="{AC23ABB6-7E63-45F0-B07E-178795C65651}"/>
-    <hyperlink ref="F22" r:id="rId58" xr:uid="{253A3216-53A1-4AD4-9A4D-31EC0F346F7B}"/>
-    <hyperlink ref="F14" r:id="rId59" xr:uid="{D369BB7D-E54A-46CB-813D-E942B4FDBDA6}"/>
-    <hyperlink ref="F23" r:id="rId60" xr:uid="{682DFEC9-B62F-4777-8B03-2A2F3AD89C26}"/>
-    <hyperlink ref="F13" r:id="rId61" xr:uid="{97B23B61-03A2-46B0-8FDC-EC67D02494CD}"/>
-    <hyperlink ref="F5" r:id="rId62" xr:uid="{026695FB-A1A0-417C-8075-98AC08B3580C}"/>
-    <hyperlink ref="F31" r:id="rId63" xr:uid="{4D7429E8-6222-42F1-BD8D-3975D3CB77C3}"/>
-    <hyperlink ref="F38" r:id="rId64" xr:uid="{DAAEC77E-D512-4617-B851-2AD89315F496}"/>
-    <hyperlink ref="F46" r:id="rId65" xr:uid="{5833C0C8-BE25-404A-BCD5-B1BE6AB6638F}"/>
-    <hyperlink ref="E44" r:id="rId66" xr:uid="{50FEBA24-D2B4-420A-AEA7-6BB2D0719A52}"/>
-    <hyperlink ref="E47" r:id="rId67" xr:uid="{75CB8FCF-26EF-4DD8-990B-CCA5D752B17C}"/>
-    <hyperlink ref="F47" r:id="rId68" xr:uid="{BC69EB40-6E47-436F-9731-11B5C17F8B14}"/>
-    <hyperlink ref="E8" r:id="rId69" xr:uid="{9F40885B-F7A9-4F17-A7CD-DEE821C50339}"/>
+    <hyperlink ref="F12" r:id="rId47" xr:uid="{E6A676E9-77F9-4254-821A-7039857E625D}"/>
+    <hyperlink ref="F26" r:id="rId48" xr:uid="{03AEB7E0-B241-406C-88D9-A0F51076BEFC}"/>
+    <hyperlink ref="F30" r:id="rId49" xr:uid="{56FA5804-441B-4115-81F2-E6F57B48EEB0}"/>
+    <hyperlink ref="F7" r:id="rId50" xr:uid="{CD854081-ECE1-4806-B8AA-BFE6EA05BB4B}"/>
+    <hyperlink ref="F37" r:id="rId51" xr:uid="{330B2B26-05E9-4ABC-ABA3-42999D67AAE8}"/>
+    <hyperlink ref="F5" r:id="rId52" xr:uid="{34A7DD68-4900-4D76-B1DC-EBBDA4A2B1A6}"/>
+    <hyperlink ref="F25" r:id="rId53" xr:uid="{2C0DFA88-75D9-4BB4-A9EE-449C4C108A11}"/>
+    <hyperlink ref="F19" r:id="rId54" xr:uid="{F4FF688C-35E4-4D35-8C51-CD53EB6C2A8E}"/>
+    <hyperlink ref="F40" r:id="rId55" xr:uid="{2CB090FD-FB84-4A03-A89B-50F8A1C9F5BD}"/>
+    <hyperlink ref="F10" r:id="rId56" xr:uid="{B03C78ED-3523-452D-AD83-025C4F648157}"/>
+    <hyperlink ref="F27" r:id="rId57" xr:uid="{AC23ABB6-7E63-45F0-B07E-178795C65651}"/>
+    <hyperlink ref="F23" r:id="rId58" xr:uid="{253A3216-53A1-4AD4-9A4D-31EC0F346F7B}"/>
+    <hyperlink ref="F15" r:id="rId59" xr:uid="{D369BB7D-E54A-46CB-813D-E942B4FDBDA6}"/>
+    <hyperlink ref="F24" r:id="rId60" xr:uid="{682DFEC9-B62F-4777-8B03-2A2F3AD89C26}"/>
+    <hyperlink ref="F14" r:id="rId61" xr:uid="{97B23B61-03A2-46B0-8FDC-EC67D02494CD}"/>
+    <hyperlink ref="F6" r:id="rId62" xr:uid="{026695FB-A1A0-417C-8075-98AC08B3580C}"/>
+    <hyperlink ref="F32" r:id="rId63" xr:uid="{4D7429E8-6222-42F1-BD8D-3975D3CB77C3}"/>
+    <hyperlink ref="F39" r:id="rId64" xr:uid="{DAAEC77E-D512-4617-B851-2AD89315F496}"/>
+    <hyperlink ref="F48" r:id="rId65" xr:uid="{5833C0C8-BE25-404A-BCD5-B1BE6AB6638F}"/>
+    <hyperlink ref="E45" r:id="rId66" xr:uid="{50FEBA24-D2B4-420A-AEA7-6BB2D0719A52}"/>
+    <hyperlink ref="E49" r:id="rId67" xr:uid="{75CB8FCF-26EF-4DD8-990B-CCA5D752B17C}"/>
+    <hyperlink ref="F49" r:id="rId68" xr:uid="{BC69EB40-6E47-436F-9731-11B5C17F8B14}"/>
+    <hyperlink ref="E9" r:id="rId69" xr:uid="{9F40885B-F7A9-4F17-A7CD-DEE821C50339}"/>
+    <hyperlink ref="E38" r:id="rId70" xr:uid="{5223544E-DDEF-48F9-9EB3-3EF1B9FDAB90}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId70"/>
+  <pageSetup orientation="portrait" r:id="rId71"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added missing setup pages
</commit_message>
<xml_diff>
--- a/CustomWorldsInstalled.xlsx
+++ b/CustomWorldsInstalled.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\Git\Archipelago\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\azyle\Documents\_code\_repos\Archipelago\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94696357-5619-4A0C-A8B5-01E1E8676929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E53807-B031-4E6C-8A3E-C5FE5B010EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{3DBB16FA-FE5F-4BB0-89C2-A45EA748065E}"/>
+    <workbookView xWindow="4810" yWindow="0" windowWidth="15490" windowHeight="10100" xr2:uid="{3DBB16FA-FE5F-4BB0-89C2-A45EA748065E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="180">
   <si>
     <t>World</t>
   </si>
@@ -180,9 +180,6 @@
 https://github.com/junglechief87/arch_ffvcd/releases</t>
   </si>
   <si>
-    <t>0.82.5</t>
-  </si>
-  <si>
     <t>Kingdom Hearts: Birth by Sleep</t>
   </si>
   <si>
@@ -532,9 +529,6 @@
     <t>2.4.3</t>
   </si>
   <si>
-    <t>0.2.1</t>
-  </si>
-  <si>
     <t>0.3.6.1</t>
   </si>
   <si>
@@ -559,9 +553,6 @@
     <t>Bingo</t>
   </si>
   <si>
-    <t>0.1.7</t>
-  </si>
-  <si>
     <t>https://github.com/Cynichill/APBingo/releases</t>
   </si>
   <si>
@@ -578,6 +569,15 @@
   </si>
   <si>
     <t>Watery Words</t>
+  </si>
+  <si>
+    <t>0.1.9</t>
+  </si>
+  <si>
+    <t>0.6.3</t>
+  </si>
+  <si>
+    <t>0.2.2</t>
   </si>
 </sst>
 </file>
@@ -1024,30 +1024,30 @@
   <dimension ref="A1:O50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A48" sqref="A48"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="75" customWidth="1"/>
-    <col min="6" max="6" width="67.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="67.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="0" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="7.28515625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="0" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="0.85546875" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="0.88671875" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="9.109375" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="6" customWidth="1"/>
-    <col min="14" max="14" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1061,19 +1061,19 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>82</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>83</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>35</v>
       </c>
       <c r="O1" s="6">
-        <v>45575</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+        <v>45603</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
@@ -1090,12 +1090,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C3" s="4">
         <v>45548</v>
@@ -1104,33 +1104,33 @@
         <v>45562</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C4" s="4">
+        <v>45614</v>
+      </c>
+      <c r="D4" s="4">
+        <v>45617</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="C4" s="4">
-        <v>45602</v>
-      </c>
-      <c r="D4" s="4">
-        <v>45603</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>7</v>
       </c>
@@ -1147,29 +1147,29 @@
         <v>32</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="4">
-        <v>45519</v>
+        <v>45617</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C7" s="4">
         <v>45533</v>
@@ -1181,15 +1181,15 @@
         <v>22</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C8" s="4">
         <v>45600</v>
@@ -1198,15 +1198,15 @@
         <v>45603</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B9" s="3">
         <v>0.3</v>
@@ -1218,41 +1218,41 @@
         <v>45575</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C10" s="4">
+        <v>45615</v>
+      </c>
+      <c r="D10" s="4">
+        <v>45617</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C10" s="4">
-        <v>45589</v>
-      </c>
-      <c r="D10" s="4">
-        <v>45603</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>81</v>
-      </c>
       <c r="F10" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>47</v>
+        <v>99</v>
+      </c>
+      <c r="B11" s="3">
+        <v>82.5</v>
       </c>
       <c r="C11" s="4">
-        <v>45493</v>
+        <v>45495</v>
       </c>
       <c r="D11" s="4">
         <v>45507</v>
@@ -1261,12 +1261,12 @@
         <v>46</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C12" s="4">
         <v>45526</v>
@@ -1281,12 +1281,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C13" s="4">
         <v>45557</v>
@@ -1298,10 +1298,10 @@
         <v>23</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>43</v>
       </c>
@@ -1318,15 +1318,15 @@
         <v>45</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C15" s="4">
         <v>45542</v>
@@ -1338,15 +1338,15 @@
         <v>19</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>40</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C16" s="4">
         <v>45597</v>
@@ -1358,15 +1358,15 @@
         <v>39</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C17" s="4">
         <v>45589</v>
@@ -1378,15 +1378,15 @@
         <v>25</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C18" s="4">
         <v>45516</v>
@@ -1398,15 +1398,15 @@
         <v>24</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C19" s="4">
         <v>45555</v>
@@ -1415,15 +1415,15 @@
         <v>45562</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>41</v>
@@ -1435,18 +1435,18 @@
         <v>45547</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C21" s="4">
         <v>45414</v>
@@ -1455,18 +1455,18 @@
         <v>45562</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="C22" s="4">
         <v>45528</v>
@@ -1475,18 +1475,18 @@
         <v>45562</v>
       </c>
       <c r="E22" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="F22" s="5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
-        <v>95</v>
-      </c>
       <c r="B23" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C23" s="4">
         <v>45555</v>
@@ -1495,18 +1495,18 @@
         <v>45562</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C24" s="4">
         <v>45527</v>
@@ -1515,35 +1515,35 @@
         <v>45562</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>164</v>
+        <v>179</v>
       </c>
       <c r="C25" s="4">
-        <v>45602</v>
+        <v>45616</v>
       </c>
       <c r="D25" s="4">
-        <v>45603</v>
+        <v>45617</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>36</v>
@@ -1555,13 +1555,13 @@
         <v>45603</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>8</v>
       </c>
@@ -1578,15 +1578,15 @@
         <v>20</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C28" s="4">
         <v>45544</v>
@@ -1595,18 +1595,18 @@
         <v>45575</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C29" s="4">
         <v>45516</v>
@@ -1618,15 +1618,15 @@
         <v>26</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C30" s="4">
         <v>45589</v>
@@ -1635,18 +1635,18 @@
         <v>45603</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
         <v>37</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C31" s="4">
         <v>45597</v>
@@ -1658,10 +1658,10 @@
         <v>38</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
         <v>10</v>
       </c>
@@ -1678,12 +1678,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C33" s="4">
         <v>45488</v>
@@ -1692,18 +1692,18 @@
         <v>45519</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C34" s="4">
         <v>45582</v>
@@ -1712,13 +1712,13 @@
         <v>45603</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="9" t="s">
         <v>9</v>
       </c>
@@ -1732,15 +1732,15 @@
         <v>21</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C36" s="4">
         <v>45568</v>
@@ -1749,18 +1749,18 @@
         <v>45575</v>
       </c>
       <c r="E36" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="F36" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="9" t="s">
+      <c r="B37" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="C37" s="4">
         <v>45376</v>
@@ -1769,18 +1769,18 @@
         <v>45533</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C38" s="4">
         <v>45572</v>
@@ -1789,13 +1789,13 @@
         <v>45603</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
         <v>11</v>
       </c>
@@ -1812,15 +1812,15 @@
         <v>30</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C40" s="4">
         <v>45603</v>
@@ -1829,18 +1829,18 @@
         <v>45603</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C41" s="4">
         <v>45599</v>
@@ -1849,18 +1849,18 @@
         <v>45603</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>153</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>154</v>
       </c>
       <c r="C42" s="4">
         <v>45518</v>
@@ -1869,18 +1869,18 @@
         <v>45575</v>
       </c>
       <c r="E42" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="F42" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="F42" s="5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C43" s="4">
         <v>45597</v>
@@ -1889,13 +1889,13 @@
         <v>45603</v>
       </c>
       <c r="E43" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F43" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="F43" s="5" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
         <v>4</v>
       </c>
@@ -1915,22 +1915,22 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C45" s="4"/>
       <c r="D45" s="4">
         <v>45519</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="s">
         <v>12</v>
       </c>
@@ -1950,12 +1950,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C47" s="4">
         <v>45598</v>
@@ -1964,18 +1964,18 @@
         <v>45603</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C48" s="4">
         <v>45513</v>
@@ -1984,18 +1984,18 @@
         <v>45562</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C49" s="4">
         <v>45582</v>
@@ -2004,18 +2004,18 @@
         <v>45603</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>157</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>158</v>
       </c>
       <c r="C50" s="4">
         <v>45530</v>
@@ -2024,10 +2024,10 @@
         <v>45575</v>
       </c>
       <c r="E50" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="F50" s="5" t="s">
         <v>159</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -2110,8 +2110,10 @@
     <hyperlink ref="F49" r:id="rId68" xr:uid="{BC69EB40-6E47-436F-9731-11B5C17F8B14}"/>
     <hyperlink ref="E9" r:id="rId69" xr:uid="{9F40885B-F7A9-4F17-A7CD-DEE821C50339}"/>
     <hyperlink ref="E38" r:id="rId70" xr:uid="{5223544E-DDEF-48F9-9EB3-3EF1B9FDAB90}"/>
+    <hyperlink ref="E4" r:id="rId71" xr:uid="{F7C2BC13-BAF9-4996-AE90-F94B1E8EA045}"/>
+    <hyperlink ref="F4" r:id="rId72" xr:uid="{C942D955-FF96-47FC-9CE5-48E87F200A13}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId71"/>
+  <pageSetup orientation="portrait" r:id="rId73"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated custom worlds worksheet
</commit_message>
<xml_diff>
--- a/CustomWorldsInstalled.xlsx
+++ b/CustomWorldsInstalled.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\azyle\Documents\_code\_repos\Archipelago\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\Git\Archipelago\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E53807-B031-4E6C-8A3E-C5FE5B010EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C904BA4A-932E-4AB8-BA7E-A12B661B2DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4810" yWindow="0" windowWidth="15490" windowHeight="10100" xr2:uid="{3DBB16FA-FE5F-4BB0-89C2-A45EA748065E}"/>
+    <workbookView xWindow="19560" yWindow="0" windowWidth="18840" windowHeight="21000" xr2:uid="{3DBB16FA-FE5F-4BB0-89C2-A45EA748065E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="181">
   <si>
     <t>World</t>
   </si>
@@ -529,9 +529,6 @@
     <t>2.4.3</t>
   </si>
   <si>
-    <t>0.3.6.1</t>
-  </si>
-  <si>
     <t>0.7.3</t>
   </si>
   <si>
@@ -559,9 +556,6 @@
     <t>https://discord.com/channels/731205301247803413/1252051532971638784</t>
   </si>
   <si>
-    <t>0.0.1</t>
-  </si>
-  <si>
     <t>https://github.com/spineraks-org/ArchipelagoWateryWords/releases</t>
   </si>
   <si>
@@ -578,6 +572,15 @@
   </si>
   <si>
     <t>0.2.2</t>
+  </si>
+  <si>
+    <t>0.3.8</t>
+  </si>
+  <si>
+    <t>0.0.7</t>
+  </si>
+  <si>
+    <t>1.1.2</t>
   </si>
 </sst>
 </file>
@@ -1024,30 +1027,30 @@
   <dimension ref="A1:O50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="75" customWidth="1"/>
-    <col min="6" max="6" width="67.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="67.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="0" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="7.33203125" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="9.109375" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="0" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="0.88671875" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="9.109375" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="0.85546875" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="6" customWidth="1"/>
-    <col min="14" max="14" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1073,7 +1076,7 @@
         <v>45603</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
@@ -1090,7 +1093,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>56</v>
       </c>
@@ -1110,12 +1113,12 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C4" s="4">
         <v>45614</v>
@@ -1124,13 +1127,13 @@
         <v>45617</v>
       </c>
       <c r="E4" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>7</v>
       </c>
@@ -1150,7 +1153,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>16</v>
       </c>
@@ -1164,7 +1167,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>15</v>
       </c>
@@ -1184,7 +1187,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>55</v>
       </c>
@@ -1204,7 +1207,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>98</v>
       </c>
@@ -1224,12 +1227,12 @@
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>79</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C10" s="4">
         <v>45615</v>
@@ -1244,7 +1247,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>99</v>
       </c>
@@ -1264,7 +1267,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>100</v>
       </c>
@@ -1281,7 +1284,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>97</v>
       </c>
@@ -1301,7 +1304,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>43</v>
       </c>
@@ -1321,7 +1324,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>13</v>
       </c>
@@ -1341,7 +1344,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>40</v>
       </c>
@@ -1361,7 +1364,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>18</v>
       </c>
@@ -1381,7 +1384,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>17</v>
       </c>
@@ -1401,7 +1404,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>47</v>
       </c>
@@ -1421,7 +1424,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>83</v>
       </c>
@@ -1441,7 +1444,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>90</v>
       </c>
@@ -1461,7 +1464,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>91</v>
       </c>
@@ -1481,7 +1484,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>94</v>
       </c>
@@ -1501,7 +1504,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>95</v>
       </c>
@@ -1521,12 +1524,12 @@
         <v>138</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>78</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C25" s="4">
         <v>45616</v>
@@ -1541,7 +1544,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>75</v>
       </c>
@@ -1561,7 +1564,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>8</v>
       </c>
@@ -1581,7 +1584,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>106</v>
       </c>
@@ -1601,7 +1604,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>6</v>
       </c>
@@ -1621,7 +1624,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>49</v>
       </c>
@@ -1641,12 +1644,12 @@
         <v>127</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>37</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>163</v>
+        <v>178</v>
       </c>
       <c r="C31" s="4">
         <v>45597</v>
@@ -1661,7 +1664,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>10</v>
       </c>
@@ -1678,7 +1681,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>59</v>
       </c>
@@ -1698,12 +1701,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>62</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C34" s="4">
         <v>45582</v>
@@ -1718,7 +1721,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>9</v>
       </c>
@@ -1735,7 +1738,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>68</v>
       </c>
@@ -1755,7 +1758,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>70</v>
       </c>
@@ -1775,27 +1778,27 @@
         <v>129</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>113</v>
       </c>
       <c r="B38" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C38" s="4">
+        <v>45611</v>
+      </c>
+      <c r="D38" s="4">
+        <v>45617</v>
+      </c>
+      <c r="E38" s="5" t="s">
         <v>165</v>
-      </c>
-      <c r="C38" s="4">
-        <v>45572</v>
-      </c>
-      <c r="D38" s="4">
-        <v>45603</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>166</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>11</v>
       </c>
@@ -1815,12 +1818,12 @@
         <v>146</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>64</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C40" s="4">
         <v>45603</v>
@@ -1835,12 +1838,12 @@
         <v>133</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>87</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C41" s="4">
         <v>45599</v>
@@ -1855,7 +1858,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>152</v>
       </c>
@@ -1875,7 +1878,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>143</v>
       </c>
@@ -1895,7 +1898,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>4</v>
       </c>
@@ -1915,7 +1918,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>53</v>
       </c>
@@ -1930,18 +1933,18 @@
         <v>54</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B46" s="3">
-        <v>1.1000000000000001</v>
+      <c r="B46" s="3" t="s">
+        <v>180</v>
       </c>
       <c r="C46" s="4">
-        <v>45540</v>
+        <v>45579</v>
       </c>
       <c r="D46" s="4">
-        <v>45575</v>
+        <v>45617</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>31</v>
@@ -1950,27 +1953,27 @@
         <v>31</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B47" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C47" s="4">
+        <v>45611</v>
+      </c>
+      <c r="D47" s="4">
+        <v>45617</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="F47" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="C47" s="4">
-        <v>45598</v>
-      </c>
-      <c r="D47" s="4">
-        <v>45603</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>125</v>
       </c>
@@ -1990,12 +1993,12 @@
         <v>126</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>73</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C49" s="4">
         <v>45582</v>
@@ -2010,7 +2013,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
         <v>156</v>
       </c>
@@ -2112,8 +2115,11 @@
     <hyperlink ref="E38" r:id="rId70" xr:uid="{5223544E-DDEF-48F9-9EB3-3EF1B9FDAB90}"/>
     <hyperlink ref="E4" r:id="rId71" xr:uid="{F7C2BC13-BAF9-4996-AE90-F94B1E8EA045}"/>
     <hyperlink ref="F4" r:id="rId72" xr:uid="{C942D955-FF96-47FC-9CE5-48E87F200A13}"/>
+    <hyperlink ref="E30" r:id="rId73" xr:uid="{9AA38BAF-4725-4754-B7EA-23E92B659CE2}"/>
+    <hyperlink ref="E34" r:id="rId74" xr:uid="{C838F4BD-E551-442C-B150-986D44024BB8}"/>
+    <hyperlink ref="F50" r:id="rId75" xr:uid="{75BD971A-96A3-46CE-985A-1488D76AC8A9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId73"/>
+  <pageSetup orientation="portrait" r:id="rId76"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated worlds to latest versions. Added new worlds. Updated Multiserver with additional events to be sent to dynx. Fully fleshed out the room hint feature.
</commit_message>
<xml_diff>
--- a/CustomWorldsInstalled.xlsx
+++ b/CustomWorldsInstalled.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\Git\Archipelago\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6846AF3F-8B9E-4DA4-BBA5-DCBB7A8E26BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3BC15D-F73A-4469-9F34-03C826BB2AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{3DBB16FA-FE5F-4BB0-89C2-A45EA748065E}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{3DBB16FA-FE5F-4BB0-89C2-A45EA748065E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="201">
   <si>
     <t>World</t>
   </si>
@@ -457,9 +457,6 @@
     <t>https://github.com/SenPierre/ArchipelagoOoA/releases</t>
   </si>
   <si>
-    <t>2.5.2</t>
-  </si>
-  <si>
     <t>https://github.com/tanjo3/tww_apworld/releases</t>
   </si>
   <si>
@@ -520,39 +517,15 @@
     <t>0.6.3</t>
   </si>
   <si>
-    <t>0.2.2</t>
-  </si>
-  <si>
     <t>1.1.2</t>
   </si>
   <si>
-    <t>2.4.1</t>
-  </si>
-  <si>
     <t>0.4.1</t>
   </si>
   <si>
     <t>0.6.6</t>
   </si>
   <si>
-    <t>0.3.9</t>
-  </si>
-  <si>
-    <t>0.0.8</t>
-  </si>
-  <si>
-    <t>0.9.0</t>
-  </si>
-  <si>
-    <t>0.5.0</t>
-  </si>
-  <si>
-    <t>1.2.3.1</t>
-  </si>
-  <si>
-    <t>0.5.10</t>
-  </si>
-  <si>
     <t>Link's Awakening - Beta</t>
   </si>
   <si>
@@ -568,13 +541,107 @@
     <t>Autopelago</t>
   </si>
   <si>
-    <t>0.6.0</t>
-  </si>
-  <si>
     <t>https://github.com/airbreather/Autopelago/releases</t>
   </si>
   <si>
     <t>https://discord.com/channels/731205301247803413/1307517897194868768</t>
+  </si>
+  <si>
+    <t>0.5.2</t>
+  </si>
+  <si>
+    <t>0.6.4</t>
+  </si>
+  <si>
+    <t>0.2.3</t>
+  </si>
+  <si>
+    <t>1.2.4</t>
+  </si>
+  <si>
+    <t>0.3.11</t>
+  </si>
+  <si>
+    <t>0.0.9</t>
+  </si>
+  <si>
+    <t>0.4.0</t>
+  </si>
+  <si>
+    <t>0.5.13</t>
+  </si>
+  <si>
+    <t>2.6.1</t>
+  </si>
+  <si>
+    <t>https://github.com/jjjj12212/Archipelago-BanjoTooie/releases</t>
+  </si>
+  <si>
+    <t>https://discord.com/channels/731205301247803413/1135352499172286505</t>
+  </si>
+  <si>
+    <t>Minishoot</t>
+  </si>
+  <si>
+    <t>https://github.com/TheNooodle/MinishootRandomizer/releases</t>
+  </si>
+  <si>
+    <t>https://discord.com/channels/731205301247803413/1307687662798508113</t>
+  </si>
+  <si>
+    <t>Banjo-Tooie</t>
+  </si>
+  <si>
+    <t>Hades</t>
+  </si>
+  <si>
+    <t>0.13.0</t>
+  </si>
+  <si>
+    <t>https://github.com/NaixGames/Polycosmos/releases</t>
+  </si>
+  <si>
+    <t>https://discord.com/channels/731205301247803413/1142985359563685898</t>
+  </si>
+  <si>
+    <t>Balatro</t>
+  </si>
+  <si>
+    <t>https://github.com/BurndiL/BalatroAP/releases</t>
+  </si>
+  <si>
+    <t>https://discord.com/channels/1085716850370957462/1217203888717828307</t>
+  </si>
+  <si>
+    <t>Metroid Prime</t>
+  </si>
+  <si>
+    <t>0.4.8</t>
+  </si>
+  <si>
+    <t>https://github.com/Electro1512/MetroidAPrime/releases</t>
+  </si>
+  <si>
+    <t>https://discord.com/channels/731205301247803413/1172631093837570068</t>
+  </si>
+  <si>
+    <t>Ratchet and Clank 2</t>
+  </si>
+  <si>
+    <t>https://github.com/evilwb/APRac2/releases</t>
+  </si>
+  <si>
+    <t>https://discord.com/channels/731205301247803413/1325015730218860554</t>
+  </si>
+  <si>
+    <t>Enter the Gungeon</t>
+  </si>
+  <si>
+    <t>https://discord.com/channels/731205301247803413/1191767250257055785</t>
+  </si>
+  <si>
+    <t>https://github.com/KinTheInfinite/Archipelago/releases
+https://thunderstore.io/c/enter-the-gungeon/p/GungeonArchipelago/Gungeon_Archipelago/</t>
   </si>
 </sst>
 </file>
@@ -651,7 +718,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -674,6 +741,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1018,17 +1088,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{901AF876-1585-4DEB-9BCA-32AAC89A46F9}">
-  <dimension ref="A1:O49"/>
+  <dimension ref="A1:O56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="75" customWidth="1"/>
@@ -1067,7 +1137,7 @@
         <v>33</v>
       </c>
       <c r="O1" s="6">
-        <v>45632</v>
+        <v>45645</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -1092,13 +1162,13 @@
         <v>53</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C3" s="4">
-        <v>45643</v>
+        <v>45646</v>
       </c>
       <c r="D3" s="4">
-        <v>45645</v>
+        <v>45675</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>55</v>
@@ -1109,381 +1179,374 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>176</v>
+        <v>148</v>
       </c>
       <c r="C4" s="4">
-        <v>45645</v>
+        <v>45668</v>
       </c>
       <c r="D4" s="4">
-        <v>45645</v>
+        <v>45675</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>152</v>
+        <v>188</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C5" s="4">
-        <v>45614</v>
+        <v>45578</v>
       </c>
       <c r="D5" s="4">
-        <v>45617</v>
+        <v>45675</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>153</v>
+        <v>189</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>154</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>34</v>
+        <v>183</v>
+      </c>
+      <c r="B6" s="3">
+        <v>4.0999999999999996</v>
       </c>
       <c r="C6" s="4">
-        <v>45308</v>
+        <v>45668</v>
       </c>
       <c r="D6" s="4">
-        <v>45410</v>
+        <v>45675</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>30</v>
+        <v>178</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>16</v>
+        <v>151</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C7" s="4">
+        <v>45614</v>
       </c>
       <c r="D7" s="4">
         <v>45617</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>130</v>
+      <c r="E7" s="5" t="s">
+        <v>152</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>129</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>159</v>
+        <v>34</v>
       </c>
       <c r="C8" s="4">
-        <v>45641</v>
+        <v>45308</v>
       </c>
       <c r="D8" s="4">
-        <v>45645</v>
+        <v>45410</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C9" s="4">
-        <v>45630</v>
+        <v>16</v>
       </c>
       <c r="D9" s="4">
-        <v>45632</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>63</v>
+        <v>45617</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>130</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="B10" s="3">
-        <v>0.4</v>
+        <v>15</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>170</v>
       </c>
       <c r="C10" s="4">
-        <v>45640</v>
+        <v>45670</v>
       </c>
       <c r="D10" s="4">
-        <v>45645</v>
+        <v>45675</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>136</v>
+        <v>21</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>159</v>
+        <v>52</v>
+      </c>
+      <c r="B11" s="3">
+        <v>3</v>
       </c>
       <c r="C11" s="4">
-        <v>45615</v>
+        <v>45668</v>
       </c>
       <c r="D11" s="4">
-        <v>45617</v>
+        <v>45675</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="B12" s="3">
-        <v>82.5</v>
-      </c>
-      <c r="C12" s="4">
-        <v>45495</v>
-      </c>
-      <c r="D12" s="4">
-        <v>45507</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
       <c r="E12" s="7" t="s">
-        <v>43</v>
+        <v>200</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>110</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0.4</v>
       </c>
       <c r="C13" s="4">
-        <v>45526</v>
+        <v>45641</v>
       </c>
       <c r="D13" s="4">
-        <v>45562</v>
+        <v>45645</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>31</v>
+        <v>136</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>31</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>79</v>
+        <v>158</v>
       </c>
       <c r="C14" s="4">
-        <v>45557</v>
+        <v>45615</v>
       </c>
       <c r="D14" s="4">
-        <v>45562</v>
+        <v>45617</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>41</v>
+        <v>91</v>
+      </c>
+      <c r="B15" s="3">
+        <v>82.5</v>
       </c>
       <c r="C15" s="4">
-        <v>45425</v>
+        <v>45495</v>
       </c>
       <c r="D15" s="4">
-        <v>45478</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>42</v>
+        <v>45507</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="C16" s="4">
-        <v>45542</v>
+        <v>45526</v>
       </c>
       <c r="D16" s="4">
-        <v>45547</v>
+        <v>45562</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>126</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>38</v>
+        <v>89</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>163</v>
+        <v>79</v>
       </c>
       <c r="C17" s="4">
-        <v>45618</v>
+        <v>45557</v>
       </c>
       <c r="D17" s="4">
-        <v>45632</v>
+        <v>45562</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C18" s="4">
-        <v>45516</v>
+        <v>45425</v>
       </c>
       <c r="D18" s="4">
-        <v>45519</v>
+        <v>45478</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>109</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>80</v>
+        <v>184</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>185</v>
       </c>
       <c r="C19" s="4">
-        <v>45555</v>
+        <v>45646</v>
       </c>
       <c r="D19" s="4">
-        <v>45562</v>
+        <v>45675</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>45</v>
+        <v>186</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>121</v>
+        <v>187</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>77</v>
+        <v>13</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="C20" s="4">
-        <v>45527</v>
+        <v>45542</v>
       </c>
       <c r="D20" s="4">
         <v>45547</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>78</v>
+        <v>18</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>94</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>171</v>
+        <v>38</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="C21" s="4">
-        <v>45640</v>
+        <v>45618</v>
       </c>
       <c r="D21" s="4">
-        <v>45645</v>
+        <v>45632</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>173</v>
+        <v>37</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>174</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>83</v>
+        <v>17</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="C22" s="4">
-        <v>45528</v>
+        <v>45516</v>
       </c>
       <c r="D22" s="4">
-        <v>45562</v>
+        <v>45519</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>85</v>
+        <v>23</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>86</v>
+        <v>44</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C23" s="4">
         <v>45555</v>
@@ -1492,607 +1555,749 @@
         <v>45562</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>84</v>
+        <v>39</v>
       </c>
       <c r="C24" s="4">
         <v>45527</v>
       </c>
       <c r="D24" s="4">
-        <v>45562</v>
+        <v>45547</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>127</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>160</v>
+        <v>162</v>
+      </c>
+      <c r="B25" s="3">
+        <v>11</v>
       </c>
       <c r="C25" s="4">
-        <v>45616</v>
+        <v>45675</v>
       </c>
       <c r="D25" s="4">
-        <v>45617</v>
+        <v>45675</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>71</v>
+        <v>164</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>120</v>
+        <v>165</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>54</v>
+        <v>84</v>
       </c>
       <c r="C26" s="4">
-        <v>45631</v>
+        <v>45528</v>
       </c>
       <c r="D26" s="4">
-        <v>45632</v>
+        <v>45562</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>164</v>
+        <v>88</v>
       </c>
       <c r="C27" s="4">
-        <v>45626</v>
+        <v>45555</v>
       </c>
       <c r="D27" s="4">
-        <v>45632</v>
+        <v>45562</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>19</v>
+        <v>85</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>137</v>
+        <v>84</v>
       </c>
       <c r="C28" s="4">
-        <v>45544</v>
+        <v>45527</v>
       </c>
       <c r="D28" s="4">
-        <v>45575</v>
+        <v>45562</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>138</v>
+        <v>85</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>97</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>6</v>
+        <v>191</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>49</v>
+        <v>192</v>
       </c>
       <c r="C29" s="4">
-        <v>45516</v>
+        <v>45623</v>
       </c>
       <c r="D29" s="4">
-        <v>45519</v>
+        <v>45675</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>24</v>
+        <v>193</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>95</v>
+        <v>194</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C30" s="4">
-        <v>45638</v>
+        <v>45674</v>
       </c>
       <c r="D30" s="4">
-        <v>45645</v>
+        <v>45675</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>165</v>
+        <v>54</v>
       </c>
       <c r="C31" s="4">
-        <v>45632</v>
+        <v>45631</v>
       </c>
       <c r="D31" s="4">
         <v>45632</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>161</v>
       </c>
       <c r="C32" s="4">
-        <v>45317</v>
+        <v>45626</v>
       </c>
       <c r="D32" s="4">
-        <v>45422</v>
+        <v>45632</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>27</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>56</v>
+        <v>180</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="C33" s="4">
-        <v>45488</v>
+        <v>45671</v>
       </c>
       <c r="D33" s="4">
-        <v>45519</v>
+        <v>45675</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>57</v>
+        <v>181</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>98</v>
+        <v>182</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>59</v>
+        <v>96</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="C34" s="4">
-        <v>45582</v>
+        <v>45544</v>
       </c>
       <c r="D34" s="4">
-        <v>45603</v>
+        <v>45575</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>60</v>
+        <v>138</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>14</v>
+        <v>49</v>
+      </c>
+      <c r="C35" s="4">
+        <v>45516</v>
       </c>
       <c r="D35" s="4">
-        <v>45422</v>
+        <v>45519</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>131</v>
+        <v>172</v>
       </c>
       <c r="C36" s="4">
-        <v>45568</v>
+        <v>45646</v>
       </c>
       <c r="D36" s="4">
-        <v>45575</v>
+        <v>45675</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>67</v>
+        <v>173</v>
       </c>
       <c r="C37" s="4">
-        <v>45376</v>
+        <v>45646</v>
       </c>
       <c r="D37" s="4">
-        <v>45533</v>
+        <v>45675</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>166</v>
+        <v>10</v>
       </c>
       <c r="C38" s="4">
-        <v>45629</v>
+        <v>45317</v>
       </c>
       <c r="D38" s="4">
-        <v>45632</v>
+        <v>45422</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>151</v>
+        <v>27</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>103</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="C39" s="4">
-        <v>45645</v>
+        <v>45488</v>
       </c>
       <c r="D39" s="4">
-        <v>45645</v>
+        <v>45519</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>135</v>
+        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
       <c r="C40" s="4">
-        <v>45640</v>
+        <v>45582</v>
       </c>
       <c r="D40" s="4">
-        <v>45645</v>
+        <v>45603</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
-        <v>81</v>
+        <v>9</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C41" s="4">
-        <v>45626</v>
+        <v>14</v>
       </c>
       <c r="D41" s="4">
-        <v>45632</v>
+        <v>45422</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>82</v>
+        <v>20</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
-        <v>141</v>
+        <v>195</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>142</v>
+        <v>175</v>
       </c>
       <c r="C42" s="4">
-        <v>45518</v>
+        <v>45674</v>
       </c>
       <c r="D42" s="4">
-        <v>45575</v>
+        <v>45675</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>143</v>
+        <v>196</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>144</v>
+        <v>197</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
-        <v>132</v>
+        <v>64</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>80</v>
+        <v>131</v>
       </c>
       <c r="C43" s="4">
-        <v>45597</v>
+        <v>45568</v>
       </c>
       <c r="D43" s="4">
-        <v>45603</v>
+        <v>45575</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>133</v>
+        <v>65</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>134</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
-        <v>4</v>
+        <v>66</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="C44" s="4">
-        <v>45442</v>
+        <v>45376</v>
       </c>
       <c r="D44" s="4">
-        <v>45447</v>
+        <v>45533</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>26</v>
+        <v>118</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C45" s="4"/>
+        <v>102</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C45" s="4">
+        <v>45638</v>
+      </c>
       <c r="D45" s="4">
-        <v>45519</v>
+        <v>45675</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>51</v>
+        <v>150</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>51</v>
+        <v>103</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="C46" s="4">
-        <v>45579</v>
+        <v>45646</v>
       </c>
       <c r="D46" s="4">
-        <v>45617</v>
+        <v>45675</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>29</v>
+        <v>135</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
-        <v>157</v>
+        <v>61</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>150</v>
+        <v>176</v>
       </c>
       <c r="C47" s="4">
-        <v>45611</v>
+        <v>45661</v>
       </c>
       <c r="D47" s="4">
-        <v>45617</v>
+        <v>45675</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>155</v>
+        <v>62</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>156</v>
+        <v>122</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
-        <v>114</v>
+        <v>81</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>139</v>
+        <v>163</v>
       </c>
       <c r="C48" s="4">
-        <v>45513</v>
+        <v>45674</v>
       </c>
       <c r="D48" s="4">
-        <v>45562</v>
+        <v>45675</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>140</v>
+        <v>82</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C49" s="4">
-        <v>45530</v>
+        <v>45518</v>
       </c>
       <c r="D49" s="4">
         <v>45575</v>
       </c>
       <c r="E49" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C50" s="4">
+        <v>45597</v>
+      </c>
+      <c r="D50" s="4">
+        <v>45603</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C51" s="4">
+        <v>45442</v>
+      </c>
+      <c r="D51" s="4">
+        <v>45447</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4">
+        <v>45519</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C53" s="4">
+        <v>45579</v>
+      </c>
+      <c r="D53" s="4">
+        <v>45617</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C54" s="4">
+        <v>45611</v>
+      </c>
+      <c r="D54" s="4">
+        <v>45617</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C55" s="4">
+        <v>45661</v>
+      </c>
+      <c r="D55" s="4">
+        <v>45675</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C56" s="4">
+        <v>45530</v>
+      </c>
+      <c r="D56" s="4">
+        <v>45575</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="F56" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="F49" s="5" t="s">
-        <v>148</v>
-      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F49">
-    <sortCondition ref="A2:A49"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F56">
+    <sortCondition ref="A2:A56"/>
   </sortState>
-  <conditionalFormatting sqref="A2:XFD125">
+  <conditionalFormatting sqref="A2:XFD132">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>$D2&gt;$O$1</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E27" r:id="rId1" xr:uid="{A5B7ED1F-2322-489C-9115-C445E82B54FB}"/>
-    <hyperlink ref="E18" r:id="rId2" xr:uid="{90F7D550-3232-4E6C-9AB7-856BDF3EA309}"/>
-    <hyperlink ref="E16" r:id="rId3" xr:uid="{5D7F93FB-6C49-403A-9AD8-F4281B6B2D94}"/>
-    <hyperlink ref="E12" r:id="rId4" display="https://github.com/cleartonic/arch_ffvcd/releases" xr:uid="{8C8885B9-A3DC-40DD-B18B-F3B348BB2202}"/>
-    <hyperlink ref="E14" r:id="rId5" xr:uid="{EC4A68ED-DCD0-44C0-9669-EAC47138143B}"/>
-    <hyperlink ref="E8" r:id="rId6" xr:uid="{2531395D-2F00-44AD-B326-97CA7E60977D}"/>
-    <hyperlink ref="E7" r:id="rId7" display="https://wiki.ctjot.com/doku.php?id=multiworld" xr:uid="{A1F02D1E-D96D-4326-BAA2-C7F18AF552BF}"/>
-    <hyperlink ref="E35" r:id="rId8" xr:uid="{39C13D86-F950-4EA9-AD8E-0CD6464A6C33}"/>
-    <hyperlink ref="E44" r:id="rId9" xr:uid="{AB23B92F-9660-4602-A770-B4DC053103FF}"/>
-    <hyperlink ref="E32" r:id="rId10" xr:uid="{AE8D7F00-E698-4DC8-8467-18A519416BF0}"/>
-    <hyperlink ref="E39" r:id="rId11" xr:uid="{2C45B0C7-121E-4FEE-90E6-19A508CC0856}"/>
-    <hyperlink ref="E46" r:id="rId12" xr:uid="{73DD7FA1-8A09-481E-9BF0-EDD88E86EAC3}"/>
-    <hyperlink ref="E6" r:id="rId13" xr:uid="{B7739609-1510-4E1E-B8C4-81240570A0B0}"/>
-    <hyperlink ref="E13" r:id="rId14" xr:uid="{9D4D35EE-2216-4D82-ABE0-0760E544D7F3}"/>
+    <hyperlink ref="E32" r:id="rId1" xr:uid="{A5B7ED1F-2322-489C-9115-C445E82B54FB}"/>
+    <hyperlink ref="E22" r:id="rId2" xr:uid="{90F7D550-3232-4E6C-9AB7-856BDF3EA309}"/>
+    <hyperlink ref="E20" r:id="rId3" xr:uid="{5D7F93FB-6C49-403A-9AD8-F4281B6B2D94}"/>
+    <hyperlink ref="E15" r:id="rId4" display="https://github.com/cleartonic/arch_ffvcd/releases" xr:uid="{8C8885B9-A3DC-40DD-B18B-F3B348BB2202}"/>
+    <hyperlink ref="E17" r:id="rId5" xr:uid="{EC4A68ED-DCD0-44C0-9669-EAC47138143B}"/>
+    <hyperlink ref="E10" r:id="rId6" xr:uid="{2531395D-2F00-44AD-B326-97CA7E60977D}"/>
+    <hyperlink ref="E9" r:id="rId7" display="https://wiki.ctjot.com/doku.php?id=multiworld" xr:uid="{A1F02D1E-D96D-4326-BAA2-C7F18AF552BF}"/>
+    <hyperlink ref="E41" r:id="rId8" xr:uid="{39C13D86-F950-4EA9-AD8E-0CD6464A6C33}"/>
+    <hyperlink ref="E51" r:id="rId9" xr:uid="{AB23B92F-9660-4602-A770-B4DC053103FF}"/>
+    <hyperlink ref="E38" r:id="rId10" xr:uid="{AE8D7F00-E698-4DC8-8467-18A519416BF0}"/>
+    <hyperlink ref="E46" r:id="rId11" xr:uid="{2C45B0C7-121E-4FEE-90E6-19A508CC0856}"/>
+    <hyperlink ref="E53" r:id="rId12" xr:uid="{73DD7FA1-8A09-481E-9BF0-EDD88E86EAC3}"/>
+    <hyperlink ref="E8" r:id="rId13" xr:uid="{B7739609-1510-4E1E-B8C4-81240570A0B0}"/>
+    <hyperlink ref="E16" r:id="rId14" xr:uid="{9D4D35EE-2216-4D82-ABE0-0760E544D7F3}"/>
     <hyperlink ref="E3" r:id="rId15" xr:uid="{BF5E4EB1-198E-4E95-86E7-1EF1374FF963}"/>
-    <hyperlink ref="E31" r:id="rId16" xr:uid="{15529467-5046-410B-9B6C-654495986B9C}"/>
-    <hyperlink ref="E17" r:id="rId17" xr:uid="{65E5E7CE-44B2-4FB0-BD3D-351DBED5A38A}"/>
-    <hyperlink ref="E15" r:id="rId18" xr:uid="{75A12DC5-3325-4C7B-9F69-1A0B70EF2357}"/>
+    <hyperlink ref="E37" r:id="rId16" xr:uid="{15529467-5046-410B-9B6C-654495986B9C}"/>
+    <hyperlink ref="E21" r:id="rId17" xr:uid="{65E5E7CE-44B2-4FB0-BD3D-351DBED5A38A}"/>
+    <hyperlink ref="E18" r:id="rId18" xr:uid="{75A12DC5-3325-4C7B-9F69-1A0B70EF2357}"/>
     <hyperlink ref="E2" r:id="rId19" xr:uid="{6A5A7183-040B-4C7C-A5E8-B8E3C0F52BCD}"/>
-    <hyperlink ref="E9" r:id="rId20" xr:uid="{C789739C-B0F4-4CB3-956F-269CAF2DFC8D}"/>
-    <hyperlink ref="E41" r:id="rId21" xr:uid="{A8E1490C-983B-4622-8DC5-5563FB81C76C}"/>
-    <hyperlink ref="E49" r:id="rId22" xr:uid="{DB56F6A2-172B-4E4C-8A53-CBAD5AE6BAAB}"/>
+    <hyperlink ref="E11" r:id="rId20" xr:uid="{C789739C-B0F4-4CB3-956F-269CAF2DFC8D}"/>
+    <hyperlink ref="E48" r:id="rId21" xr:uid="{A8E1490C-983B-4622-8DC5-5563FB81C76C}"/>
+    <hyperlink ref="E56" r:id="rId22" xr:uid="{DB56F6A2-172B-4E4C-8A53-CBAD5AE6BAAB}"/>
     <hyperlink ref="F2" r:id="rId23" xr:uid="{20EB67DC-FC82-4F1A-9B75-CBF513D8DE4E}"/>
-    <hyperlink ref="F44" r:id="rId24" xr:uid="{73781179-C544-4054-952B-FA4211662F26}"/>
-    <hyperlink ref="F46" r:id="rId25" xr:uid="{E86B653A-32F2-4FF7-91A8-FCB34C0FF2C2}"/>
-    <hyperlink ref="F10" r:id="rId26" xr:uid="{02494919-717B-478B-B79A-AE4E30A28014}"/>
-    <hyperlink ref="F20" r:id="rId27" xr:uid="{632AD9BE-E9BA-4153-995B-F235523DEE74}"/>
-    <hyperlink ref="F29" r:id="rId28" xr:uid="{7DBCE998-F80D-4D11-B542-1A4709AE8490}"/>
-    <hyperlink ref="F28" r:id="rId29" xr:uid="{5D0C808C-7E89-43C9-A13D-EED2709CC1D7}"/>
-    <hyperlink ref="F33" r:id="rId30" xr:uid="{64C3416A-7C81-40DD-BC58-E6E2E34EA840}"/>
-    <hyperlink ref="F36" r:id="rId31" xr:uid="{BAAE57A6-92DF-4790-90A3-C20208627A9C}"/>
-    <hyperlink ref="F22" r:id="rId32" xr:uid="{AF726EF3-BA18-451C-8E63-28F5F4EA1FC9}"/>
-    <hyperlink ref="F31" r:id="rId33" xr:uid="{AE1B5F2A-8864-4E2F-976A-CE56ADD6F999}"/>
-    <hyperlink ref="F38" r:id="rId34" xr:uid="{C8E38BF7-6188-48AC-A664-93E9163A8930}"/>
-    <hyperlink ref="F14" r:id="rId35" xr:uid="{994E4A5D-DC36-473B-9922-C223D8B30D3B}"/>
-    <hyperlink ref="F9" r:id="rId36" xr:uid="{D3D17A4B-395F-4F48-A33C-49AC6AA8E1E4}"/>
-    <hyperlink ref="F35" r:id="rId37" xr:uid="{E5B6EC13-EF0E-494F-8472-535EF67D8363}"/>
-    <hyperlink ref="F17" r:id="rId38" xr:uid="{2420FD62-4E63-4C9C-BE75-6AFA574DD4FA}"/>
-    <hyperlink ref="F41" r:id="rId39" xr:uid="{606EF7C0-92E0-4433-9350-F0BD9155211D}"/>
-    <hyperlink ref="F18" r:id="rId40" xr:uid="{E24CEC8F-56F5-44DD-8ED0-C170E20F245E}"/>
-    <hyperlink ref="F12" r:id="rId41" xr:uid="{CC7B146B-DFA0-437C-BD1C-353C0E3A04D8}"/>
-    <hyperlink ref="F34" r:id="rId42" xr:uid="{E1771B7F-29FC-44FD-89DE-44BF99EEAF8F}"/>
+    <hyperlink ref="F51" r:id="rId24" xr:uid="{73781179-C544-4054-952B-FA4211662F26}"/>
+    <hyperlink ref="F53" r:id="rId25" xr:uid="{E86B653A-32F2-4FF7-91A8-FCB34C0FF2C2}"/>
+    <hyperlink ref="F13" r:id="rId26" xr:uid="{02494919-717B-478B-B79A-AE4E30A28014}"/>
+    <hyperlink ref="F24" r:id="rId27" xr:uid="{632AD9BE-E9BA-4153-995B-F235523DEE74}"/>
+    <hyperlink ref="F35" r:id="rId28" xr:uid="{7DBCE998-F80D-4D11-B542-1A4709AE8490}"/>
+    <hyperlink ref="F34" r:id="rId29" xr:uid="{5D0C808C-7E89-43C9-A13D-EED2709CC1D7}"/>
+    <hyperlink ref="F39" r:id="rId30" xr:uid="{64C3416A-7C81-40DD-BC58-E6E2E34EA840}"/>
+    <hyperlink ref="F43" r:id="rId31" xr:uid="{BAAE57A6-92DF-4790-90A3-C20208627A9C}"/>
+    <hyperlink ref="F26" r:id="rId32" xr:uid="{AF726EF3-BA18-451C-8E63-28F5F4EA1FC9}"/>
+    <hyperlink ref="F37" r:id="rId33" xr:uid="{AE1B5F2A-8864-4E2F-976A-CE56ADD6F999}"/>
+    <hyperlink ref="F45" r:id="rId34" xr:uid="{C8E38BF7-6188-48AC-A664-93E9163A8930}"/>
+    <hyperlink ref="F17" r:id="rId35" xr:uid="{994E4A5D-DC36-473B-9922-C223D8B30D3B}"/>
+    <hyperlink ref="F11" r:id="rId36" xr:uid="{D3D17A4B-395F-4F48-A33C-49AC6AA8E1E4}"/>
+    <hyperlink ref="F41" r:id="rId37" xr:uid="{E5B6EC13-EF0E-494F-8472-535EF67D8363}"/>
+    <hyperlink ref="F21" r:id="rId38" xr:uid="{2420FD62-4E63-4C9C-BE75-6AFA574DD4FA}"/>
+    <hyperlink ref="F48" r:id="rId39" xr:uid="{606EF7C0-92E0-4433-9350-F0BD9155211D}"/>
+    <hyperlink ref="F22" r:id="rId40" xr:uid="{E24CEC8F-56F5-44DD-8ED0-C170E20F245E}"/>
+    <hyperlink ref="F15" r:id="rId41" xr:uid="{CC7B146B-DFA0-437C-BD1C-353C0E3A04D8}"/>
+    <hyperlink ref="F40" r:id="rId42" xr:uid="{E1771B7F-29FC-44FD-89DE-44BF99EEAF8F}"/>
     <hyperlink ref="F3" r:id="rId43" xr:uid="{8894D3F4-C9DD-4F73-B8D1-80EDE63AE046}"/>
-    <hyperlink ref="F13" r:id="rId44" xr:uid="{E6A676E9-77F9-4254-821A-7039857E625D}"/>
-    <hyperlink ref="F26" r:id="rId45" xr:uid="{03AEB7E0-B241-406C-88D9-A0F51076BEFC}"/>
-    <hyperlink ref="F30" r:id="rId46" xr:uid="{56FA5804-441B-4115-81F2-E6F57B48EEB0}"/>
-    <hyperlink ref="F8" r:id="rId47" xr:uid="{CD854081-ECE1-4806-B8AA-BFE6EA05BB4B}"/>
-    <hyperlink ref="F37" r:id="rId48" xr:uid="{330B2B26-05E9-4ABC-ABA3-42999D67AAE8}"/>
-    <hyperlink ref="F6" r:id="rId49" xr:uid="{34A7DD68-4900-4D76-B1DC-EBBDA4A2B1A6}"/>
-    <hyperlink ref="F25" r:id="rId50" xr:uid="{2C0DFA88-75D9-4BB4-A9EE-449C4C108A11}"/>
-    <hyperlink ref="F19" r:id="rId51" xr:uid="{F4FF688C-35E4-4D35-8C51-CD53EB6C2A8E}"/>
-    <hyperlink ref="F40" r:id="rId52" xr:uid="{2CB090FD-FB84-4A03-A89B-50F8A1C9F5BD}"/>
-    <hyperlink ref="F11" r:id="rId53" xr:uid="{B03C78ED-3523-452D-AD83-025C4F648157}"/>
-    <hyperlink ref="F27" r:id="rId54" xr:uid="{AC23ABB6-7E63-45F0-B07E-178795C65651}"/>
-    <hyperlink ref="F23" r:id="rId55" xr:uid="{253A3216-53A1-4AD4-9A4D-31EC0F346F7B}"/>
-    <hyperlink ref="F16" r:id="rId56" xr:uid="{D369BB7D-E54A-46CB-813D-E942B4FDBDA6}"/>
-    <hyperlink ref="F24" r:id="rId57" xr:uid="{682DFEC9-B62F-4777-8B03-2A2F3AD89C26}"/>
-    <hyperlink ref="F15" r:id="rId58" xr:uid="{97B23B61-03A2-46B0-8FDC-EC67D02494CD}"/>
-    <hyperlink ref="F7" r:id="rId59" xr:uid="{026695FB-A1A0-417C-8075-98AC08B3580C}"/>
-    <hyperlink ref="F32" r:id="rId60" xr:uid="{4D7429E8-6222-42F1-BD8D-3975D3CB77C3}"/>
-    <hyperlink ref="F39" r:id="rId61" xr:uid="{DAAEC77E-D512-4617-B851-2AD89315F496}"/>
-    <hyperlink ref="F48" r:id="rId62" xr:uid="{5833C0C8-BE25-404A-BCD5-B1BE6AB6638F}"/>
-    <hyperlink ref="E45" r:id="rId63" xr:uid="{50FEBA24-D2B4-420A-AEA7-6BB2D0719A52}"/>
-    <hyperlink ref="E10" r:id="rId64" xr:uid="{9F40885B-F7A9-4F17-A7CD-DEE821C50339}"/>
-    <hyperlink ref="E38" r:id="rId65" xr:uid="{5223544E-DDEF-48F9-9EB3-3EF1B9FDAB90}"/>
-    <hyperlink ref="E5" r:id="rId66" xr:uid="{F7C2BC13-BAF9-4996-AE90-F94B1E8EA045}"/>
-    <hyperlink ref="F5" r:id="rId67" xr:uid="{C942D955-FF96-47FC-9CE5-48E87F200A13}"/>
-    <hyperlink ref="E30" r:id="rId68" xr:uid="{9AA38BAF-4725-4754-B7EA-23E92B659CE2}"/>
-    <hyperlink ref="E34" r:id="rId69" xr:uid="{C838F4BD-E551-442C-B150-986D44024BB8}"/>
-    <hyperlink ref="F49" r:id="rId70" xr:uid="{75BD971A-96A3-46CE-985A-1488D76AC8A9}"/>
-    <hyperlink ref="E21" r:id="rId71" xr:uid="{0946638C-6244-4956-B991-62477DA31ADD}"/>
-    <hyperlink ref="F21" r:id="rId72" xr:uid="{284180A6-16F2-45D7-A1C3-FEFCA8D5DF8F}"/>
+    <hyperlink ref="F16" r:id="rId44" xr:uid="{E6A676E9-77F9-4254-821A-7039857E625D}"/>
+    <hyperlink ref="F31" r:id="rId45" xr:uid="{03AEB7E0-B241-406C-88D9-A0F51076BEFC}"/>
+    <hyperlink ref="F36" r:id="rId46" xr:uid="{56FA5804-441B-4115-81F2-E6F57B48EEB0}"/>
+    <hyperlink ref="F10" r:id="rId47" xr:uid="{CD854081-ECE1-4806-B8AA-BFE6EA05BB4B}"/>
+    <hyperlink ref="F44" r:id="rId48" xr:uid="{330B2B26-05E9-4ABC-ABA3-42999D67AAE8}"/>
+    <hyperlink ref="F8" r:id="rId49" xr:uid="{34A7DD68-4900-4D76-B1DC-EBBDA4A2B1A6}"/>
+    <hyperlink ref="F30" r:id="rId50" xr:uid="{2C0DFA88-75D9-4BB4-A9EE-449C4C108A11}"/>
+    <hyperlink ref="F23" r:id="rId51" xr:uid="{F4FF688C-35E4-4D35-8C51-CD53EB6C2A8E}"/>
+    <hyperlink ref="F47" r:id="rId52" xr:uid="{2CB090FD-FB84-4A03-A89B-50F8A1C9F5BD}"/>
+    <hyperlink ref="F14" r:id="rId53" xr:uid="{B03C78ED-3523-452D-AD83-025C4F648157}"/>
+    <hyperlink ref="F32" r:id="rId54" xr:uid="{AC23ABB6-7E63-45F0-B07E-178795C65651}"/>
+    <hyperlink ref="F27" r:id="rId55" xr:uid="{253A3216-53A1-4AD4-9A4D-31EC0F346F7B}"/>
+    <hyperlink ref="F20" r:id="rId56" xr:uid="{D369BB7D-E54A-46CB-813D-E942B4FDBDA6}"/>
+    <hyperlink ref="F28" r:id="rId57" xr:uid="{682DFEC9-B62F-4777-8B03-2A2F3AD89C26}"/>
+    <hyperlink ref="F18" r:id="rId58" xr:uid="{97B23B61-03A2-46B0-8FDC-EC67D02494CD}"/>
+    <hyperlink ref="F9" r:id="rId59" xr:uid="{026695FB-A1A0-417C-8075-98AC08B3580C}"/>
+    <hyperlink ref="F38" r:id="rId60" xr:uid="{4D7429E8-6222-42F1-BD8D-3975D3CB77C3}"/>
+    <hyperlink ref="F46" r:id="rId61" xr:uid="{DAAEC77E-D512-4617-B851-2AD89315F496}"/>
+    <hyperlink ref="F55" r:id="rId62" xr:uid="{5833C0C8-BE25-404A-BCD5-B1BE6AB6638F}"/>
+    <hyperlink ref="E52" r:id="rId63" xr:uid="{50FEBA24-D2B4-420A-AEA7-6BB2D0719A52}"/>
+    <hyperlink ref="E13" r:id="rId64" xr:uid="{9F40885B-F7A9-4F17-A7CD-DEE821C50339}"/>
+    <hyperlink ref="E45" r:id="rId65" xr:uid="{5223544E-DDEF-48F9-9EB3-3EF1B9FDAB90}"/>
+    <hyperlink ref="E7" r:id="rId66" xr:uid="{F7C2BC13-BAF9-4996-AE90-F94B1E8EA045}"/>
+    <hyperlink ref="F7" r:id="rId67" xr:uid="{C942D955-FF96-47FC-9CE5-48E87F200A13}"/>
+    <hyperlink ref="E36" r:id="rId68" xr:uid="{9AA38BAF-4725-4754-B7EA-23E92B659CE2}"/>
+    <hyperlink ref="E40" r:id="rId69" xr:uid="{C838F4BD-E551-442C-B150-986D44024BB8}"/>
+    <hyperlink ref="F56" r:id="rId70" xr:uid="{75BD971A-96A3-46CE-985A-1488D76AC8A9}"/>
+    <hyperlink ref="E25" r:id="rId71" xr:uid="{0946638C-6244-4956-B991-62477DA31ADD}"/>
+    <hyperlink ref="F25" r:id="rId72" xr:uid="{284180A6-16F2-45D7-A1C3-FEFCA8D5DF8F}"/>
     <hyperlink ref="E4" r:id="rId73" xr:uid="{25E264DA-B0C3-46BF-A97A-3AD180D45867}"/>
     <hyperlink ref="F4" r:id="rId74" xr:uid="{C0B54655-8946-4353-B1A2-7744E6BD8F27}"/>
+    <hyperlink ref="E19" r:id="rId75" xr:uid="{DA020059-D107-474F-AD71-FA4B691620C3}"/>
+    <hyperlink ref="E12" r:id="rId76" display="https://github.com/KinTheInfinite/Archipelago/releases" xr:uid="{F89569D4-6DED-42FD-92BE-2C3F7EF43530}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId75"/>
+  <pageSetup orientation="portrait" r:id="rId77"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated and added new worlds. Added ability to mark a world as experimental. Added css for experimental worlds to display a warning for the official asyncs. Updated webhost utils to allow loading option modules that do not live in the expected modules that are currently enforced.
</commit_message>
<xml_diff>
--- a/CustomWorldsInstalled.xlsx
+++ b/CustomWorldsInstalled.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\Git\Archipelago\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7649702A-0DC1-4AE3-95A5-816E908F1284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEDFCD00-C5B8-41DF-9DD0-AEB74B45C622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9630" yWindow="21480" windowWidth="29040" windowHeight="15840" xr2:uid="{3DBB16FA-FE5F-4BB0-89C2-A45EA748065E}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{3DBB16FA-FE5F-4BB0-89C2-A45EA748065E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="230">
   <si>
     <t>World</t>
   </si>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t>Chrono Trigger Jets of Time</t>
-  </si>
-  <si>
-    <t>Kingdom Hearts Re:Chain of Memories</t>
   </si>
   <si>
     <t>https://github.com/DrBibop/Archipelago_Inscryption/releases</t>
@@ -171,9 +168,6 @@
 https://github.com/junglechief87/arch_ffvcd/releases</t>
   </si>
   <si>
-    <t>Kingdom Hearts: Birth by Sleep</t>
-  </si>
-  <si>
     <t>https://github.com/gaithernOrg/ArchipelagoKHBBS/releases/</t>
   </si>
   <si>
@@ -186,9 +180,6 @@
     <t>1.4.2</t>
   </si>
   <si>
-    <t>7.2b</t>
-  </si>
-  <si>
     <t>Super Metroid Subversion</t>
   </si>
   <si>
@@ -240,9 +231,6 @@
     <t>Satisfactory</t>
   </si>
   <si>
-    <t>0.1.3.3</t>
-  </si>
-  <si>
     <t>https://github.com/Jarno458/SatisfactoryArchipelagoMod/releases</t>
   </si>
   <si>
@@ -292,9 +280,6 @@
   </si>
   <si>
     <t>1.4.0</t>
-  </si>
-  <si>
-    <t>https://github.com/TheLX5/Archipelago/releases</t>
   </si>
   <si>
     <t>Mega Man X2</t>
@@ -451,9 +436,6 @@
     <t>https://github.com/Rosalie-A/Archipelago/releases</t>
   </si>
   <si>
-    <t>0.2.4</t>
-  </si>
-  <si>
     <t>https://github.com/SenPierre/ArchipelagoOoA/releases</t>
   </si>
   <si>
@@ -484,9 +466,6 @@
     <t>https://discord.com/channels/731205301247803413/1210743818564149288</t>
   </si>
   <si>
-    <t>0.7.3</t>
-  </si>
-  <si>
     <t>0.0.2</t>
   </si>
   <si>
@@ -514,9 +493,6 @@
     <t>0.1.9</t>
   </si>
   <si>
-    <t>0.6.3</t>
-  </si>
-  <si>
     <t>1.1.2</t>
   </si>
   <si>
@@ -566,9 +542,6 @@
   </si>
   <si>
     <t>0.4.0</t>
-  </si>
-  <si>
-    <t>0.5.13</t>
   </si>
   <si>
     <t>2.6.1</t>
@@ -642,6 +615,120 @@
   <si>
     <t>https://github.com/KinTheInfinite/Archipelago/releases
 https://thunderstore.io/c/enter-the-gungeon/p/GungeonArchipelago/Gungeon_Archipelago/</t>
+  </si>
+  <si>
+    <t>0.6.5</t>
+  </si>
+  <si>
+    <t>3.0.2B</t>
+  </si>
+  <si>
+    <t>Kingdom Hearts: BBS</t>
+  </si>
+  <si>
+    <t>Kingdom Hearts: RECOM</t>
+  </si>
+  <si>
+    <t>Donkey Kong Country 2</t>
+  </si>
+  <si>
+    <t>2.0.0</t>
+  </si>
+  <si>
+    <t>https://github.com/TheLX5/Archipelago/releases?q=%22Donkey+Kong+Country+2%22&amp;expanded=true</t>
+  </si>
+  <si>
+    <t>https://github.com/TheLX5/Archipelago/releases?q=%22Mega+Man+X%22&amp;expanded=true</t>
+  </si>
+  <si>
+    <t>https://github.com/TheLX5/Archipelago/releases?q=%22Mega+Man+X2%22&amp;expanded=true</t>
+  </si>
+  <si>
+    <t>https://github.com/TheLX5/Archipelago/releases?q=%22Mega+Man+X3%22&amp;expanded=true</t>
+  </si>
+  <si>
+    <t>0.8.2</t>
+  </si>
+  <si>
+    <t>1.0.3</t>
+  </si>
+  <si>
+    <t>0.6.0</t>
+  </si>
+  <si>
+    <t>0.8.0</t>
+  </si>
+  <si>
+    <t>0.1.9b</t>
+  </si>
+  <si>
+    <t>Zelda II</t>
+  </si>
+  <si>
+    <t>https://github.com/PinkSwitch/Archipelago/releases?q=zelda&amp;expanded=true</t>
+  </si>
+  <si>
+    <t>https://discord.com/channels/731205301247803413/1239454398367924325</t>
+  </si>
+  <si>
+    <t>https://discord.com/channels/731205301247803413/1023381145565548646</t>
+  </si>
+  <si>
+    <t>Digimon World 1</t>
+  </si>
+  <si>
+    <t>https://discord.com/channels/731205301247803413/1224418923861118977</t>
+  </si>
+  <si>
+    <t>https://github.com/ArsonAssassin/DWAP/releases</t>
+  </si>
+  <si>
+    <t>0.2.1</t>
+  </si>
+  <si>
+    <t>Dark Cloud 2</t>
+  </si>
+  <si>
+    <t>0.0.1</t>
+  </si>
+  <si>
+    <t>https://discord.com/channels/731205301247803413/1220482938957729933</t>
+  </si>
+  <si>
+    <t>https://github.com/ArsonAssassin/DC2AP/releases</t>
+  </si>
+  <si>
+    <t>Keymaster's Keep</t>
+  </si>
+  <si>
+    <t>https://discord.com/channels/731205301247803413/1321323711676284939</t>
+  </si>
+  <si>
+    <t>https://github.com/SerpentAI/Archipelago/releases?q=%22Keymaster%27s+Keep%22&amp;expanded=true</t>
+  </si>
+  <si>
+    <t>pre-6</t>
+  </si>
+  <si>
+    <t>Shapez 2</t>
+  </si>
+  <si>
+    <t>https://discord.com/channels/731205301247803413/1278481415830245427</t>
+  </si>
+  <si>
+    <t>Cat Quest</t>
+  </si>
+  <si>
+    <t>https://discord.com/channels/731205301247803413/1319965826601844736</t>
+  </si>
+  <si>
+    <t>https://github.com/Nikkilites/Archipelago-CatQuest/releases</t>
+  </si>
+  <si>
+    <t>0.2.2</t>
+  </si>
+  <si>
+    <t>https://github.com/BlastSlimey/2hapezipelago/releases</t>
   </si>
 </sst>
 </file>
@@ -718,7 +805,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -745,6 +832,15 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1088,20 +1184,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{901AF876-1585-4DEB-9BCA-32AAC89A46F9}">
-  <dimension ref="A1:O56"/>
+  <dimension ref="A1:O63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomLeft" activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="75" customWidth="1"/>
+    <col min="5" max="5" width="92.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="67.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="0" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="7.28515625" hidden="1" customWidth="1"/>
@@ -1128,41 +1224,51 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O1" s="6">
-        <v>45645</v>
+        <v>45675</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4">
+      <c r="B2" s="15"/>
+      <c r="C2" s="13">
         <v>45274</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="13">
         <v>45422</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>32</v>
-      </c>
+      <c r="E2" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="C3" s="4">
         <v>45646</v>
@@ -1171,38 +1277,38 @@
         <v>45675</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>148</v>
+        <v>205</v>
       </c>
       <c r="C4" s="4">
-        <v>45668</v>
+        <v>45680</v>
       </c>
       <c r="D4" s="4">
-        <v>45675</v>
+        <v>45687</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>157</v>
+        <v>206</v>
       </c>
       <c r="C5" s="4">
         <v>45578</v>
@@ -1211,15 +1317,15 @@
         <v>45675</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="B6" s="3">
         <v>4.0999999999999996</v>
@@ -1231,18 +1337,18 @@
         <v>45675</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="C7" s="4">
         <v>45614</v>
@@ -1251,389 +1357,385 @@
         <v>45617</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="C8" s="11">
+        <v>45684</v>
+      </c>
+      <c r="D8" s="4">
+        <v>45687</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="4">
+      <c r="B9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="4">
         <v>45308</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D9" s="4">
         <v>45410</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="E9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D10" s="4">
         <v>45617</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="C10" s="4">
-        <v>45670</v>
-      </c>
-      <c r="D10" s="4">
-        <v>45675</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>21</v>
+      <c r="E10" s="7" t="s">
+        <v>125</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" s="3">
-        <v>3</v>
+        <v>15</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>192</v>
       </c>
       <c r="C11" s="4">
-        <v>45668</v>
+        <v>45684</v>
       </c>
       <c r="D11" s="4">
-        <v>45675</v>
+        <v>45687</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>63</v>
+        <v>20</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>198</v>
+        <v>215</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="C12" s="4">
-        <v>45532</v>
-      </c>
-      <c r="D12" s="4">
-        <v>45675</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>200</v>
+        <v>45906</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="5" t="s">
+        <v>218</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>199</v>
+        <v>217</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="B13" s="3">
-        <v>0.4</v>
+        <v>211</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>214</v>
       </c>
       <c r="C13" s="4">
-        <v>45641</v>
-      </c>
-      <c r="D13" s="4">
-        <v>45645</v>
-      </c>
+        <v>45588</v>
+      </c>
+      <c r="D13" s="4"/>
       <c r="E13" s="5" t="s">
-        <v>136</v>
+        <v>213</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>93</v>
+        <v>212</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>73</v>
+        <v>196</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>158</v>
+        <v>197</v>
       </c>
       <c r="C14" s="4">
-        <v>45615</v>
+        <v>45673</v>
       </c>
       <c r="D14" s="4">
-        <v>45617</v>
+        <v>45687</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>74</v>
+        <v>198</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="B15" s="3">
-        <v>82.5</v>
+        <v>49</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>193</v>
       </c>
       <c r="C15" s="4">
-        <v>45495</v>
+        <v>45687</v>
       </c>
       <c r="D15" s="4">
-        <v>45507</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>43</v>
+        <v>45687</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>60</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>92</v>
+        <v>189</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>155</v>
       </c>
       <c r="C16" s="4">
-        <v>45526</v>
+        <v>45532</v>
       </c>
       <c r="D16" s="4">
-        <v>45562</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>31</v>
+        <v>45675</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>191</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>31</v>
+        <v>190</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>79</v>
+        <v>85</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0.4</v>
       </c>
       <c r="C17" s="4">
-        <v>45557</v>
+        <v>45641</v>
       </c>
       <c r="D17" s="4">
-        <v>45562</v>
+        <v>45645</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>22</v>
+        <v>131</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>41</v>
+        <v>162</v>
       </c>
       <c r="C18" s="4">
-        <v>45425</v>
+        <v>45673</v>
       </c>
       <c r="D18" s="4">
-        <v>45478</v>
+        <v>45687</v>
       </c>
       <c r="E18" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="3">
+        <v>82.5</v>
+      </c>
+      <c r="C19" s="4">
+        <v>45495</v>
+      </c>
+      <c r="D19" s="4">
+        <v>45507</v>
+      </c>
+      <c r="E19" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="F18" s="5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="C19" s="4">
-        <v>45646</v>
-      </c>
-      <c r="D19" s="4">
-        <v>45675</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>186</v>
-      </c>
       <c r="F19" s="5" t="s">
-        <v>187</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>54</v>
+        <v>87</v>
       </c>
       <c r="C20" s="4">
-        <v>45542</v>
+        <v>45526</v>
       </c>
       <c r="D20" s="4">
-        <v>45547</v>
+        <v>45562</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>126</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>38</v>
+        <v>84</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>160</v>
+        <v>75</v>
       </c>
       <c r="C21" s="4">
-        <v>45618</v>
+        <v>45557</v>
       </c>
       <c r="D21" s="4">
-        <v>45632</v>
+        <v>45562</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C22" s="4">
-        <v>45516</v>
+        <v>45425</v>
       </c>
       <c r="D22" s="4">
-        <v>45519</v>
+        <v>45478</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>80</v>
+        <v>175</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>176</v>
       </c>
       <c r="C23" s="4">
-        <v>45555</v>
+        <v>45646</v>
       </c>
       <c r="D23" s="4">
-        <v>45562</v>
+        <v>45675</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>45</v>
+        <v>177</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>121</v>
+        <v>178</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>77</v>
+        <v>13</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="C24" s="4">
-        <v>45527</v>
+        <v>45542</v>
       </c>
       <c r="D24" s="4">
         <v>45547</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>94</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="B25" s="3">
-        <v>11</v>
+        <v>37</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>152</v>
       </c>
       <c r="C25" s="4">
-        <v>45675</v>
+        <v>45618</v>
       </c>
       <c r="D25" s="4">
-        <v>45675</v>
+        <v>45632</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>164</v>
+        <v>36</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>165</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>83</v>
+        <v>219</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>84</v>
+        <v>222</v>
       </c>
       <c r="C26" s="4">
-        <v>45528</v>
+        <v>45682</v>
       </c>
       <c r="D26" s="4">
-        <v>45562</v>
+        <v>45687</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>85</v>
+        <v>221</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>100</v>
+        <v>220</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
-        <v>86</v>
+        <v>194</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="C27" s="4">
         <v>45555</v>
@@ -1642,584 +1744,721 @@
         <v>45562</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>85</v>
+        <v>43</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>87</v>
+        <v>195</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>84</v>
+        <v>46</v>
       </c>
       <c r="C28" s="4">
-        <v>45527</v>
+        <v>45516</v>
       </c>
       <c r="D28" s="4">
-        <v>45562</v>
+        <v>45519</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>85</v>
+        <v>22</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>191</v>
+        <v>73</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>192</v>
+        <v>38</v>
       </c>
       <c r="C29" s="4">
-        <v>45623</v>
+        <v>45527</v>
       </c>
       <c r="D29" s="4">
-        <v>45675</v>
+        <v>45547</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>193</v>
+        <v>74</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>194</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>171</v>
+        <v>154</v>
+      </c>
+      <c r="B30" s="3">
+        <v>11.1</v>
       </c>
       <c r="C30" s="4">
-        <v>45674</v>
+        <v>45683</v>
       </c>
       <c r="D30" s="4">
-        <v>45675</v>
+        <v>45687</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>71</v>
+        <v>156</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>120</v>
+        <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="C31" s="4">
-        <v>45631</v>
+        <v>45528</v>
       </c>
       <c r="D31" s="4">
-        <v>45632</v>
+        <v>45562</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>70</v>
+        <v>199</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
-        <v>8</v>
+        <v>81</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>161</v>
+        <v>83</v>
       </c>
       <c r="C32" s="4">
-        <v>45626</v>
+        <v>45555</v>
       </c>
       <c r="D32" s="4">
-        <v>45632</v>
+        <v>45562</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>19</v>
+        <v>200</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>180</v>
+        <v>82</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>34</v>
+        <v>80</v>
       </c>
       <c r="C33" s="4">
-        <v>45671</v>
+        <v>45527</v>
       </c>
       <c r="D33" s="4">
-        <v>45675</v>
+        <v>45562</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>181</v>
+        <v>201</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>182</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>96</v>
+        <v>182</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>137</v>
+        <v>183</v>
       </c>
       <c r="C34" s="4">
-        <v>45544</v>
+        <v>45623</v>
       </c>
       <c r="D34" s="4">
-        <v>45575</v>
+        <v>45675</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>138</v>
+        <v>184</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>97</v>
+        <v>185</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>49</v>
+        <v>163</v>
       </c>
       <c r="C35" s="4">
-        <v>45516</v>
+        <v>45674</v>
       </c>
       <c r="D35" s="4">
-        <v>45519</v>
+        <v>45675</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>172</v>
+        <v>51</v>
       </c>
       <c r="C36" s="4">
-        <v>45646</v>
+        <v>45631</v>
       </c>
       <c r="D36" s="4">
-        <v>45675</v>
+        <v>45632</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
-        <v>35</v>
+        <v>171</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>173</v>
+        <v>33</v>
       </c>
       <c r="C37" s="4">
-        <v>45646</v>
+        <v>45671</v>
       </c>
       <c r="D37" s="4">
         <v>45675</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>36</v>
+        <v>172</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>101</v>
+        <v>173</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="C38" s="4">
-        <v>45317</v>
+        <v>45626</v>
       </c>
       <c r="D38" s="4">
-        <v>45422</v>
+        <v>45632</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>27</v>
+        <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
-        <v>56</v>
+        <v>91</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C39" s="4">
-        <v>45488</v>
+        <v>45683</v>
       </c>
       <c r="D39" s="4">
-        <v>45519</v>
+        <v>45687</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>57</v>
+        <v>132</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>148</v>
+        <v>6</v>
+      </c>
+      <c r="B40" s="3">
+        <v>8</v>
       </c>
       <c r="C40" s="4">
-        <v>45582</v>
+        <v>45683</v>
       </c>
       <c r="D40" s="4">
-        <v>45603</v>
+        <v>45687</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>14</v>
+        <v>164</v>
+      </c>
+      <c r="C41" s="4">
+        <v>45646</v>
       </c>
       <c r="D41" s="4">
-        <v>45422</v>
+        <v>45675</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
-        <v>195</v>
+        <v>34</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="C42" s="4">
-        <v>45674</v>
+        <v>45646</v>
       </c>
       <c r="D42" s="4">
         <v>45675</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>196</v>
+        <v>35</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>197</v>
+        <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>131</v>
+        <v>10</v>
       </c>
       <c r="C43" s="4">
-        <v>45568</v>
+        <v>45317</v>
       </c>
       <c r="D43" s="4">
-        <v>45575</v>
+        <v>45422</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>99</v>
+        <v>26</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C44" s="4">
-        <v>45376</v>
+        <v>45488</v>
       </c>
       <c r="D44" s="4">
-        <v>45533</v>
+        <v>45519</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
-        <v>102</v>
+        <v>56</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>174</v>
+        <v>202</v>
       </c>
       <c r="C45" s="4">
-        <v>45638</v>
+        <v>45683</v>
       </c>
       <c r="D45" s="4">
-        <v>45675</v>
+        <v>45687</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>150</v>
+        <v>57</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="C46" s="4">
-        <v>45646</v>
+        <v>14</v>
       </c>
       <c r="D46" s="4">
-        <v>45675</v>
+        <v>45422</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>135</v>
+        <v>101</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
-        <v>61</v>
+        <v>186</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="C47" s="4">
-        <v>45661</v>
+        <v>45674</v>
       </c>
       <c r="D47" s="4">
         <v>45675</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>62</v>
+        <v>187</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>122</v>
+        <v>188</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>163</v>
+        <v>126</v>
       </c>
       <c r="C48" s="4">
-        <v>45674</v>
+        <v>45568</v>
       </c>
       <c r="D48" s="4">
-        <v>45675</v>
+        <v>45575</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
-        <v>140</v>
+        <v>63</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>141</v>
+        <v>203</v>
       </c>
       <c r="C49" s="4">
-        <v>45518</v>
+        <v>45680</v>
       </c>
       <c r="D49" s="4">
-        <v>45575</v>
+        <v>45687</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>142</v>
+        <v>64</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>143</v>
+        <v>113</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
-        <v>132</v>
+        <v>97</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>80</v>
+        <v>166</v>
       </c>
       <c r="C50" s="4">
-        <v>45597</v>
+        <v>45638</v>
       </c>
       <c r="D50" s="4">
-        <v>45603</v>
+        <v>45675</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>134</v>
+        <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>25</v>
+        <v>167</v>
       </c>
       <c r="C51" s="4">
-        <v>45442</v>
+        <v>45646</v>
       </c>
       <c r="D51" s="4">
-        <v>45447</v>
+        <v>45675</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>26</v>
+        <v>130</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C52" s="4"/>
+        <v>58</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="C52" s="4">
+        <v>45682</v>
+      </c>
       <c r="D52" s="4">
-        <v>45519</v>
+        <v>45687</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>51</v>
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
-        <v>12</v>
+        <v>223</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>159</v>
+        <v>216</v>
       </c>
       <c r="C53" s="4">
-        <v>45579</v>
-      </c>
-      <c r="D53" s="4">
-        <v>45617</v>
+        <v>45656</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>29</v>
+        <v>229</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>29</v>
+        <v>224</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
-        <v>156</v>
+        <v>77</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="C54" s="4">
-        <v>45611</v>
+        <v>45674</v>
       </c>
       <c r="D54" s="4">
-        <v>45617</v>
+        <v>45675</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>154</v>
+        <v>78</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>155</v>
+        <v>103</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>177</v>
+        <v>135</v>
       </c>
       <c r="C55" s="4">
-        <v>45661</v>
+        <v>45518</v>
       </c>
       <c r="D55" s="4">
-        <v>45675</v>
+        <v>45575</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>145</v>
+        <v>76</v>
       </c>
       <c r="C56" s="4">
+        <v>45597</v>
+      </c>
+      <c r="D56" s="4">
+        <v>45603</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C57" s="4">
+        <v>45442</v>
+      </c>
+      <c r="D57" s="4">
+        <v>45447</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4">
+        <v>45519</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C59" s="4">
+        <v>45579</v>
+      </c>
+      <c r="D59" s="4">
+        <v>45617</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C60" s="4">
+        <v>45611</v>
+      </c>
+      <c r="D60" s="4">
+        <v>45617</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C61" s="4">
+        <v>45661</v>
+      </c>
+      <c r="D61" s="4">
+        <v>45675</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C62" s="4">
         <v>45530</v>
       </c>
-      <c r="D56" s="4">
+      <c r="D62" s="4">
         <v>45575</v>
       </c>
-      <c r="E56" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="F56" s="5" t="s">
-        <v>147</v>
+      <c r="E62" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="B63" s="3">
+        <v>1</v>
+      </c>
+      <c r="C63" s="4">
+        <v>45680</v>
+      </c>
+      <c r="D63" s="4">
+        <v>45687</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>209</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F56">
-    <sortCondition ref="A2:A56"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F63">
+    <sortCondition ref="A2:A63"/>
   </sortState>
   <conditionalFormatting sqref="A2:XFD132">
     <cfRule type="expression" dxfId="0" priority="2">
@@ -2227,91 +2466,108 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E32" r:id="rId1" xr:uid="{A5B7ED1F-2322-489C-9115-C445E82B54FB}"/>
-    <hyperlink ref="E22" r:id="rId2" xr:uid="{90F7D550-3232-4E6C-9AB7-856BDF3EA309}"/>
-    <hyperlink ref="E20" r:id="rId3" xr:uid="{5D7F93FB-6C49-403A-9AD8-F4281B6B2D94}"/>
-    <hyperlink ref="E15" r:id="rId4" display="https://github.com/cleartonic/arch_ffvcd/releases" xr:uid="{8C8885B9-A3DC-40DD-B18B-F3B348BB2202}"/>
-    <hyperlink ref="E17" r:id="rId5" xr:uid="{EC4A68ED-DCD0-44C0-9669-EAC47138143B}"/>
-    <hyperlink ref="E10" r:id="rId6" xr:uid="{2531395D-2F00-44AD-B326-97CA7E60977D}"/>
-    <hyperlink ref="E9" r:id="rId7" display="https://wiki.ctjot.com/doku.php?id=multiworld" xr:uid="{A1F02D1E-D96D-4326-BAA2-C7F18AF552BF}"/>
-    <hyperlink ref="E41" r:id="rId8" xr:uid="{39C13D86-F950-4EA9-AD8E-0CD6464A6C33}"/>
-    <hyperlink ref="E51" r:id="rId9" xr:uid="{AB23B92F-9660-4602-A770-B4DC053103FF}"/>
-    <hyperlink ref="E38" r:id="rId10" xr:uid="{AE8D7F00-E698-4DC8-8467-18A519416BF0}"/>
-    <hyperlink ref="E46" r:id="rId11" xr:uid="{2C45B0C7-121E-4FEE-90E6-19A508CC0856}"/>
-    <hyperlink ref="E53" r:id="rId12" xr:uid="{73DD7FA1-8A09-481E-9BF0-EDD88E86EAC3}"/>
-    <hyperlink ref="E8" r:id="rId13" xr:uid="{B7739609-1510-4E1E-B8C4-81240570A0B0}"/>
-    <hyperlink ref="E16" r:id="rId14" xr:uid="{9D4D35EE-2216-4D82-ABE0-0760E544D7F3}"/>
+    <hyperlink ref="E38" r:id="rId1" xr:uid="{A5B7ED1F-2322-489C-9115-C445E82B54FB}"/>
+    <hyperlink ref="E28" r:id="rId2" xr:uid="{90F7D550-3232-4E6C-9AB7-856BDF3EA309}"/>
+    <hyperlink ref="E24" r:id="rId3" xr:uid="{5D7F93FB-6C49-403A-9AD8-F4281B6B2D94}"/>
+    <hyperlink ref="E19" r:id="rId4" display="https://github.com/cleartonic/arch_ffvcd/releases" xr:uid="{8C8885B9-A3DC-40DD-B18B-F3B348BB2202}"/>
+    <hyperlink ref="E21" r:id="rId5" xr:uid="{EC4A68ED-DCD0-44C0-9669-EAC47138143B}"/>
+    <hyperlink ref="E11" r:id="rId6" xr:uid="{2531395D-2F00-44AD-B326-97CA7E60977D}"/>
+    <hyperlink ref="E10" r:id="rId7" display="https://wiki.ctjot.com/doku.php?id=multiworld" xr:uid="{A1F02D1E-D96D-4326-BAA2-C7F18AF552BF}"/>
+    <hyperlink ref="E46" r:id="rId8" xr:uid="{39C13D86-F950-4EA9-AD8E-0CD6464A6C33}"/>
+    <hyperlink ref="E57" r:id="rId9" xr:uid="{AB23B92F-9660-4602-A770-B4DC053103FF}"/>
+    <hyperlink ref="E43" r:id="rId10" xr:uid="{AE8D7F00-E698-4DC8-8467-18A519416BF0}"/>
+    <hyperlink ref="E51" r:id="rId11" xr:uid="{2C45B0C7-121E-4FEE-90E6-19A508CC0856}"/>
+    <hyperlink ref="E59" r:id="rId12" xr:uid="{73DD7FA1-8A09-481E-9BF0-EDD88E86EAC3}"/>
+    <hyperlink ref="E9" r:id="rId13" xr:uid="{B7739609-1510-4E1E-B8C4-81240570A0B0}"/>
+    <hyperlink ref="E20" r:id="rId14" xr:uid="{9D4D35EE-2216-4D82-ABE0-0760E544D7F3}"/>
     <hyperlink ref="E3" r:id="rId15" xr:uid="{BF5E4EB1-198E-4E95-86E7-1EF1374FF963}"/>
-    <hyperlink ref="E37" r:id="rId16" xr:uid="{15529467-5046-410B-9B6C-654495986B9C}"/>
-    <hyperlink ref="E21" r:id="rId17" xr:uid="{65E5E7CE-44B2-4FB0-BD3D-351DBED5A38A}"/>
-    <hyperlink ref="E18" r:id="rId18" xr:uid="{75A12DC5-3325-4C7B-9F69-1A0B70EF2357}"/>
+    <hyperlink ref="E42" r:id="rId16" xr:uid="{15529467-5046-410B-9B6C-654495986B9C}"/>
+    <hyperlink ref="E25" r:id="rId17" xr:uid="{65E5E7CE-44B2-4FB0-BD3D-351DBED5A38A}"/>
+    <hyperlink ref="E22" r:id="rId18" xr:uid="{75A12DC5-3325-4C7B-9F69-1A0B70EF2357}"/>
     <hyperlink ref="E2" r:id="rId19" xr:uid="{6A5A7183-040B-4C7C-A5E8-B8E3C0F52BCD}"/>
-    <hyperlink ref="E11" r:id="rId20" xr:uid="{C789739C-B0F4-4CB3-956F-269CAF2DFC8D}"/>
-    <hyperlink ref="E48" r:id="rId21" xr:uid="{A8E1490C-983B-4622-8DC5-5563FB81C76C}"/>
-    <hyperlink ref="E56" r:id="rId22" xr:uid="{DB56F6A2-172B-4E4C-8A53-CBAD5AE6BAAB}"/>
+    <hyperlink ref="E15" r:id="rId20" xr:uid="{C789739C-B0F4-4CB3-956F-269CAF2DFC8D}"/>
+    <hyperlink ref="E54" r:id="rId21" xr:uid="{A8E1490C-983B-4622-8DC5-5563FB81C76C}"/>
+    <hyperlink ref="E62" r:id="rId22" xr:uid="{DB56F6A2-172B-4E4C-8A53-CBAD5AE6BAAB}"/>
     <hyperlink ref="F2" r:id="rId23" xr:uid="{20EB67DC-FC82-4F1A-9B75-CBF513D8DE4E}"/>
-    <hyperlink ref="F51" r:id="rId24" xr:uid="{73781179-C544-4054-952B-FA4211662F26}"/>
-    <hyperlink ref="F53" r:id="rId25" xr:uid="{E86B653A-32F2-4FF7-91A8-FCB34C0FF2C2}"/>
-    <hyperlink ref="F13" r:id="rId26" xr:uid="{02494919-717B-478B-B79A-AE4E30A28014}"/>
-    <hyperlink ref="F24" r:id="rId27" xr:uid="{632AD9BE-E9BA-4153-995B-F235523DEE74}"/>
-    <hyperlink ref="F35" r:id="rId28" xr:uid="{7DBCE998-F80D-4D11-B542-1A4709AE8490}"/>
-    <hyperlink ref="F34" r:id="rId29" xr:uid="{5D0C808C-7E89-43C9-A13D-EED2709CC1D7}"/>
-    <hyperlink ref="F39" r:id="rId30" xr:uid="{64C3416A-7C81-40DD-BC58-E6E2E34EA840}"/>
-    <hyperlink ref="F43" r:id="rId31" xr:uid="{BAAE57A6-92DF-4790-90A3-C20208627A9C}"/>
-    <hyperlink ref="F26" r:id="rId32" xr:uid="{AF726EF3-BA18-451C-8E63-28F5F4EA1FC9}"/>
-    <hyperlink ref="F37" r:id="rId33" xr:uid="{AE1B5F2A-8864-4E2F-976A-CE56ADD6F999}"/>
-    <hyperlink ref="F45" r:id="rId34" xr:uid="{C8E38BF7-6188-48AC-A664-93E9163A8930}"/>
-    <hyperlink ref="F17" r:id="rId35" xr:uid="{994E4A5D-DC36-473B-9922-C223D8B30D3B}"/>
-    <hyperlink ref="F11" r:id="rId36" xr:uid="{D3D17A4B-395F-4F48-A33C-49AC6AA8E1E4}"/>
-    <hyperlink ref="F41" r:id="rId37" xr:uid="{E5B6EC13-EF0E-494F-8472-535EF67D8363}"/>
-    <hyperlink ref="F21" r:id="rId38" xr:uid="{2420FD62-4E63-4C9C-BE75-6AFA574DD4FA}"/>
-    <hyperlink ref="F48" r:id="rId39" xr:uid="{606EF7C0-92E0-4433-9350-F0BD9155211D}"/>
-    <hyperlink ref="F22" r:id="rId40" xr:uid="{E24CEC8F-56F5-44DD-8ED0-C170E20F245E}"/>
-    <hyperlink ref="F15" r:id="rId41" xr:uid="{CC7B146B-DFA0-437C-BD1C-353C0E3A04D8}"/>
-    <hyperlink ref="F40" r:id="rId42" xr:uid="{E1771B7F-29FC-44FD-89DE-44BF99EEAF8F}"/>
+    <hyperlink ref="F57" r:id="rId24" xr:uid="{73781179-C544-4054-952B-FA4211662F26}"/>
+    <hyperlink ref="F59" r:id="rId25" xr:uid="{E86B653A-32F2-4FF7-91A8-FCB34C0FF2C2}"/>
+    <hyperlink ref="F17" r:id="rId26" xr:uid="{02494919-717B-478B-B79A-AE4E30A28014}"/>
+    <hyperlink ref="F29" r:id="rId27" xr:uid="{632AD9BE-E9BA-4153-995B-F235523DEE74}"/>
+    <hyperlink ref="F40" r:id="rId28" xr:uid="{7DBCE998-F80D-4D11-B542-1A4709AE8490}"/>
+    <hyperlink ref="F39" r:id="rId29" xr:uid="{5D0C808C-7E89-43C9-A13D-EED2709CC1D7}"/>
+    <hyperlink ref="F44" r:id="rId30" xr:uid="{64C3416A-7C81-40DD-BC58-E6E2E34EA840}"/>
+    <hyperlink ref="F48" r:id="rId31" xr:uid="{BAAE57A6-92DF-4790-90A3-C20208627A9C}"/>
+    <hyperlink ref="F31" r:id="rId32" xr:uid="{AF726EF3-BA18-451C-8E63-28F5F4EA1FC9}"/>
+    <hyperlink ref="F42" r:id="rId33" xr:uid="{AE1B5F2A-8864-4E2F-976A-CE56ADD6F999}"/>
+    <hyperlink ref="F50" r:id="rId34" xr:uid="{C8E38BF7-6188-48AC-A664-93E9163A8930}"/>
+    <hyperlink ref="F21" r:id="rId35" xr:uid="{994E4A5D-DC36-473B-9922-C223D8B30D3B}"/>
+    <hyperlink ref="F15" r:id="rId36" xr:uid="{D3D17A4B-395F-4F48-A33C-49AC6AA8E1E4}"/>
+    <hyperlink ref="F46" r:id="rId37" xr:uid="{E5B6EC13-EF0E-494F-8472-535EF67D8363}"/>
+    <hyperlink ref="F25" r:id="rId38" xr:uid="{2420FD62-4E63-4C9C-BE75-6AFA574DD4FA}"/>
+    <hyperlink ref="F54" r:id="rId39" xr:uid="{606EF7C0-92E0-4433-9350-F0BD9155211D}"/>
+    <hyperlink ref="F28" r:id="rId40" xr:uid="{E24CEC8F-56F5-44DD-8ED0-C170E20F245E}"/>
+    <hyperlink ref="F19" r:id="rId41" xr:uid="{CC7B146B-DFA0-437C-BD1C-353C0E3A04D8}"/>
+    <hyperlink ref="F45" r:id="rId42" xr:uid="{E1771B7F-29FC-44FD-89DE-44BF99EEAF8F}"/>
     <hyperlink ref="F3" r:id="rId43" xr:uid="{8894D3F4-C9DD-4F73-B8D1-80EDE63AE046}"/>
-    <hyperlink ref="F16" r:id="rId44" xr:uid="{E6A676E9-77F9-4254-821A-7039857E625D}"/>
-    <hyperlink ref="F31" r:id="rId45" xr:uid="{03AEB7E0-B241-406C-88D9-A0F51076BEFC}"/>
-    <hyperlink ref="F36" r:id="rId46" xr:uid="{56FA5804-441B-4115-81F2-E6F57B48EEB0}"/>
-    <hyperlink ref="F10" r:id="rId47" xr:uid="{CD854081-ECE1-4806-B8AA-BFE6EA05BB4B}"/>
-    <hyperlink ref="F44" r:id="rId48" xr:uid="{330B2B26-05E9-4ABC-ABA3-42999D67AAE8}"/>
-    <hyperlink ref="F8" r:id="rId49" xr:uid="{34A7DD68-4900-4D76-B1DC-EBBDA4A2B1A6}"/>
-    <hyperlink ref="F30" r:id="rId50" xr:uid="{2C0DFA88-75D9-4BB4-A9EE-449C4C108A11}"/>
-    <hyperlink ref="F23" r:id="rId51" xr:uid="{F4FF688C-35E4-4D35-8C51-CD53EB6C2A8E}"/>
-    <hyperlink ref="F47" r:id="rId52" xr:uid="{2CB090FD-FB84-4A03-A89B-50F8A1C9F5BD}"/>
-    <hyperlink ref="F14" r:id="rId53" xr:uid="{B03C78ED-3523-452D-AD83-025C4F648157}"/>
-    <hyperlink ref="F32" r:id="rId54" xr:uid="{AC23ABB6-7E63-45F0-B07E-178795C65651}"/>
-    <hyperlink ref="F27" r:id="rId55" xr:uid="{253A3216-53A1-4AD4-9A4D-31EC0F346F7B}"/>
-    <hyperlink ref="F20" r:id="rId56" xr:uid="{D369BB7D-E54A-46CB-813D-E942B4FDBDA6}"/>
-    <hyperlink ref="F28" r:id="rId57" xr:uid="{682DFEC9-B62F-4777-8B03-2A2F3AD89C26}"/>
-    <hyperlink ref="F18" r:id="rId58" xr:uid="{97B23B61-03A2-46B0-8FDC-EC67D02494CD}"/>
-    <hyperlink ref="F9" r:id="rId59" xr:uid="{026695FB-A1A0-417C-8075-98AC08B3580C}"/>
-    <hyperlink ref="F38" r:id="rId60" xr:uid="{4D7429E8-6222-42F1-BD8D-3975D3CB77C3}"/>
-    <hyperlink ref="F46" r:id="rId61" xr:uid="{DAAEC77E-D512-4617-B851-2AD89315F496}"/>
-    <hyperlink ref="F55" r:id="rId62" xr:uid="{5833C0C8-BE25-404A-BCD5-B1BE6AB6638F}"/>
-    <hyperlink ref="E52" r:id="rId63" xr:uid="{50FEBA24-D2B4-420A-AEA7-6BB2D0719A52}"/>
-    <hyperlink ref="E13" r:id="rId64" xr:uid="{9F40885B-F7A9-4F17-A7CD-DEE821C50339}"/>
-    <hyperlink ref="E45" r:id="rId65" xr:uid="{5223544E-DDEF-48F9-9EB3-3EF1B9FDAB90}"/>
+    <hyperlink ref="F20" r:id="rId44" xr:uid="{E6A676E9-77F9-4254-821A-7039857E625D}"/>
+    <hyperlink ref="F36" r:id="rId45" xr:uid="{03AEB7E0-B241-406C-88D9-A0F51076BEFC}"/>
+    <hyperlink ref="F41" r:id="rId46" xr:uid="{56FA5804-441B-4115-81F2-E6F57B48EEB0}"/>
+    <hyperlink ref="F11" r:id="rId47" xr:uid="{CD854081-ECE1-4806-B8AA-BFE6EA05BB4B}"/>
+    <hyperlink ref="F49" r:id="rId48" xr:uid="{330B2B26-05E9-4ABC-ABA3-42999D67AAE8}"/>
+    <hyperlink ref="F9" r:id="rId49" xr:uid="{34A7DD68-4900-4D76-B1DC-EBBDA4A2B1A6}"/>
+    <hyperlink ref="F35" r:id="rId50" xr:uid="{2C0DFA88-75D9-4BB4-A9EE-449C4C108A11}"/>
+    <hyperlink ref="F27" r:id="rId51" xr:uid="{F4FF688C-35E4-4D35-8C51-CD53EB6C2A8E}"/>
+    <hyperlink ref="F52" r:id="rId52" xr:uid="{2CB090FD-FB84-4A03-A89B-50F8A1C9F5BD}"/>
+    <hyperlink ref="F18" r:id="rId53" xr:uid="{B03C78ED-3523-452D-AD83-025C4F648157}"/>
+    <hyperlink ref="F38" r:id="rId54" xr:uid="{AC23ABB6-7E63-45F0-B07E-178795C65651}"/>
+    <hyperlink ref="F32" r:id="rId55" xr:uid="{253A3216-53A1-4AD4-9A4D-31EC0F346F7B}"/>
+    <hyperlink ref="F24" r:id="rId56" xr:uid="{D369BB7D-E54A-46CB-813D-E942B4FDBDA6}"/>
+    <hyperlink ref="F33" r:id="rId57" xr:uid="{682DFEC9-B62F-4777-8B03-2A2F3AD89C26}"/>
+    <hyperlink ref="F22" r:id="rId58" xr:uid="{97B23B61-03A2-46B0-8FDC-EC67D02494CD}"/>
+    <hyperlink ref="F10" r:id="rId59" xr:uid="{026695FB-A1A0-417C-8075-98AC08B3580C}"/>
+    <hyperlink ref="F43" r:id="rId60" xr:uid="{4D7429E8-6222-42F1-BD8D-3975D3CB77C3}"/>
+    <hyperlink ref="F51" r:id="rId61" xr:uid="{DAAEC77E-D512-4617-B851-2AD89315F496}"/>
+    <hyperlink ref="F61" r:id="rId62" xr:uid="{5833C0C8-BE25-404A-BCD5-B1BE6AB6638F}"/>
+    <hyperlink ref="E58" r:id="rId63" xr:uid="{50FEBA24-D2B4-420A-AEA7-6BB2D0719A52}"/>
+    <hyperlink ref="E17" r:id="rId64" xr:uid="{9F40885B-F7A9-4F17-A7CD-DEE821C50339}"/>
+    <hyperlink ref="E50" r:id="rId65" xr:uid="{5223544E-DDEF-48F9-9EB3-3EF1B9FDAB90}"/>
     <hyperlink ref="E7" r:id="rId66" xr:uid="{F7C2BC13-BAF9-4996-AE90-F94B1E8EA045}"/>
     <hyperlink ref="F7" r:id="rId67" xr:uid="{C942D955-FF96-47FC-9CE5-48E87F200A13}"/>
-    <hyperlink ref="E36" r:id="rId68" xr:uid="{9AA38BAF-4725-4754-B7EA-23E92B659CE2}"/>
-    <hyperlink ref="E40" r:id="rId69" xr:uid="{C838F4BD-E551-442C-B150-986D44024BB8}"/>
-    <hyperlink ref="F56" r:id="rId70" xr:uid="{75BD971A-96A3-46CE-985A-1488D76AC8A9}"/>
-    <hyperlink ref="E25" r:id="rId71" xr:uid="{0946638C-6244-4956-B991-62477DA31ADD}"/>
-    <hyperlink ref="F25" r:id="rId72" xr:uid="{284180A6-16F2-45D7-A1C3-FEFCA8D5DF8F}"/>
+    <hyperlink ref="E41" r:id="rId68" xr:uid="{9AA38BAF-4725-4754-B7EA-23E92B659CE2}"/>
+    <hyperlink ref="E45" r:id="rId69" xr:uid="{C838F4BD-E551-442C-B150-986D44024BB8}"/>
+    <hyperlink ref="F62" r:id="rId70" xr:uid="{75BD971A-96A3-46CE-985A-1488D76AC8A9}"/>
+    <hyperlink ref="E30" r:id="rId71" xr:uid="{0946638C-6244-4956-B991-62477DA31ADD}"/>
+    <hyperlink ref="F30" r:id="rId72" xr:uid="{284180A6-16F2-45D7-A1C3-FEFCA8D5DF8F}"/>
     <hyperlink ref="E4" r:id="rId73" xr:uid="{25E264DA-B0C3-46BF-A97A-3AD180D45867}"/>
     <hyperlink ref="F4" r:id="rId74" xr:uid="{C0B54655-8946-4353-B1A2-7744E6BD8F27}"/>
-    <hyperlink ref="E19" r:id="rId75" xr:uid="{DA020059-D107-474F-AD71-FA4B691620C3}"/>
-    <hyperlink ref="E12" r:id="rId76" display="https://github.com/KinTheInfinite/Archipelago/releases" xr:uid="{F89569D4-6DED-42FD-92BE-2C3F7EF43530}"/>
+    <hyperlink ref="E23" r:id="rId75" xr:uid="{DA020059-D107-474F-AD71-FA4B691620C3}"/>
+    <hyperlink ref="E16" r:id="rId76" display="https://github.com/KinTheInfinite/Archipelago/releases" xr:uid="{F89569D4-6DED-42FD-92BE-2C3F7EF43530}"/>
     <hyperlink ref="F5" r:id="rId77" xr:uid="{BF9E4E83-5742-4615-B200-4C1F37F85400}"/>
     <hyperlink ref="F6" r:id="rId78" xr:uid="{8BBEEF6A-BE59-43A2-A2B0-3B29FB59AF38}"/>
-    <hyperlink ref="F19" r:id="rId79" xr:uid="{EB36F77B-E092-4401-A2AB-084464E6E8DA}"/>
-    <hyperlink ref="F29" r:id="rId80" xr:uid="{3713800B-0A12-4AAE-9BD5-4F93AD851F0E}"/>
-    <hyperlink ref="F33" r:id="rId81" xr:uid="{9BD0D58C-FD3A-4471-8DA0-1961D4880B10}"/>
-    <hyperlink ref="F42" r:id="rId82" xr:uid="{4EF6A25D-97B9-41C5-AD14-BF4F4D8BDF34}"/>
-    <hyperlink ref="F12" r:id="rId83" xr:uid="{2D115D7B-5F56-4E0A-95AE-0F9322EF7834}"/>
+    <hyperlink ref="F23" r:id="rId79" xr:uid="{EB36F77B-E092-4401-A2AB-084464E6E8DA}"/>
+    <hyperlink ref="F34" r:id="rId80" xr:uid="{3713800B-0A12-4AAE-9BD5-4F93AD851F0E}"/>
+    <hyperlink ref="F37" r:id="rId81" xr:uid="{9BD0D58C-FD3A-4471-8DA0-1961D4880B10}"/>
+    <hyperlink ref="F47" r:id="rId82" xr:uid="{4EF6A25D-97B9-41C5-AD14-BF4F4D8BDF34}"/>
+    <hyperlink ref="F16" r:id="rId83" xr:uid="{2D115D7B-5F56-4E0A-95AE-0F9322EF7834}"/>
+    <hyperlink ref="E14" r:id="rId84" xr:uid="{ABE8ED47-6F4D-4A6B-934E-EAF7F614157B}"/>
+    <hyperlink ref="E32" r:id="rId85" xr:uid="{A46821FE-B9E6-4DA6-86A1-423D6D8625C4}"/>
+    <hyperlink ref="E33" r:id="rId86" xr:uid="{26859566-EDF8-4D35-9633-DF0946322AF6}"/>
+    <hyperlink ref="E37" r:id="rId87" xr:uid="{7175EFCD-2552-4973-8B3D-95D63C9CD86F}"/>
+    <hyperlink ref="E47" r:id="rId88" xr:uid="{CD3C8CE1-4C32-462C-84A8-1E3130D1F63F}"/>
+    <hyperlink ref="E63" r:id="rId89" xr:uid="{654FB847-B1BF-4E9D-9F87-14D35D782BF2}"/>
+    <hyperlink ref="F63" r:id="rId90" xr:uid="{EEEC10BC-21C5-4BCA-A4F4-990220257200}"/>
+    <hyperlink ref="F14" r:id="rId91" xr:uid="{D298C803-0132-49F6-ABA7-54E1CA93013D}"/>
+    <hyperlink ref="F13" r:id="rId92" xr:uid="{44541484-41EC-488E-9C46-FD2985DEF367}"/>
+    <hyperlink ref="E13" r:id="rId93" xr:uid="{8BF2D71A-70CF-4CDE-BDBF-3033BB382FCF}"/>
+    <hyperlink ref="F12" r:id="rId94" xr:uid="{51B31C2E-3892-472A-913B-87FAC66C6F76}"/>
+    <hyperlink ref="E12" r:id="rId95" xr:uid="{5826D20D-02CD-4129-82AC-7314C8A1AEF7}"/>
+    <hyperlink ref="F26" r:id="rId96" xr:uid="{9B0E6E50-8807-4AC2-A155-706196529592}"/>
+    <hyperlink ref="E26" r:id="rId97" xr:uid="{717BD393-9CD1-456C-B170-0C0E0DE21984}"/>
+    <hyperlink ref="F53" r:id="rId98" xr:uid="{47A3461D-BB0E-485D-A69D-249CEFEFB2EA}"/>
+    <hyperlink ref="F8" r:id="rId99" xr:uid="{9193DF21-E100-42C4-BE99-FD9D65FAAB4A}"/>
+    <hyperlink ref="E8" r:id="rId100" xr:uid="{0529A15C-C3F2-4FE1-B402-51C24807BA8A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId84"/>
+  <pageSetup orientation="portrait" r:id="rId101"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated and added new worlds
</commit_message>
<xml_diff>
--- a/CustomWorldsInstalled.xlsx
+++ b/CustomWorldsInstalled.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\Git\Archipelago\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39B4AC8-BA3B-4EA6-BEC8-BEB28D935E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0CD892-810F-4E00-963F-954397B9D09E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9750" yWindow="21765" windowWidth="28800" windowHeight="15435" xr2:uid="{3DBB16FA-FE5F-4BB0-89C2-A45EA748065E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{3DBB16FA-FE5F-4BB0-89C2-A45EA748065E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="243">
   <si>
     <t>World</t>
   </si>
@@ -150,9 +150,6 @@
   </si>
   <si>
     <t>Jak and Daxter</t>
-  </si>
-  <si>
-    <t>0.1.1</t>
   </si>
   <si>
     <t>Fire Emblem 8</t>
@@ -526,9 +523,6 @@
     <t>0.5.2</t>
   </si>
   <si>
-    <t>0.6.4</t>
-  </si>
-  <si>
     <t>0.2.3</t>
   </si>
   <si>
@@ -566,9 +560,6 @@
   </si>
   <si>
     <t>Hades</t>
-  </si>
-  <si>
-    <t>0.13.0</t>
   </si>
   <si>
     <t>https://github.com/NaixGames/Polycosmos/releases</t>
@@ -620,9 +611,6 @@
     <t>0.6.5</t>
   </si>
   <si>
-    <t>3.0.2B</t>
-  </si>
-  <si>
     <t>Kingdom Hearts: BBS</t>
   </si>
   <si>
@@ -647,21 +635,9 @@
     <t>https://github.com/TheLX5/Archipelago/releases?q=%22Mega+Man+X3%22&amp;expanded=true</t>
   </si>
   <si>
-    <t>0.8.2</t>
-  </si>
-  <si>
     <t>1.0.3</t>
   </si>
   <si>
-    <t>0.6.0</t>
-  </si>
-  <si>
-    <t>0.8.0</t>
-  </si>
-  <si>
-    <t>0.1.9b</t>
-  </si>
-  <si>
     <t>Zelda II</t>
   </si>
   <si>
@@ -707,9 +683,6 @@
     <t>https://github.com/SerpentAI/Archipelago/releases?q=%22Keymaster%27s+Keep%22&amp;expanded=true</t>
   </si>
   <si>
-    <t>pre-6</t>
-  </si>
-  <si>
     <t>Shapez 2</t>
   </si>
   <si>
@@ -729,6 +702,72 @@
   </si>
   <si>
     <t>https://github.com/BlastSlimey/2hapezipelago/releases</t>
+  </si>
+  <si>
+    <t>0.3.2</t>
+  </si>
+  <si>
+    <t>0.9.0</t>
+  </si>
+  <si>
+    <t>0.1.9c</t>
+  </si>
+  <si>
+    <t>0.13.1</t>
+  </si>
+  <si>
+    <t>pre-8</t>
+  </si>
+  <si>
+    <t>0.8.4</t>
+  </si>
+  <si>
+    <t>0.6.1</t>
+  </si>
+  <si>
+    <t>1.1.0</t>
+  </si>
+  <si>
+    <t>Super Mario RPG</t>
+  </si>
+  <si>
+    <t>https://github.com/dontjoome/SMRPG_apworld/releases</t>
+  </si>
+  <si>
+    <t>https://discord.com/channels/731205301247803413/1091478379963883651</t>
+  </si>
+  <si>
+    <t>Jigsaw</t>
+  </si>
+  <si>
+    <t>0.0.3</t>
+  </si>
+  <si>
+    <t>https://github.com/spineraks-org/ArchipelagoJigsaw/releases</t>
+  </si>
+  <si>
+    <t>https://discord.com/channels/731205301247803413/1337582193802870907</t>
+  </si>
+  <si>
+    <t>Kirby Super Star</t>
+  </si>
+  <si>
+    <t>https://github.com/Silvris/Archipelago/releases?q=%22Kirby%20Super%20Star%22&amp;expanded=true</t>
+  </si>
+  <si>
+    <t>https://discord.com/channels/731205301247803413/1170152771043999764</t>
+  </si>
+  <si>
+    <t>Kirby 64 The Crystal Shards</t>
+  </si>
+  <si>
+    <t>0.1.4</t>
+  </si>
+  <si>
+    <t>https://github.com/Silvris/Archipelago/releases?q=Kirby+64&amp;expanded=true</t>
+  </si>
+  <si>
+    <t>https://discord.com/channels/731205301247803413/1175344681928904806</t>
   </si>
 </sst>
 </file>
@@ -805,7 +844,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -833,6 +872,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1176,11 +1218,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{901AF876-1585-4DEB-9BCA-32AAC89A46F9}">
-  <dimension ref="A1:O63"/>
+  <dimension ref="A1:O67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F63" sqref="F63"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1216,16 +1258,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>71</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>72</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>32</v>
       </c>
       <c r="O1" s="6">
-        <v>45675</v>
+        <v>45687</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -1247,10 +1289,10 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C3" s="4">
         <v>45646</v>
@@ -1259,78 +1301,78 @@
         <v>45675</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="C4" s="4">
+        <v>45697</v>
+      </c>
+      <c r="D4" s="4">
+        <v>45701</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="C4" s="4">
-        <v>45680</v>
-      </c>
-      <c r="D4" s="4">
-        <v>45687</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>159</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>206</v>
+        <v>223</v>
       </c>
       <c r="C5" s="4">
-        <v>45578</v>
+        <v>45699</v>
       </c>
       <c r="D5" s="4">
-        <v>45675</v>
+        <v>45701</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B6" s="3">
-        <v>4.0999999999999996</v>
+        <v>4.2</v>
       </c>
       <c r="C6" s="4">
-        <v>45668</v>
+        <v>45694</v>
       </c>
       <c r="D6" s="4">
-        <v>45675</v>
+        <v>45701</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C7" s="4">
         <v>45614</v>
@@ -1339,30 +1381,30 @@
         <v>45617</v>
       </c>
       <c r="E7" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>145</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="C8" s="11">
+        <v>219</v>
+      </c>
+      <c r="C8" s="13">
         <v>45684</v>
       </c>
       <c r="D8" s="4">
         <v>45687</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -1382,7 +1424,7 @@
         <v>29</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -1393,10 +1435,10 @@
         <v>45617</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -1404,7 +1446,7 @@
         <v>15</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C11" s="4">
         <v>45684</v>
@@ -1416,15 +1458,15 @@
         <v>20</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="C12" s="4">
         <v>45906</v>
@@ -1433,18 +1475,18 @@
         <v>45687</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="C13" s="4">
         <v>45588</v>
@@ -1453,18 +1495,18 @@
         <v>45687</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C14" s="4">
         <v>45673</v>
@@ -1473,38 +1515,38 @@
         <v>45687</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>193</v>
+        <v>48</v>
+      </c>
+      <c r="B15" s="3">
+        <v>3.1</v>
       </c>
       <c r="C15" s="4">
-        <v>45687</v>
+        <v>45694</v>
       </c>
       <c r="D15" s="4">
-        <v>45687</v>
+        <v>45701</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C16" s="4">
         <v>45532</v>
@@ -1513,15 +1555,15 @@
         <v>45675</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B17" s="3">
         <v>0.4</v>
@@ -1533,35 +1575,35 @@
         <v>45645</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C18" s="4">
+        <v>45688</v>
+      </c>
+      <c r="D18" s="4">
+        <v>45701</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C18" s="4">
-        <v>45673</v>
-      </c>
-      <c r="D18" s="4">
-        <v>45687</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>70</v>
-      </c>
       <c r="F18" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B19" s="3">
         <v>82.5</v>
@@ -1573,15 +1615,15 @@
         <v>45507</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C20" s="4">
         <v>45526</v>
@@ -1598,10 +1640,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C21" s="4">
         <v>45557</v>
@@ -1613,15 +1655,15 @@
         <v>21</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="C22" s="4">
         <v>45425</v>
@@ -1630,30 +1672,30 @@
         <v>45478</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="C23" s="4">
+        <v>45697</v>
+      </c>
+      <c r="D23" s="4">
+        <v>45701</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="F23" s="5" t="s">
         <v>175</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="C23" s="4">
-        <v>45646</v>
-      </c>
-      <c r="D23" s="4">
-        <v>45675</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1661,7 +1703,7 @@
         <v>13</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C24" s="4">
         <v>45542</v>
@@ -1673,7 +1715,7 @@
         <v>17</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1681,7 +1723,7 @@
         <v>37</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C25" s="4">
         <v>45618</v>
@@ -1693,35 +1735,35 @@
         <v>36</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C26" s="4">
-        <v>45682</v>
+        <v>45694</v>
       </c>
       <c r="D26" s="4">
-        <v>45687</v>
+        <v>45701</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C27" s="4">
         <v>45555</v>
@@ -1730,18 +1772,18 @@
         <v>45562</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C28" s="4">
         <v>45516</v>
@@ -1753,32 +1795,32 @@
         <v>22</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" s="4">
+        <v>45694</v>
+      </c>
+      <c r="D29" s="4">
+        <v>45701</v>
+      </c>
+      <c r="E29" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C29" s="4">
-        <v>45527</v>
-      </c>
-      <c r="D29" s="4">
-        <v>45547</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>74</v>
-      </c>
       <c r="F29" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B30" s="3">
         <v>11.1</v>
@@ -1790,18 +1832,18 @@
         <v>45687</v>
       </c>
       <c r="E30" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>156</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>80</v>
       </c>
       <c r="C31" s="4">
         <v>45528</v>
@@ -1810,18 +1852,18 @@
         <v>45562</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C32" s="4">
         <v>45555</v>
@@ -1830,18 +1872,18 @@
         <v>45562</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C33" s="4">
         <v>45527</v>
@@ -1850,18 +1892,18 @@
         <v>45562</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C34" s="4">
         <v>45623</v>
@@ -1870,18 +1912,18 @@
         <v>45675</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C35" s="4">
         <v>45674</v>
@@ -1890,18 +1932,18 @@
         <v>45675</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C36" s="4">
         <v>45631</v>
@@ -1910,30 +1952,30 @@
         <v>45632</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37" s="4">
+        <v>45688</v>
+      </c>
+      <c r="D37" s="4">
+        <v>45701</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="F37" s="5" t="s">
         <v>171</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C37" s="4">
-        <v>45671</v>
-      </c>
-      <c r="D37" s="4">
-        <v>45675</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1941,7 +1983,7 @@
         <v>8</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C38" s="4">
         <v>45626</v>
@@ -1953,15 +1995,15 @@
         <v>18</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>51</v>
+        <v>221</v>
       </c>
       <c r="C39" s="4">
         <v>45683</v>
@@ -1970,10 +2012,10 @@
         <v>45687</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1993,15 +2035,15 @@
         <v>23</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C41" s="4">
         <v>45646</v>
@@ -2010,10 +2052,10 @@
         <v>45675</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -2021,7 +2063,7 @@
         <v>34</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C42" s="4">
         <v>45646</v>
@@ -2033,7 +2075,7 @@
         <v>35</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -2055,10 +2097,10 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C44" s="4">
         <v>45488</v>
@@ -2067,30 +2109,30 @@
         <v>45519</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="C45" s="4">
+        <v>45694</v>
+      </c>
+      <c r="D45" s="4">
+        <v>45701</v>
+      </c>
+      <c r="E45" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B45" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="C45" s="4">
-        <v>45683</v>
-      </c>
-      <c r="D45" s="4">
-        <v>45687</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>57</v>
-      </c>
       <c r="F45" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -2107,35 +2149,35 @@
         <v>19</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>167</v>
+        <v>74</v>
       </c>
       <c r="C47" s="4">
-        <v>45674</v>
+        <v>45694</v>
       </c>
       <c r="D47" s="4">
-        <v>45675</v>
+        <v>45701</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C48" s="4">
         <v>45568</v>
@@ -2144,18 +2186,18 @@
         <v>45575</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C49" s="4">
         <v>45680</v>
@@ -2164,18 +2206,18 @@
         <v>45687</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C50" s="4">
         <v>45638</v>
@@ -2184,10 +2226,10 @@
         <v>45675</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -2195,7 +2237,7 @@
         <v>11</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C51" s="4">
         <v>45646</v>
@@ -2207,72 +2249,72 @@
         <v>27</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C52" s="4">
+        <v>45688</v>
+      </c>
+      <c r="D52" s="4">
+        <v>45701</v>
+      </c>
+      <c r="E52" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B52" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="C52" s="4">
-        <v>45682</v>
-      </c>
-      <c r="D52" s="4">
-        <v>45687</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="F52" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="C53" s="4">
         <v>45656</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="C54" s="4">
+        <v>45699</v>
+      </c>
+      <c r="D54" s="4">
+        <v>45701</v>
+      </c>
+      <c r="E54" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B54" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C54" s="4">
-        <v>45674</v>
-      </c>
-      <c r="D54" s="4">
-        <v>45675</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>78</v>
-      </c>
       <c r="F54" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>135</v>
       </c>
       <c r="C55" s="4">
         <v>45518</v>
@@ -2281,18 +2323,18 @@
         <v>45575</v>
       </c>
       <c r="E55" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="F55" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C56" s="4">
         <v>45597</v>
@@ -2301,10 +2343,10 @@
         <v>45603</v>
       </c>
       <c r="E56" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="F56" s="5" t="s">
         <v>128</v>
-      </c>
-      <c r="F56" s="5" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -2329,17 +2371,17 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C58" s="4"/>
       <c r="D58" s="4">
         <v>45519</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -2347,7 +2389,7 @@
         <v>12</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C59" s="4">
         <v>45579</v>
@@ -2364,10 +2406,10 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C60" s="4">
         <v>45611</v>
@@ -2376,18 +2418,18 @@
         <v>45617</v>
       </c>
       <c r="E60" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="F60" s="5" t="s">
         <v>147</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C61" s="4">
         <v>45661</v>
@@ -2396,18 +2438,18 @@
         <v>45675</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B62" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>139</v>
       </c>
       <c r="C62" s="4">
         <v>45530</v>
@@ -2416,15 +2458,15 @@
         <v>45575</v>
       </c>
       <c r="E62" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F62" s="5" t="s">
         <v>140</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="B63" s="3">
         <v>1</v>
@@ -2436,10 +2478,90 @@
         <v>45687</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>209</v>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C64" s="4">
+        <v>45698</v>
+      </c>
+      <c r="D64" s="4">
+        <v>45701</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="C65" s="4">
+        <v>45699</v>
+      </c>
+      <c r="D65" s="4">
+        <v>45701</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C66" s="4">
+        <v>45694</v>
+      </c>
+      <c r="D66" s="4">
+        <v>45701</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C67" s="4">
+        <v>45640</v>
+      </c>
+      <c r="D67" s="4">
+        <v>45701</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -2552,8 +2674,16 @@
     <hyperlink ref="F53" r:id="rId98" xr:uid="{47A3461D-BB0E-485D-A69D-249CEFEFB2EA}"/>
     <hyperlink ref="F8" r:id="rId99" xr:uid="{9193DF21-E100-42C4-BE99-FD9D65FAAB4A}"/>
     <hyperlink ref="E8" r:id="rId100" xr:uid="{0529A15C-C3F2-4FE1-B402-51C24807BA8A}"/>
+    <hyperlink ref="E64" r:id="rId101" xr:uid="{5EEE8774-5BFE-4091-8D5B-AECA259D6AC7}"/>
+    <hyperlink ref="F64" r:id="rId102" xr:uid="{5BC10617-F8EE-400C-BDC5-07113421E148}"/>
+    <hyperlink ref="E65" r:id="rId103" xr:uid="{6F5DEAF7-DD57-4D97-B227-F245CE16EAEB}"/>
+    <hyperlink ref="F65" r:id="rId104" xr:uid="{F84F7FA1-A12B-4794-8B3A-2C84C6A0C78D}"/>
+    <hyperlink ref="E66" r:id="rId105" xr:uid="{2F675965-8E88-4605-9B06-9379AFD65861}"/>
+    <hyperlink ref="F66" r:id="rId106" xr:uid="{07818C94-99C0-4FA9-AB24-BA30A4D6874F}"/>
+    <hyperlink ref="E67" r:id="rId107" xr:uid="{B74BD8C3-4C40-406B-AECA-E72A9F2219F0}"/>
+    <hyperlink ref="F67" r:id="rId108" xr:uid="{301AE9A9-71A3-4FD6-8723-DCA05CE807B9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId101"/>
+  <pageSetup orientation="portrait" r:id="rId109"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated and added new worlds. Starting plotting hooks for shared hint system when not using room hints. Fixed issue with ALttp not hashing properly.
</commit_message>
<xml_diff>
--- a/CustomWorldsInstalled.xlsx
+++ b/CustomWorldsInstalled.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\Git\Archipelago\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0CD892-810F-4E00-963F-954397B9D09E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC396B8-65E7-497D-A57B-D2E9B2AA6346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{3DBB16FA-FE5F-4BB0-89C2-A45EA748065E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="247">
   <si>
     <t>World</t>
   </si>
@@ -493,9 +493,6 @@
     <t>1.1.2</t>
   </si>
   <si>
-    <t>0.4.1</t>
-  </si>
-  <si>
     <t>0.6.6</t>
   </si>
   <si>
@@ -710,21 +707,9 @@
     <t>0.9.0</t>
   </si>
   <si>
-    <t>0.1.9c</t>
-  </si>
-  <si>
     <t>0.13.1</t>
   </si>
   <si>
-    <t>pre-8</t>
-  </si>
-  <si>
-    <t>0.8.4</t>
-  </si>
-  <si>
-    <t>0.6.1</t>
-  </si>
-  <si>
     <t>1.1.0</t>
   </si>
   <si>
@@ -768,6 +753,33 @@
   </si>
   <si>
     <t>https://discord.com/channels/731205301247803413/1175344681928904806</t>
+  </si>
+  <si>
+    <t>0.1.9d</t>
+  </si>
+  <si>
+    <t>0.5.1</t>
+  </si>
+  <si>
+    <t>pre-9</t>
+  </si>
+  <si>
+    <t>0.8.5</t>
+  </si>
+  <si>
+    <t>0.6.2</t>
+  </si>
+  <si>
+    <t>0.0.4</t>
+  </si>
+  <si>
+    <t>Rift of the NecroDancer</t>
+  </si>
+  <si>
+    <t>https://github.com/studkid/RiftArchipelago/releases</t>
+  </si>
+  <si>
+    <t>https://discord.com/channels/731205301247803413/1337112354130759757</t>
   </si>
 </sst>
 </file>
@@ -844,7 +856,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -875,6 +887,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1218,11 +1231,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{901AF876-1585-4DEB-9BCA-32AAC89A46F9}">
-  <dimension ref="A1:O67"/>
+  <dimension ref="A1:O68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F68" sqref="F68"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1267,7 +1280,7 @@
         <v>32</v>
       </c>
       <c r="O1" s="6">
-        <v>45687</v>
+        <v>45701</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -1292,7 +1305,7 @@
         <v>49</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C3" s="4">
         <v>45646</v>
@@ -1309,10 +1322,10 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C4" s="4">
         <v>45697</v>
@@ -1321,35 +1334,35 @@
         <v>45701</v>
       </c>
       <c r="E4" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>158</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="C5" s="4">
+        <v>45706</v>
+      </c>
+      <c r="D5" s="4">
+        <v>45713</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="C5" s="4">
-        <v>45699</v>
-      </c>
-      <c r="D5" s="4">
-        <v>45701</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>177</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B6" s="3">
         <v>4.2</v>
@@ -1361,10 +1374,10 @@
         <v>45701</v>
       </c>
       <c r="E6" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>167</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1389,10 +1402,10 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C8" s="13">
         <v>45684</v>
@@ -1401,10 +1414,10 @@
         <v>45687</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -1446,13 +1459,13 @@
         <v>15</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>189</v>
+        <v>151</v>
       </c>
       <c r="C11" s="4">
-        <v>45684</v>
+        <v>45706</v>
       </c>
       <c r="D11" s="4">
-        <v>45687</v>
+        <v>45713</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>20</v>
@@ -1463,10 +1476,10 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>208</v>
       </c>
       <c r="C12" s="4">
         <v>45906</v>
@@ -1475,18 +1488,18 @@
         <v>45687</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C13" s="4">
         <v>45588</v>
@@ -1495,18 +1508,18 @@
         <v>45687</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>192</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>193</v>
       </c>
       <c r="C14" s="4">
         <v>45673</v>
@@ -1515,10 +1528,10 @@
         <v>45687</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -1526,13 +1539,13 @@
         <v>48</v>
       </c>
       <c r="B15" s="3">
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
       <c r="C15" s="4">
-        <v>45694</v>
+        <v>45706</v>
       </c>
       <c r="D15" s="4">
-        <v>45701</v>
+        <v>45713</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>59</v>
@@ -1543,10 +1556,10 @@
     </row>
     <row r="16" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C16" s="4">
         <v>45532</v>
@@ -1555,10 +1568,10 @@
         <v>45675</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1586,7 +1599,7 @@
         <v>68</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C18" s="4">
         <v>45688</v>
@@ -1680,10 +1693,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C23" s="4">
         <v>45697</v>
@@ -1692,10 +1705,10 @@
         <v>45701</v>
       </c>
       <c r="E23" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="F23" s="5" t="s">
         <v>174</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1723,13 +1736,13 @@
         <v>37</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>151</v>
+        <v>239</v>
       </c>
       <c r="C25" s="4">
-        <v>45618</v>
+        <v>45710</v>
       </c>
       <c r="D25" s="4">
-        <v>45632</v>
+        <v>45713</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>36</v>
@@ -1740,833 +1753,853 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>211</v>
+        <v>227</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>225</v>
+        <v>134</v>
       </c>
       <c r="C26" s="4">
-        <v>45694</v>
+        <v>45706</v>
       </c>
       <c r="D26" s="4">
-        <v>45701</v>
+        <v>45713</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>213</v>
+        <v>229</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>212</v>
+        <v>230</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>75</v>
+        <v>240</v>
       </c>
       <c r="C27" s="4">
-        <v>45555</v>
+        <v>45702</v>
       </c>
       <c r="D27" s="4">
-        <v>45562</v>
+        <v>45713</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>42</v>
+        <v>212</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>115</v>
+        <v>211</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="C28" s="4">
-        <v>45516</v>
+        <v>45555</v>
       </c>
       <c r="D28" s="4">
-        <v>45519</v>
+        <v>45562</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>72</v>
+        <v>190</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="C29" s="4">
-        <v>45694</v>
+        <v>45516</v>
       </c>
       <c r="D29" s="4">
-        <v>45701</v>
+        <v>45519</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="B30" s="3">
-        <v>11.1</v>
+        <v>234</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>235</v>
       </c>
       <c r="C30" s="4">
-        <v>45683</v>
+        <v>45640</v>
       </c>
       <c r="D30" s="4">
-        <v>45687</v>
+        <v>45701</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>155</v>
+        <v>236</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>156</v>
+        <v>237</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
-        <v>78</v>
+        <v>231</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>79</v>
+        <v>228</v>
       </c>
       <c r="C31" s="4">
-        <v>45528</v>
+        <v>45709</v>
       </c>
       <c r="D31" s="4">
-        <v>45562</v>
+        <v>45713</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>195</v>
+        <v>232</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>94</v>
+        <v>233</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C32" s="4">
-        <v>45555</v>
+        <v>45694</v>
       </c>
       <c r="D32" s="4">
-        <v>45562</v>
+        <v>45701</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>196</v>
+        <v>73</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>79</v>
+        <v>152</v>
+      </c>
+      <c r="B33" s="3">
+        <v>11.4</v>
       </c>
       <c r="C33" s="4">
-        <v>45527</v>
+        <v>45713</v>
       </c>
       <c r="D33" s="4">
-        <v>45562</v>
+        <v>45713</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>197</v>
+        <v>154</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>121</v>
+        <v>155</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>179</v>
+        <v>78</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>180</v>
+        <v>79</v>
       </c>
       <c r="C34" s="4">
-        <v>45623</v>
+        <v>45528</v>
       </c>
       <c r="D34" s="4">
-        <v>45675</v>
+        <v>45562</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>181</v>
+        <v>194</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>182</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>161</v>
+        <v>82</v>
       </c>
       <c r="C35" s="4">
-        <v>45674</v>
+        <v>45555</v>
       </c>
       <c r="D35" s="4">
-        <v>45675</v>
+        <v>45562</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>66</v>
+        <v>195</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="C36" s="4">
-        <v>45631</v>
+        <v>45527</v>
       </c>
       <c r="D36" s="4">
-        <v>45632</v>
+        <v>45562</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>65</v>
+        <v>196</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>50</v>
+        <v>179</v>
       </c>
       <c r="C37" s="4">
-        <v>45688</v>
+        <v>45623</v>
       </c>
       <c r="D37" s="4">
-        <v>45701</v>
+        <v>45675</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="C38" s="4">
-        <v>45626</v>
+        <v>45674</v>
       </c>
       <c r="D38" s="4">
-        <v>45632</v>
+        <v>45675</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>221</v>
+        <v>50</v>
       </c>
       <c r="C39" s="4">
-        <v>45683</v>
+        <v>45631</v>
       </c>
       <c r="D39" s="4">
-        <v>45687</v>
+        <v>45632</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>131</v>
+        <v>65</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B40" s="3">
-        <v>8</v>
+        <v>168</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>220</v>
       </c>
       <c r="C40" s="4">
-        <v>45683</v>
+        <v>45712</v>
       </c>
       <c r="D40" s="4">
-        <v>45687</v>
+        <v>45713</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>23</v>
+        <v>169</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>89</v>
+        <v>170</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="C41" s="4">
-        <v>45646</v>
+        <v>45626</v>
       </c>
       <c r="D41" s="4">
-        <v>45675</v>
+        <v>45632</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>163</v>
+        <v>220</v>
       </c>
       <c r="C42" s="4">
-        <v>45646</v>
+        <v>45683</v>
       </c>
       <c r="D42" s="4">
-        <v>45675</v>
+        <v>45687</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>35</v>
+        <v>131</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
-        <v>10</v>
+        <v>6</v>
+      </c>
+      <c r="B43" s="3">
+        <v>8</v>
       </c>
       <c r="C43" s="4">
-        <v>45317</v>
+        <v>45683</v>
       </c>
       <c r="D43" s="4">
-        <v>45422</v>
+        <v>45687</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>26</v>
+        <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>54</v>
+        <v>161</v>
       </c>
       <c r="C44" s="4">
-        <v>45488</v>
+        <v>45646</v>
       </c>
       <c r="D44" s="4">
-        <v>45519</v>
+        <v>45675</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>226</v>
+        <v>162</v>
       </c>
       <c r="C45" s="4">
-        <v>45694</v>
+        <v>45646</v>
       </c>
       <c r="D45" s="4">
-        <v>45701</v>
+        <v>45675</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
+      </c>
+      <c r="C46" s="4">
+        <v>45317</v>
       </c>
       <c r="D46" s="4">
         <v>45422</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>100</v>
+        <v>26</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
-        <v>183</v>
+        <v>52</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="C47" s="4">
-        <v>45694</v>
+        <v>45488</v>
       </c>
       <c r="D47" s="4">
-        <v>45701</v>
+        <v>45519</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>184</v>
+        <v>53</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>185</v>
+        <v>92</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>125</v>
+        <v>241</v>
       </c>
       <c r="C48" s="4">
-        <v>45568</v>
+        <v>45710</v>
       </c>
       <c r="D48" s="4">
-        <v>45575</v>
+        <v>45713</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
-        <v>62</v>
+        <v>9</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="C49" s="4">
-        <v>45680</v>
+        <v>14</v>
       </c>
       <c r="D49" s="4">
-        <v>45687</v>
+        <v>45422</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
-        <v>96</v>
+        <v>182</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>164</v>
+        <v>239</v>
       </c>
       <c r="C50" s="4">
-        <v>45638</v>
+        <v>45706</v>
       </c>
       <c r="D50" s="4">
-        <v>45675</v>
+        <v>45713</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>142</v>
+        <v>183</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>97</v>
+        <v>184</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>165</v>
+        <v>125</v>
       </c>
       <c r="C51" s="4">
-        <v>45646</v>
+        <v>45568</v>
       </c>
       <c r="D51" s="4">
-        <v>45675</v>
+        <v>45575</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>129</v>
+        <v>93</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>227</v>
+        <v>197</v>
       </c>
       <c r="C52" s="4">
-        <v>45688</v>
+        <v>45680</v>
       </c>
       <c r="D52" s="4">
-        <v>45701</v>
+        <v>45687</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
-        <v>214</v>
+        <v>96</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>208</v>
+        <v>163</v>
       </c>
       <c r="C53" s="4">
-        <v>45656</v>
+        <v>45638</v>
+      </c>
+      <c r="D53" s="4">
+        <v>45675</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>220</v>
+        <v>142</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>215</v>
+        <v>97</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
-        <v>76</v>
+        <v>11</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>228</v>
+        <v>164</v>
       </c>
       <c r="C54" s="4">
-        <v>45699</v>
+        <v>45646</v>
       </c>
       <c r="D54" s="4">
-        <v>45701</v>
+        <v>45675</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>102</v>
+        <v>129</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
-        <v>133</v>
+        <v>57</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>134</v>
+        <v>242</v>
       </c>
       <c r="C55" s="4">
-        <v>45518</v>
+        <v>45706</v>
       </c>
       <c r="D55" s="4">
-        <v>45575</v>
+        <v>45713</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>135</v>
+        <v>58</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
-        <v>126</v>
+        <v>213</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>75</v>
+        <v>207</v>
       </c>
       <c r="C56" s="4">
-        <v>45597</v>
-      </c>
-      <c r="D56" s="4">
-        <v>45603</v>
+        <v>45656</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>127</v>
+        <v>219</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>128</v>
+        <v>214</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
-        <v>4</v>
+        <v>76</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>24</v>
+        <v>223</v>
       </c>
       <c r="C57" s="4">
-        <v>45442</v>
+        <v>45706</v>
       </c>
       <c r="D57" s="4">
-        <v>45447</v>
+        <v>45713</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>25</v>
+        <v>77</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>25</v>
+        <v>102</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C58" s="4"/>
+        <v>133</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C58" s="4">
+        <v>45518</v>
+      </c>
       <c r="D58" s="4">
-        <v>45519</v>
+        <v>45575</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>47</v>
+        <v>135</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>47</v>
+        <v>136</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
-        <v>12</v>
+        <v>126</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>150</v>
+        <v>75</v>
       </c>
       <c r="C59" s="4">
-        <v>45579</v>
+        <v>45597</v>
       </c>
       <c r="D59" s="4">
-        <v>45617</v>
+        <v>45603</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>28</v>
+        <v>127</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>28</v>
+        <v>128</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
-        <v>148</v>
+        <v>224</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>141</v>
+        <v>243</v>
       </c>
       <c r="C60" s="4">
-        <v>45611</v>
+        <v>45706</v>
       </c>
       <c r="D60" s="4">
-        <v>45617</v>
+        <v>45713</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>146</v>
+        <v>225</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>147</v>
+        <v>226</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
-        <v>108</v>
+        <v>4</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>166</v>
+        <v>24</v>
       </c>
       <c r="C61" s="4">
-        <v>45661</v>
+        <v>45442</v>
       </c>
       <c r="D61" s="4">
-        <v>45675</v>
+        <v>45447</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>132</v>
+        <v>25</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>109</v>
+        <v>25</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C62" s="4">
-        <v>45530</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="C62" s="4"/>
       <c r="D62" s="4">
-        <v>45575</v>
+        <v>45519</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>139</v>
+        <v>47</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>140</v>
+        <v>47</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="B63" s="3">
-        <v>1</v>
+        <v>12</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>150</v>
       </c>
       <c r="C63" s="4">
-        <v>45680</v>
+        <v>45579</v>
       </c>
       <c r="D63" s="4">
-        <v>45687</v>
+        <v>45617</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>200</v>
+        <v>28</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>201</v>
+        <v>28</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
-        <v>229</v>
+        <v>148</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>141</v>
       </c>
       <c r="C64" s="4">
-        <v>45698</v>
+        <v>45611</v>
       </c>
       <c r="D64" s="4">
-        <v>45701</v>
+        <v>45617</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>230</v>
+        <v>146</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>231</v>
+        <v>147</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
-        <v>232</v>
+        <v>108</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>233</v>
+        <v>165</v>
       </c>
       <c r="C65" s="4">
-        <v>45699</v>
+        <v>45661</v>
       </c>
       <c r="D65" s="4">
-        <v>45701</v>
+        <v>45675</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>234</v>
+        <v>132</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>235</v>
+        <v>109</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
-        <v>236</v>
+        <v>137</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C66" s="4">
-        <v>45694</v>
+        <v>45530</v>
       </c>
       <c r="D66" s="4">
-        <v>45701</v>
+        <v>45575</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>237</v>
+        <v>139</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>238</v>
+        <v>140</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
-        <v>239</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>240</v>
+        <v>198</v>
+      </c>
+      <c r="B67" s="3">
+        <v>1</v>
       </c>
       <c r="C67" s="4">
-        <v>45640</v>
+        <v>45680</v>
       </c>
       <c r="D67" s="4">
-        <v>45701</v>
+        <v>45687</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>241</v>
+        <v>199</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>242</v>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C68" s="4">
+        <v>45711</v>
+      </c>
+      <c r="D68" s="14">
+        <v>45713</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>246</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F63">
-    <sortCondition ref="A2:A63"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F67">
+    <sortCondition ref="A2:A67"/>
   </sortState>
   <conditionalFormatting sqref="A2:XFD132">
     <cfRule type="expression" dxfId="0" priority="2">
@@ -2574,78 +2607,78 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E38" r:id="rId1" xr:uid="{A5B7ED1F-2322-489C-9115-C445E82B54FB}"/>
-    <hyperlink ref="E28" r:id="rId2" xr:uid="{90F7D550-3232-4E6C-9AB7-856BDF3EA309}"/>
+    <hyperlink ref="E41" r:id="rId1" xr:uid="{A5B7ED1F-2322-489C-9115-C445E82B54FB}"/>
+    <hyperlink ref="E29" r:id="rId2" xr:uid="{90F7D550-3232-4E6C-9AB7-856BDF3EA309}"/>
     <hyperlink ref="E24" r:id="rId3" xr:uid="{5D7F93FB-6C49-403A-9AD8-F4281B6B2D94}"/>
     <hyperlink ref="E19" r:id="rId4" display="https://github.com/cleartonic/arch_ffvcd/releases" xr:uid="{8C8885B9-A3DC-40DD-B18B-F3B348BB2202}"/>
     <hyperlink ref="E21" r:id="rId5" xr:uid="{EC4A68ED-DCD0-44C0-9669-EAC47138143B}"/>
     <hyperlink ref="E11" r:id="rId6" xr:uid="{2531395D-2F00-44AD-B326-97CA7E60977D}"/>
     <hyperlink ref="E10" r:id="rId7" display="https://wiki.ctjot.com/doku.php?id=multiworld" xr:uid="{A1F02D1E-D96D-4326-BAA2-C7F18AF552BF}"/>
-    <hyperlink ref="E46" r:id="rId8" xr:uid="{39C13D86-F950-4EA9-AD8E-0CD6464A6C33}"/>
-    <hyperlink ref="E57" r:id="rId9" xr:uid="{AB23B92F-9660-4602-A770-B4DC053103FF}"/>
-    <hyperlink ref="E43" r:id="rId10" xr:uid="{AE8D7F00-E698-4DC8-8467-18A519416BF0}"/>
-    <hyperlink ref="E51" r:id="rId11" xr:uid="{2C45B0C7-121E-4FEE-90E6-19A508CC0856}"/>
-    <hyperlink ref="E59" r:id="rId12" xr:uid="{73DD7FA1-8A09-481E-9BF0-EDD88E86EAC3}"/>
+    <hyperlink ref="E49" r:id="rId8" xr:uid="{39C13D86-F950-4EA9-AD8E-0CD6464A6C33}"/>
+    <hyperlink ref="E61" r:id="rId9" xr:uid="{AB23B92F-9660-4602-A770-B4DC053103FF}"/>
+    <hyperlink ref="E46" r:id="rId10" xr:uid="{AE8D7F00-E698-4DC8-8467-18A519416BF0}"/>
+    <hyperlink ref="E54" r:id="rId11" xr:uid="{2C45B0C7-121E-4FEE-90E6-19A508CC0856}"/>
+    <hyperlink ref="E63" r:id="rId12" xr:uid="{73DD7FA1-8A09-481E-9BF0-EDD88E86EAC3}"/>
     <hyperlink ref="E9" r:id="rId13" xr:uid="{B7739609-1510-4E1E-B8C4-81240570A0B0}"/>
     <hyperlink ref="E20" r:id="rId14" xr:uid="{9D4D35EE-2216-4D82-ABE0-0760E544D7F3}"/>
     <hyperlink ref="E3" r:id="rId15" xr:uid="{BF5E4EB1-198E-4E95-86E7-1EF1374FF963}"/>
-    <hyperlink ref="E42" r:id="rId16" xr:uid="{15529467-5046-410B-9B6C-654495986B9C}"/>
+    <hyperlink ref="E45" r:id="rId16" xr:uid="{15529467-5046-410B-9B6C-654495986B9C}"/>
     <hyperlink ref="E25" r:id="rId17" xr:uid="{65E5E7CE-44B2-4FB0-BD3D-351DBED5A38A}"/>
     <hyperlink ref="E22" r:id="rId18" xr:uid="{75A12DC5-3325-4C7B-9F69-1A0B70EF2357}"/>
     <hyperlink ref="E2" r:id="rId19" xr:uid="{6A5A7183-040B-4C7C-A5E8-B8E3C0F52BCD}"/>
     <hyperlink ref="E15" r:id="rId20" xr:uid="{C789739C-B0F4-4CB3-956F-269CAF2DFC8D}"/>
-    <hyperlink ref="E54" r:id="rId21" xr:uid="{A8E1490C-983B-4622-8DC5-5563FB81C76C}"/>
-    <hyperlink ref="E62" r:id="rId22" xr:uid="{DB56F6A2-172B-4E4C-8A53-CBAD5AE6BAAB}"/>
+    <hyperlink ref="E57" r:id="rId21" xr:uid="{A8E1490C-983B-4622-8DC5-5563FB81C76C}"/>
+    <hyperlink ref="E66" r:id="rId22" xr:uid="{DB56F6A2-172B-4E4C-8A53-CBAD5AE6BAAB}"/>
     <hyperlink ref="F2" r:id="rId23" xr:uid="{20EB67DC-FC82-4F1A-9B75-CBF513D8DE4E}"/>
-    <hyperlink ref="F57" r:id="rId24" xr:uid="{73781179-C544-4054-952B-FA4211662F26}"/>
-    <hyperlink ref="F59" r:id="rId25" xr:uid="{E86B653A-32F2-4FF7-91A8-FCB34C0FF2C2}"/>
+    <hyperlink ref="F61" r:id="rId24" xr:uid="{73781179-C544-4054-952B-FA4211662F26}"/>
+    <hyperlink ref="F63" r:id="rId25" xr:uid="{E86B653A-32F2-4FF7-91A8-FCB34C0FF2C2}"/>
     <hyperlink ref="F17" r:id="rId26" xr:uid="{02494919-717B-478B-B79A-AE4E30A28014}"/>
-    <hyperlink ref="F29" r:id="rId27" xr:uid="{632AD9BE-E9BA-4153-995B-F235523DEE74}"/>
-    <hyperlink ref="F40" r:id="rId28" xr:uid="{7DBCE998-F80D-4D11-B542-1A4709AE8490}"/>
-    <hyperlink ref="F39" r:id="rId29" xr:uid="{5D0C808C-7E89-43C9-A13D-EED2709CC1D7}"/>
-    <hyperlink ref="F44" r:id="rId30" xr:uid="{64C3416A-7C81-40DD-BC58-E6E2E34EA840}"/>
-    <hyperlink ref="F48" r:id="rId31" xr:uid="{BAAE57A6-92DF-4790-90A3-C20208627A9C}"/>
-    <hyperlink ref="F31" r:id="rId32" xr:uid="{AF726EF3-BA18-451C-8E63-28F5F4EA1FC9}"/>
-    <hyperlink ref="F42" r:id="rId33" xr:uid="{AE1B5F2A-8864-4E2F-976A-CE56ADD6F999}"/>
-    <hyperlink ref="F50" r:id="rId34" xr:uid="{C8E38BF7-6188-48AC-A664-93E9163A8930}"/>
+    <hyperlink ref="F32" r:id="rId27" xr:uid="{632AD9BE-E9BA-4153-995B-F235523DEE74}"/>
+    <hyperlink ref="F43" r:id="rId28" xr:uid="{7DBCE998-F80D-4D11-B542-1A4709AE8490}"/>
+    <hyperlink ref="F42" r:id="rId29" xr:uid="{5D0C808C-7E89-43C9-A13D-EED2709CC1D7}"/>
+    <hyperlink ref="F47" r:id="rId30" xr:uid="{64C3416A-7C81-40DD-BC58-E6E2E34EA840}"/>
+    <hyperlink ref="F51" r:id="rId31" xr:uid="{BAAE57A6-92DF-4790-90A3-C20208627A9C}"/>
+    <hyperlink ref="F34" r:id="rId32" xr:uid="{AF726EF3-BA18-451C-8E63-28F5F4EA1FC9}"/>
+    <hyperlink ref="F45" r:id="rId33" xr:uid="{AE1B5F2A-8864-4E2F-976A-CE56ADD6F999}"/>
+    <hyperlink ref="F53" r:id="rId34" xr:uid="{C8E38BF7-6188-48AC-A664-93E9163A8930}"/>
     <hyperlink ref="F21" r:id="rId35" xr:uid="{994E4A5D-DC36-473B-9922-C223D8B30D3B}"/>
     <hyperlink ref="F15" r:id="rId36" xr:uid="{D3D17A4B-395F-4F48-A33C-49AC6AA8E1E4}"/>
-    <hyperlink ref="F46" r:id="rId37" xr:uid="{E5B6EC13-EF0E-494F-8472-535EF67D8363}"/>
+    <hyperlink ref="F49" r:id="rId37" xr:uid="{E5B6EC13-EF0E-494F-8472-535EF67D8363}"/>
     <hyperlink ref="F25" r:id="rId38" xr:uid="{2420FD62-4E63-4C9C-BE75-6AFA574DD4FA}"/>
-    <hyperlink ref="F54" r:id="rId39" xr:uid="{606EF7C0-92E0-4433-9350-F0BD9155211D}"/>
-    <hyperlink ref="F28" r:id="rId40" xr:uid="{E24CEC8F-56F5-44DD-8ED0-C170E20F245E}"/>
+    <hyperlink ref="F57" r:id="rId39" xr:uid="{606EF7C0-92E0-4433-9350-F0BD9155211D}"/>
+    <hyperlink ref="F29" r:id="rId40" xr:uid="{E24CEC8F-56F5-44DD-8ED0-C170E20F245E}"/>
     <hyperlink ref="F19" r:id="rId41" xr:uid="{CC7B146B-DFA0-437C-BD1C-353C0E3A04D8}"/>
-    <hyperlink ref="F45" r:id="rId42" xr:uid="{E1771B7F-29FC-44FD-89DE-44BF99EEAF8F}"/>
+    <hyperlink ref="F48" r:id="rId42" xr:uid="{E1771B7F-29FC-44FD-89DE-44BF99EEAF8F}"/>
     <hyperlink ref="F3" r:id="rId43" xr:uid="{8894D3F4-C9DD-4F73-B8D1-80EDE63AE046}"/>
     <hyperlink ref="F20" r:id="rId44" xr:uid="{E6A676E9-77F9-4254-821A-7039857E625D}"/>
-    <hyperlink ref="F36" r:id="rId45" xr:uid="{03AEB7E0-B241-406C-88D9-A0F51076BEFC}"/>
-    <hyperlink ref="F41" r:id="rId46" xr:uid="{56FA5804-441B-4115-81F2-E6F57B48EEB0}"/>
+    <hyperlink ref="F39" r:id="rId45" xr:uid="{03AEB7E0-B241-406C-88D9-A0F51076BEFC}"/>
+    <hyperlink ref="F44" r:id="rId46" xr:uid="{56FA5804-441B-4115-81F2-E6F57B48EEB0}"/>
     <hyperlink ref="F11" r:id="rId47" xr:uid="{CD854081-ECE1-4806-B8AA-BFE6EA05BB4B}"/>
-    <hyperlink ref="F49" r:id="rId48" xr:uid="{330B2B26-05E9-4ABC-ABA3-42999D67AAE8}"/>
+    <hyperlink ref="F52" r:id="rId48" xr:uid="{330B2B26-05E9-4ABC-ABA3-42999D67AAE8}"/>
     <hyperlink ref="F9" r:id="rId49" xr:uid="{34A7DD68-4900-4D76-B1DC-EBBDA4A2B1A6}"/>
-    <hyperlink ref="F35" r:id="rId50" xr:uid="{2C0DFA88-75D9-4BB4-A9EE-449C4C108A11}"/>
-    <hyperlink ref="F27" r:id="rId51" xr:uid="{F4FF688C-35E4-4D35-8C51-CD53EB6C2A8E}"/>
-    <hyperlink ref="F52" r:id="rId52" xr:uid="{2CB090FD-FB84-4A03-A89B-50F8A1C9F5BD}"/>
+    <hyperlink ref="F38" r:id="rId50" xr:uid="{2C0DFA88-75D9-4BB4-A9EE-449C4C108A11}"/>
+    <hyperlink ref="F28" r:id="rId51" xr:uid="{F4FF688C-35E4-4D35-8C51-CD53EB6C2A8E}"/>
+    <hyperlink ref="F55" r:id="rId52" xr:uid="{2CB090FD-FB84-4A03-A89B-50F8A1C9F5BD}"/>
     <hyperlink ref="F18" r:id="rId53" xr:uid="{B03C78ED-3523-452D-AD83-025C4F648157}"/>
-    <hyperlink ref="F38" r:id="rId54" xr:uid="{AC23ABB6-7E63-45F0-B07E-178795C65651}"/>
-    <hyperlink ref="F32" r:id="rId55" xr:uid="{253A3216-53A1-4AD4-9A4D-31EC0F346F7B}"/>
+    <hyperlink ref="F41" r:id="rId54" xr:uid="{AC23ABB6-7E63-45F0-B07E-178795C65651}"/>
+    <hyperlink ref="F35" r:id="rId55" xr:uid="{253A3216-53A1-4AD4-9A4D-31EC0F346F7B}"/>
     <hyperlink ref="F24" r:id="rId56" xr:uid="{D369BB7D-E54A-46CB-813D-E942B4FDBDA6}"/>
-    <hyperlink ref="F33" r:id="rId57" xr:uid="{682DFEC9-B62F-4777-8B03-2A2F3AD89C26}"/>
+    <hyperlink ref="F36" r:id="rId57" xr:uid="{682DFEC9-B62F-4777-8B03-2A2F3AD89C26}"/>
     <hyperlink ref="F22" r:id="rId58" xr:uid="{97B23B61-03A2-46B0-8FDC-EC67D02494CD}"/>
     <hyperlink ref="F10" r:id="rId59" xr:uid="{026695FB-A1A0-417C-8075-98AC08B3580C}"/>
-    <hyperlink ref="F43" r:id="rId60" xr:uid="{4D7429E8-6222-42F1-BD8D-3975D3CB77C3}"/>
-    <hyperlink ref="F51" r:id="rId61" xr:uid="{DAAEC77E-D512-4617-B851-2AD89315F496}"/>
-    <hyperlink ref="F61" r:id="rId62" xr:uid="{5833C0C8-BE25-404A-BCD5-B1BE6AB6638F}"/>
-    <hyperlink ref="E58" r:id="rId63" xr:uid="{50FEBA24-D2B4-420A-AEA7-6BB2D0719A52}"/>
+    <hyperlink ref="F46" r:id="rId60" xr:uid="{4D7429E8-6222-42F1-BD8D-3975D3CB77C3}"/>
+    <hyperlink ref="F54" r:id="rId61" xr:uid="{DAAEC77E-D512-4617-B851-2AD89315F496}"/>
+    <hyperlink ref="F65" r:id="rId62" xr:uid="{5833C0C8-BE25-404A-BCD5-B1BE6AB6638F}"/>
+    <hyperlink ref="E62" r:id="rId63" xr:uid="{50FEBA24-D2B4-420A-AEA7-6BB2D0719A52}"/>
     <hyperlink ref="E17" r:id="rId64" xr:uid="{9F40885B-F7A9-4F17-A7CD-DEE821C50339}"/>
-    <hyperlink ref="E50" r:id="rId65" xr:uid="{5223544E-DDEF-48F9-9EB3-3EF1B9FDAB90}"/>
+    <hyperlink ref="E53" r:id="rId65" xr:uid="{5223544E-DDEF-48F9-9EB3-3EF1B9FDAB90}"/>
     <hyperlink ref="E7" r:id="rId66" xr:uid="{F7C2BC13-BAF9-4996-AE90-F94B1E8EA045}"/>
     <hyperlink ref="F7" r:id="rId67" xr:uid="{C942D955-FF96-47FC-9CE5-48E87F200A13}"/>
-    <hyperlink ref="E41" r:id="rId68" xr:uid="{9AA38BAF-4725-4754-B7EA-23E92B659CE2}"/>
-    <hyperlink ref="E45" r:id="rId69" xr:uid="{C838F4BD-E551-442C-B150-986D44024BB8}"/>
-    <hyperlink ref="F62" r:id="rId70" xr:uid="{75BD971A-96A3-46CE-985A-1488D76AC8A9}"/>
-    <hyperlink ref="E30" r:id="rId71" xr:uid="{0946638C-6244-4956-B991-62477DA31ADD}"/>
-    <hyperlink ref="F30" r:id="rId72" xr:uid="{284180A6-16F2-45D7-A1C3-FEFCA8D5DF8F}"/>
+    <hyperlink ref="E44" r:id="rId68" xr:uid="{9AA38BAF-4725-4754-B7EA-23E92B659CE2}"/>
+    <hyperlink ref="E48" r:id="rId69" xr:uid="{C838F4BD-E551-442C-B150-986D44024BB8}"/>
+    <hyperlink ref="F66" r:id="rId70" xr:uid="{75BD971A-96A3-46CE-985A-1488D76AC8A9}"/>
+    <hyperlink ref="E33" r:id="rId71" xr:uid="{0946638C-6244-4956-B991-62477DA31ADD}"/>
+    <hyperlink ref="F33" r:id="rId72" xr:uid="{284180A6-16F2-45D7-A1C3-FEFCA8D5DF8F}"/>
     <hyperlink ref="E4" r:id="rId73" xr:uid="{25E264DA-B0C3-46BF-A97A-3AD180D45867}"/>
     <hyperlink ref="F4" r:id="rId74" xr:uid="{C0B54655-8946-4353-B1A2-7744E6BD8F27}"/>
     <hyperlink ref="E23" r:id="rId75" xr:uid="{DA020059-D107-474F-AD71-FA4B691620C3}"/>
@@ -2653,37 +2686,40 @@
     <hyperlink ref="F5" r:id="rId77" xr:uid="{BF9E4E83-5742-4615-B200-4C1F37F85400}"/>
     <hyperlink ref="F6" r:id="rId78" xr:uid="{8BBEEF6A-BE59-43A2-A2B0-3B29FB59AF38}"/>
     <hyperlink ref="F23" r:id="rId79" xr:uid="{EB36F77B-E092-4401-A2AB-084464E6E8DA}"/>
-    <hyperlink ref="F34" r:id="rId80" xr:uid="{3713800B-0A12-4AAE-9BD5-4F93AD851F0E}"/>
-    <hyperlink ref="F37" r:id="rId81" xr:uid="{9BD0D58C-FD3A-4471-8DA0-1961D4880B10}"/>
-    <hyperlink ref="F47" r:id="rId82" xr:uid="{4EF6A25D-97B9-41C5-AD14-BF4F4D8BDF34}"/>
+    <hyperlink ref="F37" r:id="rId80" xr:uid="{3713800B-0A12-4AAE-9BD5-4F93AD851F0E}"/>
+    <hyperlink ref="F40" r:id="rId81" xr:uid="{9BD0D58C-FD3A-4471-8DA0-1961D4880B10}"/>
+    <hyperlink ref="F50" r:id="rId82" xr:uid="{4EF6A25D-97B9-41C5-AD14-BF4F4D8BDF34}"/>
     <hyperlink ref="F16" r:id="rId83" xr:uid="{2D115D7B-5F56-4E0A-95AE-0F9322EF7834}"/>
     <hyperlink ref="E14" r:id="rId84" xr:uid="{ABE8ED47-6F4D-4A6B-934E-EAF7F614157B}"/>
-    <hyperlink ref="E32" r:id="rId85" xr:uid="{A46821FE-B9E6-4DA6-86A1-423D6D8625C4}"/>
-    <hyperlink ref="E33" r:id="rId86" xr:uid="{26859566-EDF8-4D35-9633-DF0946322AF6}"/>
-    <hyperlink ref="E37" r:id="rId87" xr:uid="{7175EFCD-2552-4973-8B3D-95D63C9CD86F}"/>
-    <hyperlink ref="E47" r:id="rId88" xr:uid="{CD3C8CE1-4C32-462C-84A8-1E3130D1F63F}"/>
-    <hyperlink ref="E63" r:id="rId89" xr:uid="{654FB847-B1BF-4E9D-9F87-14D35D782BF2}"/>
-    <hyperlink ref="F63" r:id="rId90" xr:uid="{EEEC10BC-21C5-4BCA-A4F4-990220257200}"/>
+    <hyperlink ref="E35" r:id="rId85" xr:uid="{A46821FE-B9E6-4DA6-86A1-423D6D8625C4}"/>
+    <hyperlink ref="E36" r:id="rId86" xr:uid="{26859566-EDF8-4D35-9633-DF0946322AF6}"/>
+    <hyperlink ref="E40" r:id="rId87" xr:uid="{7175EFCD-2552-4973-8B3D-95D63C9CD86F}"/>
+    <hyperlink ref="E50" r:id="rId88" xr:uid="{CD3C8CE1-4C32-462C-84A8-1E3130D1F63F}"/>
+    <hyperlink ref="E67" r:id="rId89" xr:uid="{654FB847-B1BF-4E9D-9F87-14D35D782BF2}"/>
+    <hyperlink ref="F67" r:id="rId90" xr:uid="{EEEC10BC-21C5-4BCA-A4F4-990220257200}"/>
     <hyperlink ref="F14" r:id="rId91" xr:uid="{D298C803-0132-49F6-ABA7-54E1CA93013D}"/>
     <hyperlink ref="F13" r:id="rId92" xr:uid="{44541484-41EC-488E-9C46-FD2985DEF367}"/>
     <hyperlink ref="E13" r:id="rId93" xr:uid="{8BF2D71A-70CF-4CDE-BDBF-3033BB382FCF}"/>
     <hyperlink ref="F12" r:id="rId94" xr:uid="{51B31C2E-3892-472A-913B-87FAC66C6F76}"/>
     <hyperlink ref="E12" r:id="rId95" xr:uid="{5826D20D-02CD-4129-82AC-7314C8A1AEF7}"/>
-    <hyperlink ref="F26" r:id="rId96" xr:uid="{9B0E6E50-8807-4AC2-A155-706196529592}"/>
-    <hyperlink ref="E26" r:id="rId97" xr:uid="{717BD393-9CD1-456C-B170-0C0E0DE21984}"/>
-    <hyperlink ref="F53" r:id="rId98" xr:uid="{47A3461D-BB0E-485D-A69D-249CEFEFB2EA}"/>
+    <hyperlink ref="F27" r:id="rId96" xr:uid="{9B0E6E50-8807-4AC2-A155-706196529592}"/>
+    <hyperlink ref="E27" r:id="rId97" xr:uid="{717BD393-9CD1-456C-B170-0C0E0DE21984}"/>
+    <hyperlink ref="F56" r:id="rId98" xr:uid="{47A3461D-BB0E-485D-A69D-249CEFEFB2EA}"/>
     <hyperlink ref="F8" r:id="rId99" xr:uid="{9193DF21-E100-42C4-BE99-FD9D65FAAB4A}"/>
     <hyperlink ref="E8" r:id="rId100" xr:uid="{0529A15C-C3F2-4FE1-B402-51C24807BA8A}"/>
-    <hyperlink ref="E64" r:id="rId101" xr:uid="{5EEE8774-5BFE-4091-8D5B-AECA259D6AC7}"/>
-    <hyperlink ref="F64" r:id="rId102" xr:uid="{5BC10617-F8EE-400C-BDC5-07113421E148}"/>
-    <hyperlink ref="E65" r:id="rId103" xr:uid="{6F5DEAF7-DD57-4D97-B227-F245CE16EAEB}"/>
-    <hyperlink ref="F65" r:id="rId104" xr:uid="{F84F7FA1-A12B-4794-8B3A-2C84C6A0C78D}"/>
-    <hyperlink ref="E66" r:id="rId105" xr:uid="{2F675965-8E88-4605-9B06-9379AFD65861}"/>
-    <hyperlink ref="F66" r:id="rId106" xr:uid="{07818C94-99C0-4FA9-AB24-BA30A4D6874F}"/>
-    <hyperlink ref="E67" r:id="rId107" xr:uid="{B74BD8C3-4C40-406B-AECA-E72A9F2219F0}"/>
-    <hyperlink ref="F67" r:id="rId108" xr:uid="{301AE9A9-71A3-4FD6-8723-DCA05CE807B9}"/>
+    <hyperlink ref="E60" r:id="rId101" xr:uid="{5EEE8774-5BFE-4091-8D5B-AECA259D6AC7}"/>
+    <hyperlink ref="F60" r:id="rId102" xr:uid="{5BC10617-F8EE-400C-BDC5-07113421E148}"/>
+    <hyperlink ref="E26" r:id="rId103" xr:uid="{6F5DEAF7-DD57-4D97-B227-F245CE16EAEB}"/>
+    <hyperlink ref="F26" r:id="rId104" xr:uid="{F84F7FA1-A12B-4794-8B3A-2C84C6A0C78D}"/>
+    <hyperlink ref="E31" r:id="rId105" xr:uid="{2F675965-8E88-4605-9B06-9379AFD65861}"/>
+    <hyperlink ref="F31" r:id="rId106" xr:uid="{07818C94-99C0-4FA9-AB24-BA30A4D6874F}"/>
+    <hyperlink ref="E30" r:id="rId107" xr:uid="{B74BD8C3-4C40-406B-AECA-E72A9F2219F0}"/>
+    <hyperlink ref="F30" r:id="rId108" xr:uid="{301AE9A9-71A3-4FD6-8723-DCA05CE807B9}"/>
+    <hyperlink ref="E68" r:id="rId109" xr:uid="{1696E89E-16D6-45DD-BBF0-2C162C5D99AB}"/>
+    <hyperlink ref="F68" r:id="rId110" xr:uid="{FF9A5E23-4EA2-4D92-AABB-E0559D090ACE}"/>
+    <hyperlink ref="E56" r:id="rId111" xr:uid="{A4F70388-5266-477A-9C7D-F1847571E0D7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId109"/>
+  <pageSetup orientation="portrait" r:id="rId112"/>
 </worksheet>
 </file>
</xml_diff>